<commit_message>
Added measures to the workflow: roof sheathing, floor sheathing, and furniture thermal mass.
</commit_message>
<xml_diff>
--- a/projects/res_stock_national_existing.xlsx
+++ b/projects/res_stock_national_existing.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14160" windowHeight="8295" tabRatio="562" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14160" windowHeight="8295" tabRatio="562"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="7" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1383" uniqueCount="591">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1434" uniqueCount="606">
   <si>
     <t>type</t>
   </si>
@@ -1807,6 +1807,51 @@
   </si>
   <si>
     <t>Set Res Stock Mode - National</t>
+  </si>
+  <si>
+    <t>Set Roof Sheathing</t>
+  </si>
+  <si>
+    <t>Roof Sheathing.tsv</t>
+  </si>
+  <si>
+    <t>Roof Sheathing Sample Value</t>
+  </si>
+  <si>
+    <t>Set Floor Sheathing</t>
+  </si>
+  <si>
+    <t>Floor Sheathing.tsv</t>
+  </si>
+  <si>
+    <t>Floor Sheathing Sample Value</t>
+  </si>
+  <si>
+    <t>Roof Sheathing</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.Roof Sheathing</t>
+  </si>
+  <si>
+    <t>Floor Sheathing</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.Floor Sheathing</t>
+  </si>
+  <si>
+    <t>Set Thermal Mass Furniture</t>
+  </si>
+  <si>
+    <t>Thermal Mass Furniture Sample Value</t>
+  </si>
+  <si>
+    <t>Thermal Mass Furniture.tsv</t>
+  </si>
+  <si>
+    <t>Thermal Mass Furniture</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.Thermal Mass Furniture</t>
   </si>
 </sst>
 </file>
@@ -5398,7 +5443,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6033,9 +6078,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z185"/>
+  <dimension ref="A1:Z194"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -9411,7 +9456,7 @@
         <v>1</v>
       </c>
       <c r="B84" s="40" t="s">
-        <v>269</v>
+        <v>591</v>
       </c>
       <c r="C84" s="40" t="s">
         <v>235</v>
@@ -9460,7 +9505,7 @@
       </c>
       <c r="H85" s="10"/>
       <c r="I85" s="10" t="s">
-        <v>423</v>
+        <v>592</v>
       </c>
       <c r="J85" s="10"/>
       <c r="K85" s="10"/>
@@ -9487,7 +9532,7 @@
       </c>
       <c r="C86" s="41"/>
       <c r="D86" s="41" t="s">
-        <v>270</v>
+        <v>593</v>
       </c>
       <c r="E86" s="41" t="s">
         <v>237</v>
@@ -9531,7 +9576,7 @@
         <v>1</v>
       </c>
       <c r="B87" s="40" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C87" s="40" t="s">
         <v>235</v>
@@ -9580,7 +9625,7 @@
       </c>
       <c r="H88" s="10"/>
       <c r="I88" s="10" t="s">
-        <v>378</v>
+        <v>423</v>
       </c>
       <c r="J88" s="10"/>
       <c r="K88" s="10"/>
@@ -9607,7 +9652,7 @@
       </c>
       <c r="C89" s="41"/>
       <c r="D89" s="41" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="E89" s="41" t="s">
         <v>237</v>
@@ -9651,7 +9696,7 @@
         <v>1</v>
       </c>
       <c r="B90" s="40" t="s">
-        <v>273</v>
+        <v>594</v>
       </c>
       <c r="C90" s="40" t="s">
         <v>235</v>
@@ -9700,7 +9745,7 @@
       </c>
       <c r="H91" s="10"/>
       <c r="I91" s="10" t="s">
-        <v>415</v>
+        <v>595</v>
       </c>
       <c r="J91" s="10"/>
       <c r="K91" s="10"/>
@@ -9727,7 +9772,7 @@
       </c>
       <c r="C92" s="41"/>
       <c r="D92" s="41" t="s">
-        <v>274</v>
+        <v>596</v>
       </c>
       <c r="E92" s="41" t="s">
         <v>237</v>
@@ -9771,7 +9816,7 @@
         <v>1</v>
       </c>
       <c r="B93" s="40" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C93" s="40" t="s">
         <v>235</v>
@@ -9820,7 +9865,7 @@
       </c>
       <c r="H94" s="10"/>
       <c r="I94" s="10" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="J94" s="10"/>
       <c r="K94" s="10"/>
@@ -9847,7 +9892,7 @@
       </c>
       <c r="C95" s="41"/>
       <c r="D95" s="41" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="E95" s="41" t="s">
         <v>237</v>
@@ -9891,7 +9936,7 @@
         <v>1</v>
       </c>
       <c r="B96" s="40" t="s">
-        <v>514</v>
+        <v>273</v>
       </c>
       <c r="C96" s="40" t="s">
         <v>235</v>
@@ -9940,7 +9985,7 @@
       </c>
       <c r="H97" s="10"/>
       <c r="I97" s="10" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="J97" s="10"/>
       <c r="K97" s="10"/>
@@ -9967,7 +10012,7 @@
       </c>
       <c r="C98" s="41"/>
       <c r="D98" s="41" t="s">
-        <v>515</v>
+        <v>274</v>
       </c>
       <c r="E98" s="41" t="s">
         <v>237</v>
@@ -10011,7 +10056,7 @@
         <v>1</v>
       </c>
       <c r="B99" s="40" t="s">
-        <v>516</v>
+        <v>275</v>
       </c>
       <c r="C99" s="40" t="s">
         <v>235</v>
@@ -10060,7 +10105,7 @@
       </c>
       <c r="H100" s="10"/>
       <c r="I100" s="10" t="s">
-        <v>417</v>
+        <v>379</v>
       </c>
       <c r="J100" s="10"/>
       <c r="K100" s="10"/>
@@ -10087,7 +10132,7 @@
       </c>
       <c r="C101" s="41"/>
       <c r="D101" s="41" t="s">
-        <v>517</v>
+        <v>276</v>
       </c>
       <c r="E101" s="41" t="s">
         <v>237</v>
@@ -10131,7 +10176,7 @@
         <v>1</v>
       </c>
       <c r="B102" s="40" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="C102" s="40" t="s">
         <v>235</v>
@@ -10180,7 +10225,7 @@
       </c>
       <c r="H103" s="10"/>
       <c r="I103" s="10" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="J103" s="10"/>
       <c r="K103" s="10"/>
@@ -10207,7 +10252,7 @@
       </c>
       <c r="C104" s="41"/>
       <c r="D104" s="41" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="E104" s="41" t="s">
         <v>237</v>
@@ -10251,7 +10296,7 @@
         <v>1</v>
       </c>
       <c r="B105" s="40" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="C105" s="40" t="s">
         <v>235</v>
@@ -10300,7 +10345,7 @@
       </c>
       <c r="H106" s="10"/>
       <c r="I106" s="10" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="J106" s="10"/>
       <c r="K106" s="10"/>
@@ -10327,7 +10372,7 @@
       </c>
       <c r="C107" s="41"/>
       <c r="D107" s="41" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="E107" s="41" t="s">
         <v>237</v>
@@ -10371,7 +10416,7 @@
         <v>1</v>
       </c>
       <c r="B108" s="40" t="s">
-        <v>281</v>
+        <v>518</v>
       </c>
       <c r="C108" s="40" t="s">
         <v>235</v>
@@ -10420,7 +10465,7 @@
       </c>
       <c r="H109" s="10"/>
       <c r="I109" s="10" t="s">
-        <v>376</v>
+        <v>419</v>
       </c>
       <c r="J109" s="10"/>
       <c r="K109" s="10"/>
@@ -10447,7 +10492,7 @@
       </c>
       <c r="C110" s="41"/>
       <c r="D110" s="41" t="s">
-        <v>282</v>
+        <v>519</v>
       </c>
       <c r="E110" s="41" t="s">
         <v>237</v>
@@ -10491,7 +10536,7 @@
         <v>1</v>
       </c>
       <c r="B111" s="40" t="s">
-        <v>344</v>
+        <v>520</v>
       </c>
       <c r="C111" s="40" t="s">
         <v>235</v>
@@ -10540,7 +10585,7 @@
       </c>
       <c r="H112" s="10"/>
       <c r="I112" s="10" t="s">
-        <v>426</v>
+        <v>416</v>
       </c>
       <c r="J112" s="10"/>
       <c r="K112" s="10"/>
@@ -10567,7 +10612,7 @@
       </c>
       <c r="C113" s="41"/>
       <c r="D113" s="41" t="s">
-        <v>345</v>
+        <v>521</v>
       </c>
       <c r="E113" s="41" t="s">
         <v>237</v>
@@ -10611,7 +10656,7 @@
         <v>1</v>
       </c>
       <c r="B114" s="40" t="s">
-        <v>303</v>
+        <v>601</v>
       </c>
       <c r="C114" s="40" t="s">
         <v>235</v>
@@ -10660,7 +10705,7 @@
       </c>
       <c r="H115" s="10"/>
       <c r="I115" s="10" t="s">
-        <v>424</v>
+        <v>603</v>
       </c>
       <c r="J115" s="10"/>
       <c r="K115" s="10"/>
@@ -10687,7 +10732,7 @@
       </c>
       <c r="C116" s="41"/>
       <c r="D116" s="41" t="s">
-        <v>304</v>
+        <v>602</v>
       </c>
       <c r="E116" s="41" t="s">
         <v>237</v>
@@ -10731,7 +10776,7 @@
         <v>1</v>
       </c>
       <c r="B117" s="40" t="s">
-        <v>369</v>
+        <v>281</v>
       </c>
       <c r="C117" s="40" t="s">
         <v>235</v>
@@ -10780,7 +10825,7 @@
       </c>
       <c r="H118" s="10"/>
       <c r="I118" s="10" t="s">
-        <v>386</v>
+        <v>376</v>
       </c>
       <c r="J118" s="10"/>
       <c r="K118" s="10"/>
@@ -10807,7 +10852,7 @@
       </c>
       <c r="C119" s="41"/>
       <c r="D119" s="41" t="s">
-        <v>370</v>
+        <v>282</v>
       </c>
       <c r="E119" s="41" t="s">
         <v>237</v>
@@ -10851,7 +10896,7 @@
         <v>1</v>
       </c>
       <c r="B120" s="40" t="s">
-        <v>358</v>
+        <v>344</v>
       </c>
       <c r="C120" s="40" t="s">
         <v>235</v>
@@ -10900,7 +10945,7 @@
       </c>
       <c r="H121" s="10"/>
       <c r="I121" s="10" t="s">
-        <v>390</v>
+        <v>426</v>
       </c>
       <c r="J121" s="10"/>
       <c r="K121" s="10"/>
@@ -10927,7 +10972,7 @@
       </c>
       <c r="C122" s="41"/>
       <c r="D122" s="41" t="s">
-        <v>359</v>
+        <v>345</v>
       </c>
       <c r="E122" s="41" t="s">
         <v>237</v>
@@ -10971,7 +11016,7 @@
         <v>1</v>
       </c>
       <c r="B123" s="40" t="s">
-        <v>356</v>
+        <v>303</v>
       </c>
       <c r="C123" s="40" t="s">
         <v>235</v>
@@ -11020,7 +11065,7 @@
       </c>
       <c r="H124" s="10"/>
       <c r="I124" s="10" t="s">
-        <v>387</v>
+        <v>424</v>
       </c>
       <c r="J124" s="10"/>
       <c r="K124" s="10"/>
@@ -11047,7 +11092,7 @@
       </c>
       <c r="C125" s="41"/>
       <c r="D125" s="41" t="s">
-        <v>357</v>
+        <v>304</v>
       </c>
       <c r="E125" s="41" t="s">
         <v>237</v>
@@ -11091,7 +11136,7 @@
         <v>1</v>
       </c>
       <c r="B126" s="40" t="s">
-        <v>364</v>
+        <v>369</v>
       </c>
       <c r="C126" s="40" t="s">
         <v>235</v>
@@ -11140,7 +11185,7 @@
       </c>
       <c r="H127" s="10"/>
       <c r="I127" s="10" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="J127" s="10"/>
       <c r="K127" s="10"/>
@@ -11167,7 +11212,7 @@
       </c>
       <c r="C128" s="41"/>
       <c r="D128" s="41" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="E128" s="41" t="s">
         <v>237</v>
@@ -11211,7 +11256,7 @@
         <v>1</v>
       </c>
       <c r="B129" s="40" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="C129" s="40" t="s">
         <v>235</v>
@@ -11260,7 +11305,7 @@
       </c>
       <c r="H130" s="10"/>
       <c r="I130" s="10" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="J130" s="10"/>
       <c r="K130" s="10"/>
@@ -11287,7 +11332,7 @@
       </c>
       <c r="C131" s="41"/>
       <c r="D131" s="41" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
       <c r="E131" s="41" t="s">
         <v>237</v>
@@ -11331,7 +11376,7 @@
         <v>1</v>
       </c>
       <c r="B132" s="40" t="s">
-        <v>578</v>
+        <v>356</v>
       </c>
       <c r="C132" s="40" t="s">
         <v>235</v>
@@ -11380,7 +11425,7 @@
       </c>
       <c r="H133" s="10"/>
       <c r="I133" s="10" t="s">
-        <v>582</v>
+        <v>387</v>
       </c>
       <c r="J133" s="10"/>
       <c r="K133" s="10"/>
@@ -11407,7 +11452,7 @@
       </c>
       <c r="C134" s="41"/>
       <c r="D134" s="41" t="s">
-        <v>579</v>
+        <v>357</v>
       </c>
       <c r="E134" s="41" t="s">
         <v>237</v>
@@ -11451,7 +11496,7 @@
         <v>1</v>
       </c>
       <c r="B135" s="40" t="s">
-        <v>577</v>
+        <v>364</v>
       </c>
       <c r="C135" s="40" t="s">
         <v>235</v>
@@ -11500,7 +11545,7 @@
       </c>
       <c r="H136" s="10"/>
       <c r="I136" s="10" t="s">
-        <v>581</v>
+        <v>389</v>
       </c>
       <c r="J136" s="10"/>
       <c r="K136" s="10"/>
@@ -11527,7 +11572,7 @@
       </c>
       <c r="C137" s="41"/>
       <c r="D137" s="41" t="s">
-        <v>580</v>
+        <v>367</v>
       </c>
       <c r="E137" s="41" t="s">
         <v>237</v>
@@ -11571,7 +11616,7 @@
         <v>1</v>
       </c>
       <c r="B138" s="40" t="s">
-        <v>287</v>
+        <v>365</v>
       </c>
       <c r="C138" s="40" t="s">
         <v>235</v>
@@ -11620,7 +11665,7 @@
       </c>
       <c r="H139" s="10"/>
       <c r="I139" s="10" t="s">
-        <v>414</v>
+        <v>388</v>
       </c>
       <c r="J139" s="10"/>
       <c r="K139" s="10"/>
@@ -11647,7 +11692,7 @@
       </c>
       <c r="C140" s="41"/>
       <c r="D140" s="41" t="s">
-        <v>288</v>
+        <v>366</v>
       </c>
       <c r="E140" s="41" t="s">
         <v>237</v>
@@ -11691,7 +11736,7 @@
         <v>1</v>
       </c>
       <c r="B141" s="40" t="s">
-        <v>291</v>
+        <v>578</v>
       </c>
       <c r="C141" s="40" t="s">
         <v>235</v>
@@ -11740,7 +11785,7 @@
       </c>
       <c r="H142" s="10"/>
       <c r="I142" s="10" t="s">
-        <v>373</v>
+        <v>582</v>
       </c>
       <c r="J142" s="10"/>
       <c r="K142" s="10"/>
@@ -11767,7 +11812,7 @@
       </c>
       <c r="C143" s="41"/>
       <c r="D143" s="41" t="s">
-        <v>292</v>
+        <v>579</v>
       </c>
       <c r="E143" s="41" t="s">
         <v>237</v>
@@ -11811,7 +11856,7 @@
         <v>1</v>
       </c>
       <c r="B144" s="40" t="s">
-        <v>295</v>
+        <v>577</v>
       </c>
       <c r="C144" s="40" t="s">
         <v>235</v>
@@ -11860,7 +11905,7 @@
       </c>
       <c r="H145" s="10"/>
       <c r="I145" s="10" t="s">
-        <v>374</v>
+        <v>581</v>
       </c>
       <c r="J145" s="10"/>
       <c r="K145" s="10"/>
@@ -11887,7 +11932,7 @@
       </c>
       <c r="C146" s="41"/>
       <c r="D146" s="41" t="s">
-        <v>296</v>
+        <v>580</v>
       </c>
       <c r="E146" s="41" t="s">
         <v>237</v>
@@ -11931,7 +11976,7 @@
         <v>1</v>
       </c>
       <c r="B147" s="40" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
       <c r="C147" s="40" t="s">
         <v>235</v>
@@ -11980,7 +12025,7 @@
       </c>
       <c r="H148" s="10"/>
       <c r="I148" s="10" t="s">
-        <v>372</v>
+        <v>414</v>
       </c>
       <c r="J148" s="10"/>
       <c r="K148" s="10"/>
@@ -12007,7 +12052,7 @@
       </c>
       <c r="C149" s="41"/>
       <c r="D149" s="41" t="s">
-        <v>298</v>
+        <v>288</v>
       </c>
       <c r="E149" s="41" t="s">
         <v>237</v>
@@ -12051,7 +12096,7 @@
         <v>1</v>
       </c>
       <c r="B150" s="40" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
       <c r="C150" s="40" t="s">
         <v>235</v>
@@ -12100,7 +12145,7 @@
       </c>
       <c r="H151" s="10"/>
       <c r="I151" s="10" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="J151" s="10"/>
       <c r="K151" s="10"/>
@@ -12127,7 +12172,7 @@
       </c>
       <c r="C152" s="41"/>
       <c r="D152" s="41" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="E152" s="41" t="s">
         <v>237</v>
@@ -12171,7 +12216,7 @@
         <v>1</v>
       </c>
       <c r="B153" s="40" t="s">
-        <v>348</v>
+        <v>295</v>
       </c>
       <c r="C153" s="40" t="s">
         <v>235</v>
@@ -12220,7 +12265,7 @@
       </c>
       <c r="H154" s="10"/>
       <c r="I154" s="10" t="s">
-        <v>399</v>
+        <v>374</v>
       </c>
       <c r="J154" s="10"/>
       <c r="K154" s="10"/>
@@ -12247,7 +12292,7 @@
       </c>
       <c r="C155" s="41"/>
       <c r="D155" s="41" t="s">
-        <v>349</v>
+        <v>296</v>
       </c>
       <c r="E155" s="41" t="s">
         <v>237</v>
@@ -12291,7 +12336,7 @@
         <v>1</v>
       </c>
       <c r="B156" s="40" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="C156" s="40" t="s">
         <v>235</v>
@@ -12340,7 +12385,7 @@
       </c>
       <c r="H157" s="10"/>
       <c r="I157" s="10" t="s">
-        <v>413</v>
+        <v>372</v>
       </c>
       <c r="J157" s="10"/>
       <c r="K157" s="10"/>
@@ -12367,7 +12412,7 @@
       </c>
       <c r="C158" s="41"/>
       <c r="D158" s="41" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="E158" s="41" t="s">
         <v>237</v>
@@ -12411,7 +12456,7 @@
         <v>1</v>
       </c>
       <c r="B159" s="40" t="s">
-        <v>523</v>
+        <v>299</v>
       </c>
       <c r="C159" s="40" t="s">
         <v>235</v>
@@ -12460,7 +12505,7 @@
       </c>
       <c r="H160" s="10"/>
       <c r="I160" s="10" t="s">
-        <v>402</v>
+        <v>371</v>
       </c>
       <c r="J160" s="10"/>
       <c r="K160" s="10"/>
@@ -12487,7 +12532,7 @@
       </c>
       <c r="C161" s="41"/>
       <c r="D161" s="41" t="s">
-        <v>522</v>
+        <v>300</v>
       </c>
       <c r="E161" s="41" t="s">
         <v>237</v>
@@ -12531,7 +12576,7 @@
         <v>1</v>
       </c>
       <c r="B162" s="40" t="s">
-        <v>524</v>
+        <v>348</v>
       </c>
       <c r="C162" s="40" t="s">
         <v>235</v>
@@ -12580,7 +12625,7 @@
       </c>
       <c r="H163" s="10"/>
       <c r="I163" s="10" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="J163" s="10"/>
       <c r="K163" s="10"/>
@@ -12607,7 +12652,7 @@
       </c>
       <c r="C164" s="41"/>
       <c r="D164" s="41" t="s">
-        <v>525</v>
+        <v>349</v>
       </c>
       <c r="E164" s="41" t="s">
         <v>237</v>
@@ -12651,7 +12696,7 @@
         <v>1</v>
       </c>
       <c r="B165" s="40" t="s">
-        <v>526</v>
+        <v>301</v>
       </c>
       <c r="C165" s="40" t="s">
         <v>235</v>
@@ -12700,7 +12745,7 @@
       </c>
       <c r="H166" s="10"/>
       <c r="I166" s="10" t="s">
-        <v>404</v>
+        <v>413</v>
       </c>
       <c r="J166" s="10"/>
       <c r="K166" s="10"/>
@@ -12727,7 +12772,7 @@
       </c>
       <c r="C167" s="41"/>
       <c r="D167" s="41" t="s">
-        <v>527</v>
+        <v>302</v>
       </c>
       <c r="E167" s="41" t="s">
         <v>237</v>
@@ -12771,7 +12816,7 @@
         <v>1</v>
       </c>
       <c r="B168" s="40" t="s">
-        <v>528</v>
+        <v>523</v>
       </c>
       <c r="C168" s="40" t="s">
         <v>235</v>
@@ -12820,7 +12865,7 @@
       </c>
       <c r="H169" s="10"/>
       <c r="I169" s="10" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="J169" s="10"/>
       <c r="K169" s="10"/>
@@ -12847,7 +12892,7 @@
       </c>
       <c r="C170" s="41"/>
       <c r="D170" s="41" t="s">
-        <v>529</v>
+        <v>522</v>
       </c>
       <c r="E170" s="41" t="s">
         <v>237</v>
@@ -12891,7 +12936,7 @@
         <v>1</v>
       </c>
       <c r="B171" s="40" t="s">
-        <v>530</v>
+        <v>524</v>
       </c>
       <c r="C171" s="40" t="s">
         <v>235</v>
@@ -12940,7 +12985,7 @@
       </c>
       <c r="H172" s="10"/>
       <c r="I172" s="10" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="J172" s="10"/>
       <c r="K172" s="10"/>
@@ -12967,7 +13012,7 @@
       </c>
       <c r="C173" s="41"/>
       <c r="D173" s="41" t="s">
-        <v>531</v>
+        <v>525</v>
       </c>
       <c r="E173" s="41" t="s">
         <v>237</v>
@@ -13011,7 +13056,7 @@
         <v>1</v>
       </c>
       <c r="B174" s="40" t="s">
-        <v>532</v>
+        <v>526</v>
       </c>
       <c r="C174" s="40" t="s">
         <v>235</v>
@@ -13060,7 +13105,7 @@
       </c>
       <c r="H175" s="10"/>
       <c r="I175" s="10" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="J175" s="10"/>
       <c r="K175" s="10"/>
@@ -13087,7 +13132,7 @@
       </c>
       <c r="C176" s="41"/>
       <c r="D176" s="41" t="s">
-        <v>533</v>
+        <v>527</v>
       </c>
       <c r="E176" s="41" t="s">
         <v>237</v>
@@ -13131,7 +13176,7 @@
         <v>1</v>
       </c>
       <c r="B177" s="40" t="s">
-        <v>534</v>
+        <v>528</v>
       </c>
       <c r="C177" s="40" t="s">
         <v>235</v>
@@ -13180,7 +13225,7 @@
       </c>
       <c r="H178" s="10"/>
       <c r="I178" s="10" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="J178" s="10"/>
       <c r="K178" s="10"/>
@@ -13207,7 +13252,7 @@
       </c>
       <c r="C179" s="41"/>
       <c r="D179" s="41" t="s">
-        <v>535</v>
+        <v>529</v>
       </c>
       <c r="E179" s="41" t="s">
         <v>237</v>
@@ -13251,7 +13296,7 @@
         <v>1</v>
       </c>
       <c r="B180" s="40" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
       <c r="C180" s="40" t="s">
         <v>235</v>
@@ -13300,7 +13345,7 @@
       </c>
       <c r="H181" s="10"/>
       <c r="I181" s="10" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="J181" s="10"/>
       <c r="K181" s="10"/>
@@ -13327,7 +13372,7 @@
       </c>
       <c r="C182" s="41"/>
       <c r="D182" s="41" t="s">
-        <v>537</v>
+        <v>531</v>
       </c>
       <c r="E182" s="41" t="s">
         <v>237</v>
@@ -13366,113 +13411,473 @@
       <c r="W182" s="41"/>
       <c r="X182" s="41"/>
     </row>
-    <row r="183" spans="1:26" s="39" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A183" s="42" t="b">
+    <row r="183" spans="1:26" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A183" s="40" t="b">
         <v>1</v>
       </c>
-      <c r="B183" s="42" t="s">
+      <c r="B183" s="40" t="s">
+        <v>532</v>
+      </c>
+      <c r="C183" s="40" t="s">
+        <v>235</v>
+      </c>
+      <c r="D183" s="40" t="s">
+        <v>235</v>
+      </c>
+      <c r="E183" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="F183" s="40"/>
+      <c r="G183" s="40"/>
+      <c r="H183" s="40"/>
+      <c r="I183" s="40"/>
+      <c r="J183" s="40"/>
+      <c r="K183" s="40"/>
+      <c r="L183" s="40"/>
+      <c r="M183" s="40"/>
+      <c r="N183" s="40"/>
+      <c r="O183" s="40"/>
+      <c r="P183" s="40"/>
+      <c r="Q183" s="40"/>
+      <c r="R183" s="40"/>
+      <c r="S183" s="40"/>
+      <c r="T183" s="40"/>
+      <c r="U183" s="40"/>
+      <c r="V183" s="40"/>
+      <c r="W183" s="40"/>
+      <c r="X183" s="40"/>
+    </row>
+    <row r="184" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A184" s="10"/>
+      <c r="B184" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C184" s="10"/>
+      <c r="D184" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="E184" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="F184" s="10"/>
+      <c r="G184" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="H184" s="10"/>
+      <c r="I184" s="10" t="s">
+        <v>407</v>
+      </c>
+      <c r="J184" s="10"/>
+      <c r="K184" s="10"/>
+      <c r="L184" s="10"/>
+      <c r="M184" s="10"/>
+      <c r="N184" s="10"/>
+      <c r="O184" s="10"/>
+      <c r="P184" s="10"/>
+      <c r="Q184" s="10"/>
+      <c r="R184" s="10"/>
+      <c r="S184" s="10"/>
+      <c r="T184" s="10"/>
+      <c r="U184" s="10"/>
+      <c r="V184" s="10"/>
+      <c r="W184" s="10"/>
+      <c r="X184" s="10"/>
+      <c r="Y184" s="15"/>
+      <c r="Z184" s="15"/>
+    </row>
+    <row r="185" spans="1:26" s="37" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A185" s="41"/>
+      <c r="B185" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="C185" s="41"/>
+      <c r="D185" s="41" t="s">
+        <v>533</v>
+      </c>
+      <c r="E185" s="41" t="s">
+        <v>237</v>
+      </c>
+      <c r="F185" s="41"/>
+      <c r="G185" s="41" t="s">
+        <v>170</v>
+      </c>
+      <c r="H185" s="41"/>
+      <c r="I185" s="41">
+        <v>0.5</v>
+      </c>
+      <c r="J185" s="41"/>
+      <c r="K185" s="41">
+        <v>0</v>
+      </c>
+      <c r="L185" s="41">
+        <v>1</v>
+      </c>
+      <c r="M185" s="41">
+        <v>0.5</v>
+      </c>
+      <c r="N185" s="41">
+        <v>0.1666667</v>
+      </c>
+      <c r="O185" s="41"/>
+      <c r="P185" s="41"/>
+      <c r="Q185" s="41"/>
+      <c r="R185" s="41" t="s">
+        <v>224</v>
+      </c>
+      <c r="S185" s="41"/>
+      <c r="T185" s="41"/>
+      <c r="U185" s="41"/>
+      <c r="V185" s="41"/>
+      <c r="W185" s="41"/>
+      <c r="X185" s="41"/>
+    </row>
+    <row r="186" spans="1:26" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A186" s="40" t="b">
+        <v>1</v>
+      </c>
+      <c r="B186" s="40" t="s">
+        <v>534</v>
+      </c>
+      <c r="C186" s="40" t="s">
+        <v>235</v>
+      </c>
+      <c r="D186" s="40" t="s">
+        <v>235</v>
+      </c>
+      <c r="E186" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="F186" s="40"/>
+      <c r="G186" s="40"/>
+      <c r="H186" s="40"/>
+      <c r="I186" s="40"/>
+      <c r="J186" s="40"/>
+      <c r="K186" s="40"/>
+      <c r="L186" s="40"/>
+      <c r="M186" s="40"/>
+      <c r="N186" s="40"/>
+      <c r="O186" s="40"/>
+      <c r="P186" s="40"/>
+      <c r="Q186" s="40"/>
+      <c r="R186" s="40"/>
+      <c r="S186" s="40"/>
+      <c r="T186" s="40"/>
+      <c r="U186" s="40"/>
+      <c r="V186" s="40"/>
+      <c r="W186" s="40"/>
+      <c r="X186" s="40"/>
+    </row>
+    <row r="187" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A187" s="10"/>
+      <c r="B187" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C187" s="10"/>
+      <c r="D187" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="E187" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="F187" s="10"/>
+      <c r="G187" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="H187" s="10"/>
+      <c r="I187" s="10" t="s">
+        <v>408</v>
+      </c>
+      <c r="J187" s="10"/>
+      <c r="K187" s="10"/>
+      <c r="L187" s="10"/>
+      <c r="M187" s="10"/>
+      <c r="N187" s="10"/>
+      <c r="O187" s="10"/>
+      <c r="P187" s="10"/>
+      <c r="Q187" s="10"/>
+      <c r="R187" s="10"/>
+      <c r="S187" s="10"/>
+      <c r="T187" s="10"/>
+      <c r="U187" s="10"/>
+      <c r="V187" s="10"/>
+      <c r="W187" s="10"/>
+      <c r="X187" s="10"/>
+      <c r="Y187" s="15"/>
+      <c r="Z187" s="15"/>
+    </row>
+    <row r="188" spans="1:26" s="37" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A188" s="41"/>
+      <c r="B188" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="C188" s="41"/>
+      <c r="D188" s="41" t="s">
+        <v>535</v>
+      </c>
+      <c r="E188" s="41" t="s">
+        <v>237</v>
+      </c>
+      <c r="F188" s="41"/>
+      <c r="G188" s="41" t="s">
+        <v>170</v>
+      </c>
+      <c r="H188" s="41"/>
+      <c r="I188" s="41">
+        <v>0.5</v>
+      </c>
+      <c r="J188" s="41"/>
+      <c r="K188" s="41">
+        <v>0</v>
+      </c>
+      <c r="L188" s="41">
+        <v>1</v>
+      </c>
+      <c r="M188" s="41">
+        <v>0.5</v>
+      </c>
+      <c r="N188" s="41">
+        <v>0.1666667</v>
+      </c>
+      <c r="O188" s="41"/>
+      <c r="P188" s="41"/>
+      <c r="Q188" s="41"/>
+      <c r="R188" s="41" t="s">
+        <v>224</v>
+      </c>
+      <c r="S188" s="41"/>
+      <c r="T188" s="41"/>
+      <c r="U188" s="41"/>
+      <c r="V188" s="41"/>
+      <c r="W188" s="41"/>
+      <c r="X188" s="41"/>
+    </row>
+    <row r="189" spans="1:26" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A189" s="40" t="b">
+        <v>1</v>
+      </c>
+      <c r="B189" s="40" t="s">
+        <v>536</v>
+      </c>
+      <c r="C189" s="40" t="s">
+        <v>235</v>
+      </c>
+      <c r="D189" s="40" t="s">
+        <v>235</v>
+      </c>
+      <c r="E189" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="F189" s="40"/>
+      <c r="G189" s="40"/>
+      <c r="H189" s="40"/>
+      <c r="I189" s="40"/>
+      <c r="J189" s="40"/>
+      <c r="K189" s="40"/>
+      <c r="L189" s="40"/>
+      <c r="M189" s="40"/>
+      <c r="N189" s="40"/>
+      <c r="O189" s="40"/>
+      <c r="P189" s="40"/>
+      <c r="Q189" s="40"/>
+      <c r="R189" s="40"/>
+      <c r="S189" s="40"/>
+      <c r="T189" s="40"/>
+      <c r="U189" s="40"/>
+      <c r="V189" s="40"/>
+      <c r="W189" s="40"/>
+      <c r="X189" s="40"/>
+    </row>
+    <row r="190" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A190" s="10"/>
+      <c r="B190" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C190" s="10"/>
+      <c r="D190" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="E190" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="F190" s="10"/>
+      <c r="G190" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="H190" s="10"/>
+      <c r="I190" s="10" t="s">
+        <v>409</v>
+      </c>
+      <c r="J190" s="10"/>
+      <c r="K190" s="10"/>
+      <c r="L190" s="10"/>
+      <c r="M190" s="10"/>
+      <c r="N190" s="10"/>
+      <c r="O190" s="10"/>
+      <c r="P190" s="10"/>
+      <c r="Q190" s="10"/>
+      <c r="R190" s="10"/>
+      <c r="S190" s="10"/>
+      <c r="T190" s="10"/>
+      <c r="U190" s="10"/>
+      <c r="V190" s="10"/>
+      <c r="W190" s="10"/>
+      <c r="X190" s="10"/>
+      <c r="Y190" s="15"/>
+      <c r="Z190" s="15"/>
+    </row>
+    <row r="191" spans="1:26" s="37" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A191" s="41"/>
+      <c r="B191" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="C191" s="41"/>
+      <c r="D191" s="41" t="s">
+        <v>537</v>
+      </c>
+      <c r="E191" s="41" t="s">
+        <v>237</v>
+      </c>
+      <c r="F191" s="41"/>
+      <c r="G191" s="41" t="s">
+        <v>170</v>
+      </c>
+      <c r="H191" s="41"/>
+      <c r="I191" s="41">
+        <v>0.5</v>
+      </c>
+      <c r="J191" s="41"/>
+      <c r="K191" s="41">
+        <v>0</v>
+      </c>
+      <c r="L191" s="41">
+        <v>1</v>
+      </c>
+      <c r="M191" s="41">
+        <v>0.5</v>
+      </c>
+      <c r="N191" s="41">
+        <v>0.1666667</v>
+      </c>
+      <c r="O191" s="41"/>
+      <c r="P191" s="41"/>
+      <c r="Q191" s="41"/>
+      <c r="R191" s="41" t="s">
+        <v>224</v>
+      </c>
+      <c r="S191" s="41"/>
+      <c r="T191" s="41"/>
+      <c r="U191" s="41"/>
+      <c r="V191" s="41"/>
+      <c r="W191" s="41"/>
+      <c r="X191" s="41"/>
+    </row>
+    <row r="192" spans="1:26" s="39" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A192" s="42" t="b">
+        <v>1</v>
+      </c>
+      <c r="B192" s="42" t="s">
         <v>284</v>
       </c>
-      <c r="C183" s="42" t="s">
+      <c r="C192" s="42" t="s">
         <v>285</v>
       </c>
-      <c r="D183" s="42" t="s">
+      <c r="D192" s="42" t="s">
         <v>285</v>
       </c>
-      <c r="E183" s="42" t="s">
+      <c r="E192" s="42" t="s">
         <v>283</v>
       </c>
-      <c r="F183" s="42"/>
-      <c r="G183" s="42"/>
-      <c r="H183" s="43"/>
-      <c r="I183" s="43"/>
-      <c r="J183" s="42"/>
-      <c r="K183" s="42"/>
-      <c r="L183" s="42"/>
-      <c r="M183" s="42"/>
-      <c r="N183" s="42"/>
-      <c r="O183" s="42"/>
-      <c r="P183" s="42"/>
-      <c r="Q183" s="42"/>
-      <c r="R183" s="42"/>
-      <c r="S183" s="42"/>
-      <c r="T183" s="42"/>
-      <c r="U183" s="42"/>
-      <c r="V183" s="42"/>
-      <c r="W183" s="42"/>
-      <c r="X183" s="42"/>
-    </row>
-    <row r="184" spans="1:26" s="39" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A184" s="42" t="b">
+      <c r="F192" s="42"/>
+      <c r="G192" s="42"/>
+      <c r="H192" s="43"/>
+      <c r="I192" s="43"/>
+      <c r="J192" s="42"/>
+      <c r="K192" s="42"/>
+      <c r="L192" s="42"/>
+      <c r="M192" s="42"/>
+      <c r="N192" s="42"/>
+      <c r="O192" s="42"/>
+      <c r="P192" s="42"/>
+      <c r="Q192" s="42"/>
+      <c r="R192" s="42"/>
+      <c r="S192" s="42"/>
+      <c r="T192" s="42"/>
+      <c r="U192" s="42"/>
+      <c r="V192" s="42"/>
+      <c r="W192" s="42"/>
+      <c r="X192" s="42"/>
+    </row>
+    <row r="193" spans="1:24" s="39" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A193" s="42" t="b">
         <v>1</v>
       </c>
-      <c r="B184" s="42" t="s">
+      <c r="B193" s="42" t="s">
         <v>539</v>
       </c>
-      <c r="C184" s="42" t="s">
+      <c r="C193" s="42" t="s">
         <v>540</v>
       </c>
-      <c r="D184" s="42" t="s">
+      <c r="D193" s="42" t="s">
         <v>540</v>
       </c>
-      <c r="E184" s="42" t="s">
+      <c r="E193" s="42" t="s">
         <v>283</v>
       </c>
-      <c r="F184" s="42"/>
-      <c r="G184" s="42"/>
-      <c r="H184" s="43"/>
-      <c r="I184" s="43"/>
-      <c r="J184" s="42"/>
-      <c r="K184" s="42"/>
-      <c r="L184" s="42"/>
-      <c r="M184" s="42"/>
-      <c r="N184" s="42"/>
-      <c r="O184" s="42"/>
-      <c r="P184" s="42"/>
-      <c r="Q184" s="42"/>
-      <c r="R184" s="42"/>
-      <c r="S184" s="42"/>
-      <c r="T184" s="42"/>
-      <c r="U184" s="42"/>
-      <c r="V184" s="42"/>
-      <c r="W184" s="42"/>
-      <c r="X184" s="42"/>
-    </row>
-    <row r="185" spans="1:26" s="39" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A185" s="42" t="b">
+      <c r="F193" s="42"/>
+      <c r="G193" s="42"/>
+      <c r="H193" s="43"/>
+      <c r="I193" s="43"/>
+      <c r="J193" s="42"/>
+      <c r="K193" s="42"/>
+      <c r="L193" s="42"/>
+      <c r="M193" s="42"/>
+      <c r="N193" s="42"/>
+      <c r="O193" s="42"/>
+      <c r="P193" s="42"/>
+      <c r="Q193" s="42"/>
+      <c r="R193" s="42"/>
+      <c r="S193" s="42"/>
+      <c r="T193" s="42"/>
+      <c r="U193" s="42"/>
+      <c r="V193" s="42"/>
+      <c r="W193" s="42"/>
+      <c r="X193" s="42"/>
+    </row>
+    <row r="194" spans="1:24" s="39" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A194" s="42" t="b">
         <v>1</v>
       </c>
-      <c r="B185" s="42" t="s">
+      <c r="B194" s="42" t="s">
         <v>352</v>
       </c>
-      <c r="C185" s="42" t="s">
+      <c r="C194" s="42" t="s">
         <v>351</v>
       </c>
-      <c r="D185" s="42" t="s">
+      <c r="D194" s="42" t="s">
         <v>351</v>
       </c>
-      <c r="E185" s="42" t="s">
+      <c r="E194" s="42" t="s">
         <v>283</v>
       </c>
-      <c r="F185" s="42"/>
-      <c r="G185" s="42"/>
-      <c r="H185" s="43"/>
-      <c r="I185" s="43"/>
-      <c r="J185" s="42"/>
-      <c r="K185" s="42"/>
-      <c r="L185" s="42"/>
-      <c r="M185" s="42"/>
-      <c r="N185" s="42"/>
-      <c r="O185" s="42"/>
-      <c r="P185" s="42"/>
-      <c r="Q185" s="42"/>
-      <c r="R185" s="42"/>
-      <c r="S185" s="42"/>
-      <c r="T185" s="42"/>
-      <c r="U185" s="42"/>
-      <c r="V185" s="42"/>
-      <c r="W185" s="42"/>
-      <c r="X185" s="42"/>
+      <c r="F194" s="42"/>
+      <c r="G194" s="42"/>
+      <c r="H194" s="43"/>
+      <c r="I194" s="43"/>
+      <c r="J194" s="42"/>
+      <c r="K194" s="42"/>
+      <c r="L194" s="42"/>
+      <c r="M194" s="42"/>
+      <c r="N194" s="42"/>
+      <c r="O194" s="42"/>
+      <c r="P194" s="42"/>
+      <c r="Q194" s="42"/>
+      <c r="R194" s="42"/>
+      <c r="S194" s="42"/>
+      <c r="T194" s="42"/>
+      <c r="U194" s="42"/>
+      <c r="V194" s="42"/>
+      <c r="W194" s="42"/>
+      <c r="X194" s="42"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:AA3"/>
@@ -13491,7 +13896,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M79"/>
+  <dimension ref="A1:M82"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
@@ -14237,10 +14642,10 @@
     </row>
     <row r="29" spans="1:13" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="49" t="s">
-        <v>316</v>
+        <v>597</v>
       </c>
       <c r="D29" s="49" t="s">
-        <v>480</v>
+        <v>598</v>
       </c>
       <c r="F29" s="49" t="s">
         <v>286</v>
@@ -14257,10 +14662,10 @@
     </row>
     <row r="30" spans="1:13" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="49" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D30" s="49" t="s">
-        <v>436</v>
+        <v>480</v>
       </c>
       <c r="F30" s="49" t="s">
         <v>286</v>
@@ -14277,10 +14682,10 @@
     </row>
     <row r="31" spans="1:13" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="49" t="s">
-        <v>318</v>
+        <v>599</v>
       </c>
       <c r="D31" s="49" t="s">
-        <v>472</v>
+        <v>600</v>
       </c>
       <c r="F31" s="49" t="s">
         <v>286</v>
@@ -14297,10 +14702,10 @@
     </row>
     <row r="32" spans="1:13" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="49" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D32" s="49" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="F32" s="49" t="s">
         <v>286</v>
@@ -14317,10 +14722,10 @@
     </row>
     <row r="33" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="49" t="s">
-        <v>492</v>
+        <v>318</v>
       </c>
       <c r="D33" s="49" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="F33" s="49" t="s">
         <v>286</v>
@@ -14337,10 +14742,10 @@
     </row>
     <row r="34" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="49" t="s">
-        <v>493</v>
+        <v>319</v>
       </c>
       <c r="D34" s="49" t="s">
-        <v>474</v>
+        <v>437</v>
       </c>
       <c r="F34" s="49" t="s">
         <v>286</v>
@@ -14357,10 +14762,10 @@
     </row>
     <row r="35" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="49" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="D35" s="49" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="F35" s="49" t="s">
         <v>286</v>
@@ -14377,10 +14782,10 @@
     </row>
     <row r="36" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="49" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="D36" s="49" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="F36" s="49" t="s">
         <v>286</v>
@@ -14397,10 +14802,10 @@
     </row>
     <row r="37" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="49" t="s">
-        <v>321</v>
+        <v>494</v>
       </c>
       <c r="D37" s="49" t="s">
-        <v>434</v>
+        <v>476</v>
       </c>
       <c r="F37" s="49" t="s">
         <v>286</v>
@@ -14417,10 +14822,10 @@
     </row>
     <row r="38" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="49" t="s">
-        <v>346</v>
+        <v>495</v>
       </c>
       <c r="D38" s="49" t="s">
-        <v>483</v>
+        <v>473</v>
       </c>
       <c r="F38" s="49" t="s">
         <v>286</v>
@@ -14437,10 +14842,10 @@
     </row>
     <row r="39" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="49" t="s">
-        <v>322</v>
+        <v>604</v>
       </c>
       <c r="D39" s="49" t="s">
-        <v>481</v>
+        <v>605</v>
       </c>
       <c r="F39" s="49" t="s">
         <v>286</v>
@@ -14457,10 +14862,10 @@
     </row>
     <row r="40" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="49" t="s">
-        <v>368</v>
+        <v>321</v>
       </c>
       <c r="D40" s="49" t="s">
-        <v>444</v>
+        <v>434</v>
       </c>
       <c r="F40" s="49" t="s">
         <v>286</v>
@@ -14477,10 +14882,10 @@
     </row>
     <row r="41" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="49" t="s">
-        <v>360</v>
+        <v>346</v>
       </c>
       <c r="D41" s="49" t="s">
-        <v>448</v>
+        <v>483</v>
       </c>
       <c r="F41" s="49" t="s">
         <v>286</v>
@@ -14497,10 +14902,10 @@
     </row>
     <row r="42" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="49" t="s">
-        <v>361</v>
+        <v>322</v>
       </c>
       <c r="D42" s="49" t="s">
-        <v>445</v>
+        <v>481</v>
       </c>
       <c r="F42" s="49" t="s">
         <v>286</v>
@@ -14517,10 +14922,10 @@
     </row>
     <row r="43" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="49" t="s">
-        <v>363</v>
+        <v>368</v>
       </c>
       <c r="D43" s="49" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="F43" s="49" t="s">
         <v>286</v>
@@ -14537,10 +14942,10 @@
     </row>
     <row r="44" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="49" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D44" s="49" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="F44" s="49" t="s">
         <v>286</v>
@@ -14557,10 +14962,10 @@
     </row>
     <row r="45" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="49" t="s">
-        <v>583</v>
+        <v>361</v>
       </c>
       <c r="D45" s="49" t="s">
-        <v>584</v>
+        <v>445</v>
       </c>
       <c r="F45" s="49" t="s">
         <v>286</v>
@@ -14577,10 +14982,10 @@
     </row>
     <row r="46" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="49" t="s">
-        <v>585</v>
+        <v>363</v>
       </c>
       <c r="D46" s="49" t="s">
-        <v>586</v>
+        <v>447</v>
       </c>
       <c r="F46" s="49" t="s">
         <v>286</v>
@@ -14597,10 +15002,10 @@
     </row>
     <row r="47" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="49" t="s">
-        <v>323</v>
+        <v>362</v>
       </c>
       <c r="D47" s="49" t="s">
-        <v>471</v>
+        <v>446</v>
       </c>
       <c r="F47" s="49" t="s">
         <v>286</v>
@@ -14617,10 +15022,10 @@
     </row>
     <row r="48" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="49" t="s">
-        <v>324</v>
+        <v>583</v>
       </c>
       <c r="D48" s="49" t="s">
-        <v>431</v>
+        <v>584</v>
       </c>
       <c r="F48" s="49" t="s">
         <v>286</v>
@@ -14637,10 +15042,10 @@
     </row>
     <row r="49" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="49" t="s">
-        <v>325</v>
+        <v>585</v>
       </c>
       <c r="D49" s="49" t="s">
-        <v>432</v>
+        <v>586</v>
       </c>
       <c r="F49" s="49" t="s">
         <v>286</v>
@@ -14657,10 +15062,10 @@
     </row>
     <row r="50" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="49" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="D50" s="49" t="s">
-        <v>430</v>
+        <v>471</v>
       </c>
       <c r="F50" s="49" t="s">
         <v>286</v>
@@ -14677,10 +15082,10 @@
     </row>
     <row r="51" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="49" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="D51" s="49" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="F51" s="49" t="s">
         <v>286</v>
@@ -14697,10 +15102,10 @@
     </row>
     <row r="52" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="49" t="s">
-        <v>350</v>
+        <v>325</v>
       </c>
       <c r="D52" s="49" t="s">
-        <v>457</v>
+        <v>432</v>
       </c>
       <c r="F52" s="49" t="s">
         <v>286</v>
@@ -14717,10 +15122,10 @@
     </row>
     <row r="53" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="49" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D53" s="49" t="s">
-        <v>470</v>
+        <v>430</v>
       </c>
       <c r="F53" s="49" t="s">
         <v>286</v>
@@ -14737,10 +15142,10 @@
     </row>
     <row r="54" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="49" t="s">
-        <v>496</v>
+        <v>327</v>
       </c>
       <c r="D54" s="49" t="s">
-        <v>459</v>
+        <v>429</v>
       </c>
       <c r="F54" s="49" t="s">
         <v>286</v>
@@ -14757,10 +15162,10 @@
     </row>
     <row r="55" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="49" t="s">
-        <v>497</v>
+        <v>350</v>
       </c>
       <c r="D55" s="49" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="F55" s="49" t="s">
         <v>286</v>
@@ -14777,10 +15182,10 @@
     </row>
     <row r="56" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="49" t="s">
-        <v>498</v>
+        <v>328</v>
       </c>
       <c r="D56" s="49" t="s">
-        <v>461</v>
+        <v>470</v>
       </c>
       <c r="F56" s="49" t="s">
         <v>286</v>
@@ -14797,10 +15202,10 @@
     </row>
     <row r="57" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="49" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="D57" s="49" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="F57" s="49" t="s">
         <v>286</v>
@@ -14817,10 +15222,10 @@
     </row>
     <row r="58" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="49" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="D58" s="49" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="F58" s="49" t="s">
         <v>286</v>
@@ -14837,10 +15242,10 @@
     </row>
     <row r="59" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="49" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="D59" s="49" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="F59" s="49" t="s">
         <v>286</v>
@@ -14857,10 +15262,10 @@
     </row>
     <row r="60" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="49" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="D60" s="49" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="F60" s="49" t="s">
         <v>286</v>
@@ -14877,10 +15282,10 @@
     </row>
     <row r="61" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="49" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="D61" s="49" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="F61" s="49" t="s">
         <v>286</v>
@@ -14895,72 +15300,72 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="48" t="s">
-        <v>541</v>
-      </c>
-      <c r="D62" s="14" t="s">
-        <v>564</v>
-      </c>
-      <c r="F62" s="14" t="s">
+    <row r="62" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="49" t="s">
+        <v>501</v>
+      </c>
+      <c r="D62" s="49" t="s">
+        <v>464</v>
+      </c>
+      <c r="F62" s="49" t="s">
         <v>286</v>
       </c>
-      <c r="G62" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="H62" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="I62" s="14" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="48" t="s">
-        <v>542</v>
-      </c>
-      <c r="D63" s="14" t="s">
-        <v>565</v>
-      </c>
-      <c r="F63" s="14" t="s">
+      <c r="G62" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H62" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I62" s="49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="49" t="s">
+        <v>502</v>
+      </c>
+      <c r="D63" s="49" t="s">
+        <v>465</v>
+      </c>
+      <c r="F63" s="49" t="s">
         <v>286</v>
       </c>
-      <c r="G63" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="H63" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="I63" s="14" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="48" t="s">
-        <v>543</v>
-      </c>
-      <c r="D64" s="14" t="s">
-        <v>566</v>
-      </c>
-      <c r="F64" s="14" t="s">
+      <c r="G63" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H63" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I63" s="49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="49" t="s">
+        <v>503</v>
+      </c>
+      <c r="D64" s="49" t="s">
+        <v>466</v>
+      </c>
+      <c r="F64" s="49" t="s">
         <v>286</v>
       </c>
-      <c r="G64" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="H64" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="I64" s="14" t="b">
+      <c r="G64" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H64" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I64" s="49" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="48" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="D65" s="14" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="F65" s="14" t="s">
         <v>286</v>
@@ -14977,10 +15382,10 @@
     </row>
     <row r="66" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="48" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="D66" s="14" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="F66" s="14" t="s">
         <v>286</v>
@@ -14997,10 +15402,10 @@
     </row>
     <row r="67" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="48" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="D67" s="14" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="F67" s="14" t="s">
         <v>286</v>
@@ -15017,10 +15422,10 @@
     </row>
     <row r="68" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="48" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="D68" s="14" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="F68" s="14" t="s">
         <v>286</v>
@@ -15037,10 +15442,10 @@
     </row>
     <row r="69" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="48" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="D69" s="14" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="F69" s="14" t="s">
         <v>286</v>
@@ -15057,10 +15462,10 @@
     </row>
     <row r="70" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="48" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="D70" s="14" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="F70" s="14" t="s">
         <v>286</v>
@@ -15077,10 +15482,10 @@
     </row>
     <row r="71" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="48" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="D71" s="14" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="F71" s="14" t="s">
         <v>286</v>
@@ -15097,10 +15502,10 @@
     </row>
     <row r="72" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="48" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D72" s="14" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="F72" s="14" t="s">
         <v>286</v>
@@ -15117,10 +15522,10 @@
     </row>
     <row r="73" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="48" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="D73" s="14" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="F73" s="14" t="s">
         <v>286</v>
@@ -15136,11 +15541,11 @@
       </c>
     </row>
     <row r="74" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="14" t="s">
-        <v>553</v>
+      <c r="A74" s="48" t="s">
+        <v>550</v>
       </c>
       <c r="D74" s="14" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="F74" s="14" t="s">
         <v>286</v>
@@ -15156,11 +15561,11 @@
       </c>
     </row>
     <row r="75" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="14" t="s">
-        <v>554</v>
+      <c r="A75" s="48" t="s">
+        <v>551</v>
       </c>
       <c r="D75" s="14" t="s">
-        <v>563</v>
+        <v>574</v>
       </c>
       <c r="F75" s="14" t="s">
         <v>286</v>
@@ -15176,11 +15581,11 @@
       </c>
     </row>
     <row r="76" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="14" t="s">
-        <v>555</v>
+      <c r="A76" s="48" t="s">
+        <v>552</v>
       </c>
       <c r="D76" s="14" t="s">
-        <v>562</v>
+        <v>575</v>
       </c>
       <c r="F76" s="14" t="s">
         <v>286</v>
@@ -15197,10 +15602,10 @@
     </row>
     <row r="77" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="14" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="D77" s="14" t="s">
-        <v>561</v>
+        <v>576</v>
       </c>
       <c r="F77" s="14" t="s">
         <v>286</v>
@@ -15217,10 +15622,10 @@
     </row>
     <row r="78" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="14" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="D78" s="14" t="s">
-        <v>560</v>
+        <v>563</v>
       </c>
       <c r="F78" s="14" t="s">
         <v>286</v>
@@ -15237,10 +15642,10 @@
     </row>
     <row r="79" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="14" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="D79" s="14" t="s">
-        <v>559</v>
+        <v>562</v>
       </c>
       <c r="F79" s="14" t="s">
         <v>286</v>
@@ -15252,6 +15657,66 @@
         <v>0</v>
       </c>
       <c r="I79" s="14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="14" t="s">
+        <v>556</v>
+      </c>
+      <c r="D80" s="14" t="s">
+        <v>561</v>
+      </c>
+      <c r="F80" s="14" t="s">
+        <v>286</v>
+      </c>
+      <c r="G80" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H80" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I80" s="14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="14" t="s">
+        <v>557</v>
+      </c>
+      <c r="D81" s="14" t="s">
+        <v>560</v>
+      </c>
+      <c r="F81" s="14" t="s">
+        <v>286</v>
+      </c>
+      <c r="G81" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H81" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I81" s="14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="14" t="s">
+        <v>558</v>
+      </c>
+      <c r="D82" s="14" t="s">
+        <v>559</v>
+      </c>
+      <c r="F82" s="14" t="s">
+        <v>286</v>
+      </c>
+      <c r="G82" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H82" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I82" s="14" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added airflow measure into workflow, addresses #4. Currently disabled and untested due to OS error.
</commit_message>
<xml_diff>
--- a/projects/res_stock_national_existing.xlsx
+++ b/projects/res_stock_national_existing.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1434" uniqueCount="606">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1519" uniqueCount="631">
   <si>
     <t>type</t>
   </si>
@@ -1650,9 +1650,6 @@
     <t>Misc Well Pump Sample Value</t>
   </si>
   <si>
-    <t>1.18.0-rc0</t>
-  </si>
-  <si>
     <t>Standard Reports</t>
   </si>
   <si>
@@ -1852,6 +1849,84 @@
   </si>
   <si>
     <t>res_stock_reporting.Thermal Mass Furniture</t>
+  </si>
+  <si>
+    <t>Set Ducts</t>
+  </si>
+  <si>
+    <t>Ducts.tsv</t>
+  </si>
+  <si>
+    <t>Ducts Sample Value</t>
+  </si>
+  <si>
+    <t>Set Infiltration</t>
+  </si>
+  <si>
+    <t>Infiltration.tsv</t>
+  </si>
+  <si>
+    <t>Infiltration Sample Value</t>
+  </si>
+  <si>
+    <t>Set Natural Ventilation</t>
+  </si>
+  <si>
+    <t>Natural Ventilation.tsv</t>
+  </si>
+  <si>
+    <t>Natural Ventilation Sample Value</t>
+  </si>
+  <si>
+    <t>Set Mechanical Ventilation</t>
+  </si>
+  <si>
+    <t>Mechanical Ventilation.tsv</t>
+  </si>
+  <si>
+    <t>Mechanical Ventilation Sample Value</t>
+  </si>
+  <si>
+    <t>Set Airflow</t>
+  </si>
+  <si>
+    <t>Airflow.tsv</t>
+  </si>
+  <si>
+    <t>Airflow Sample Value</t>
+  </si>
+  <si>
+    <t>Ducts</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.Ducts</t>
+  </si>
+  <si>
+    <t>Infiltration</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.Infiltration</t>
+  </si>
+  <si>
+    <t>Natural Ventilation</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.Natural Ventilation</t>
+  </si>
+  <si>
+    <t>Mechanical Ventilation</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.Mechanical Ventilation</t>
+  </si>
+  <si>
+    <t>Airflow</t>
+  </si>
+  <si>
+    <t>res_stock_reporting.Airflow</t>
+  </si>
+  <si>
+    <t>1.19.0-rc0</t>
   </si>
 </sst>
 </file>
@@ -5502,7 +5577,7 @@
         <v>75</v>
       </c>
       <c r="B5" s="44" t="s">
-        <v>538</v>
+        <v>630</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>155</v>
@@ -5635,7 +5710,7 @@
         <v>23</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="F15" s="22" t="s">
         <v>156</v>
@@ -5948,7 +6023,7 @@
         <v>26</v>
       </c>
       <c r="B38" s="25" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="40" spans="1:6" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -6078,7 +6153,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z194"/>
+  <dimension ref="A1:Z209"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
@@ -6262,7 +6337,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="40" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="C4" s="40" t="s">
         <v>240</v>
@@ -6311,7 +6386,7 @@
       </c>
       <c r="H5" s="10"/>
       <c r="I5" s="10" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="J5" s="10"/>
       <c r="K5" s="10"/>
@@ -9456,7 +9531,7 @@
         <v>1</v>
       </c>
       <c r="B84" s="40" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="C84" s="40" t="s">
         <v>235</v>
@@ -9505,7 +9580,7 @@
       </c>
       <c r="H85" s="10"/>
       <c r="I85" s="10" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="J85" s="10"/>
       <c r="K85" s="10"/>
@@ -9532,7 +9607,7 @@
       </c>
       <c r="C86" s="41"/>
       <c r="D86" s="41" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="E86" s="41" t="s">
         <v>237</v>
@@ -9696,7 +9771,7 @@
         <v>1</v>
       </c>
       <c r="B90" s="40" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="C90" s="40" t="s">
         <v>235</v>
@@ -9745,7 +9820,7 @@
       </c>
       <c r="H91" s="10"/>
       <c r="I91" s="10" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="J91" s="10"/>
       <c r="K91" s="10"/>
@@ -9772,7 +9847,7 @@
       </c>
       <c r="C92" s="41"/>
       <c r="D92" s="41" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="E92" s="41" t="s">
         <v>237</v>
@@ -10656,7 +10731,7 @@
         <v>1</v>
       </c>
       <c r="B114" s="40" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="C114" s="40" t="s">
         <v>235</v>
@@ -10705,7 +10780,7 @@
       </c>
       <c r="H115" s="10"/>
       <c r="I115" s="10" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="J115" s="10"/>
       <c r="K115" s="10"/>
@@ -10732,7 +10807,7 @@
       </c>
       <c r="C116" s="41"/>
       <c r="D116" s="41" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="E116" s="41" t="s">
         <v>237</v>
@@ -11736,7 +11811,7 @@
         <v>1</v>
       </c>
       <c r="B141" s="40" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="C141" s="40" t="s">
         <v>235</v>
@@ -11785,7 +11860,7 @@
       </c>
       <c r="H142" s="10"/>
       <c r="I142" s="10" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="J142" s="10"/>
       <c r="K142" s="10"/>
@@ -11812,7 +11887,7 @@
       </c>
       <c r="C143" s="41"/>
       <c r="D143" s="41" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="E143" s="41" t="s">
         <v>237</v>
@@ -11856,7 +11931,7 @@
         <v>1</v>
       </c>
       <c r="B144" s="40" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="C144" s="40" t="s">
         <v>235</v>
@@ -11905,7 +11980,7 @@
       </c>
       <c r="H145" s="10"/>
       <c r="I145" s="10" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="J145" s="10"/>
       <c r="K145" s="10"/>
@@ -11932,7 +12007,7 @@
       </c>
       <c r="C146" s="41"/>
       <c r="D146" s="41" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="E146" s="41" t="s">
         <v>237</v>
@@ -13771,113 +13846,713 @@
       <c r="W191" s="41"/>
       <c r="X191" s="41"/>
     </row>
-    <row r="192" spans="1:26" s="39" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A192" s="42" t="b">
+    <row r="192" spans="1:26" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A192" s="40" t="b">
         <v>1</v>
       </c>
-      <c r="B192" s="42" t="s">
+      <c r="B192" s="40" t="s">
+        <v>605</v>
+      </c>
+      <c r="C192" s="40" t="s">
+        <v>235</v>
+      </c>
+      <c r="D192" s="40" t="s">
+        <v>235</v>
+      </c>
+      <c r="E192" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="F192" s="40"/>
+      <c r="G192" s="40"/>
+      <c r="H192" s="40"/>
+      <c r="I192" s="40"/>
+      <c r="J192" s="40"/>
+      <c r="K192" s="40"/>
+      <c r="L192" s="40"/>
+      <c r="M192" s="40"/>
+      <c r="N192" s="40"/>
+      <c r="O192" s="40"/>
+      <c r="P192" s="40"/>
+      <c r="Q192" s="40"/>
+      <c r="R192" s="40"/>
+      <c r="S192" s="40"/>
+      <c r="T192" s="40"/>
+      <c r="U192" s="40"/>
+      <c r="V192" s="40"/>
+      <c r="W192" s="40"/>
+      <c r="X192" s="40"/>
+    </row>
+    <row r="193" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A193" s="10"/>
+      <c r="B193" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C193" s="10"/>
+      <c r="D193" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="E193" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="F193" s="10"/>
+      <c r="G193" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="H193" s="10"/>
+      <c r="I193" s="10" t="s">
+        <v>606</v>
+      </c>
+      <c r="J193" s="10"/>
+      <c r="K193" s="10"/>
+      <c r="L193" s="10"/>
+      <c r="M193" s="10"/>
+      <c r="N193" s="10"/>
+      <c r="O193" s="10"/>
+      <c r="P193" s="10"/>
+      <c r="Q193" s="10"/>
+      <c r="R193" s="10"/>
+      <c r="S193" s="10"/>
+      <c r="T193" s="10"/>
+      <c r="U193" s="10"/>
+      <c r="V193" s="10"/>
+      <c r="W193" s="10"/>
+      <c r="X193" s="10"/>
+      <c r="Y193" s="15"/>
+      <c r="Z193" s="15"/>
+    </row>
+    <row r="194" spans="1:26" s="37" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A194" s="41"/>
+      <c r="B194" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="C194" s="41"/>
+      <c r="D194" s="41" t="s">
+        <v>607</v>
+      </c>
+      <c r="E194" s="41" t="s">
+        <v>237</v>
+      </c>
+      <c r="F194" s="41"/>
+      <c r="G194" s="41" t="s">
+        <v>170</v>
+      </c>
+      <c r="H194" s="41"/>
+      <c r="I194" s="41">
+        <v>0.5</v>
+      </c>
+      <c r="J194" s="41"/>
+      <c r="K194" s="41">
+        <v>0</v>
+      </c>
+      <c r="L194" s="41">
+        <v>1</v>
+      </c>
+      <c r="M194" s="41">
+        <v>0.5</v>
+      </c>
+      <c r="N194" s="41">
+        <v>0.1666667</v>
+      </c>
+      <c r="O194" s="41"/>
+      <c r="P194" s="41"/>
+      <c r="Q194" s="41"/>
+      <c r="R194" s="41" t="s">
+        <v>224</v>
+      </c>
+      <c r="S194" s="41"/>
+      <c r="T194" s="41"/>
+      <c r="U194" s="41"/>
+      <c r="V194" s="41"/>
+      <c r="W194" s="41"/>
+      <c r="X194" s="41"/>
+    </row>
+    <row r="195" spans="1:26" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A195" s="40" t="b">
+        <v>1</v>
+      </c>
+      <c r="B195" s="40" t="s">
+        <v>608</v>
+      </c>
+      <c r="C195" s="40" t="s">
+        <v>235</v>
+      </c>
+      <c r="D195" s="40" t="s">
+        <v>235</v>
+      </c>
+      <c r="E195" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="F195" s="40"/>
+      <c r="G195" s="40"/>
+      <c r="H195" s="40"/>
+      <c r="I195" s="40"/>
+      <c r="J195" s="40"/>
+      <c r="K195" s="40"/>
+      <c r="L195" s="40"/>
+      <c r="M195" s="40"/>
+      <c r="N195" s="40"/>
+      <c r="O195" s="40"/>
+      <c r="P195" s="40"/>
+      <c r="Q195" s="40"/>
+      <c r="R195" s="40"/>
+      <c r="S195" s="40"/>
+      <c r="T195" s="40"/>
+      <c r="U195" s="40"/>
+      <c r="V195" s="40"/>
+      <c r="W195" s="40"/>
+      <c r="X195" s="40"/>
+    </row>
+    <row r="196" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A196" s="10"/>
+      <c r="B196" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C196" s="10"/>
+      <c r="D196" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="E196" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="F196" s="10"/>
+      <c r="G196" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="H196" s="10"/>
+      <c r="I196" s="10" t="s">
+        <v>609</v>
+      </c>
+      <c r="J196" s="10"/>
+      <c r="K196" s="10"/>
+      <c r="L196" s="10"/>
+      <c r="M196" s="10"/>
+      <c r="N196" s="10"/>
+      <c r="O196" s="10"/>
+      <c r="P196" s="10"/>
+      <c r="Q196" s="10"/>
+      <c r="R196" s="10"/>
+      <c r="S196" s="10"/>
+      <c r="T196" s="10"/>
+      <c r="U196" s="10"/>
+      <c r="V196" s="10"/>
+      <c r="W196" s="10"/>
+      <c r="X196" s="10"/>
+      <c r="Y196" s="15"/>
+      <c r="Z196" s="15"/>
+    </row>
+    <row r="197" spans="1:26" s="37" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A197" s="41"/>
+      <c r="B197" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="C197" s="41"/>
+      <c r="D197" s="41" t="s">
+        <v>610</v>
+      </c>
+      <c r="E197" s="41" t="s">
+        <v>237</v>
+      </c>
+      <c r="F197" s="41"/>
+      <c r="G197" s="41" t="s">
+        <v>170</v>
+      </c>
+      <c r="H197" s="41"/>
+      <c r="I197" s="41">
+        <v>0.5</v>
+      </c>
+      <c r="J197" s="41"/>
+      <c r="K197" s="41">
+        <v>0</v>
+      </c>
+      <c r="L197" s="41">
+        <v>1</v>
+      </c>
+      <c r="M197" s="41">
+        <v>0.5</v>
+      </c>
+      <c r="N197" s="41">
+        <v>0.1666667</v>
+      </c>
+      <c r="O197" s="41"/>
+      <c r="P197" s="41"/>
+      <c r="Q197" s="41"/>
+      <c r="R197" s="41" t="s">
+        <v>224</v>
+      </c>
+      <c r="S197" s="41"/>
+      <c r="T197" s="41"/>
+      <c r="U197" s="41"/>
+      <c r="V197" s="41"/>
+      <c r="W197" s="41"/>
+      <c r="X197" s="41"/>
+    </row>
+    <row r="198" spans="1:26" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A198" s="40" t="b">
+        <v>1</v>
+      </c>
+      <c r="B198" s="40" t="s">
+        <v>611</v>
+      </c>
+      <c r="C198" s="40" t="s">
+        <v>235</v>
+      </c>
+      <c r="D198" s="40" t="s">
+        <v>235</v>
+      </c>
+      <c r="E198" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="F198" s="40"/>
+      <c r="G198" s="40"/>
+      <c r="H198" s="40"/>
+      <c r="I198" s="40"/>
+      <c r="J198" s="40"/>
+      <c r="K198" s="40"/>
+      <c r="L198" s="40"/>
+      <c r="M198" s="40"/>
+      <c r="N198" s="40"/>
+      <c r="O198" s="40"/>
+      <c r="P198" s="40"/>
+      <c r="Q198" s="40"/>
+      <c r="R198" s="40"/>
+      <c r="S198" s="40"/>
+      <c r="T198" s="40"/>
+      <c r="U198" s="40"/>
+      <c r="V198" s="40"/>
+      <c r="W198" s="40"/>
+      <c r="X198" s="40"/>
+    </row>
+    <row r="199" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A199" s="10"/>
+      <c r="B199" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C199" s="10"/>
+      <c r="D199" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="E199" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="F199" s="10"/>
+      <c r="G199" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="H199" s="10"/>
+      <c r="I199" s="10" t="s">
+        <v>612</v>
+      </c>
+      <c r="J199" s="10"/>
+      <c r="K199" s="10"/>
+      <c r="L199" s="10"/>
+      <c r="M199" s="10"/>
+      <c r="N199" s="10"/>
+      <c r="O199" s="10"/>
+      <c r="P199" s="10"/>
+      <c r="Q199" s="10"/>
+      <c r="R199" s="10"/>
+      <c r="S199" s="10"/>
+      <c r="T199" s="10"/>
+      <c r="U199" s="10"/>
+      <c r="V199" s="10"/>
+      <c r="W199" s="10"/>
+      <c r="X199" s="10"/>
+      <c r="Y199" s="15"/>
+      <c r="Z199" s="15"/>
+    </row>
+    <row r="200" spans="1:26" s="37" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A200" s="41"/>
+      <c r="B200" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="C200" s="41"/>
+      <c r="D200" s="41" t="s">
+        <v>613</v>
+      </c>
+      <c r="E200" s="41" t="s">
+        <v>237</v>
+      </c>
+      <c r="F200" s="41"/>
+      <c r="G200" s="41" t="s">
+        <v>170</v>
+      </c>
+      <c r="H200" s="41"/>
+      <c r="I200" s="41">
+        <v>0.5</v>
+      </c>
+      <c r="J200" s="41"/>
+      <c r="K200" s="41">
+        <v>0</v>
+      </c>
+      <c r="L200" s="41">
+        <v>1</v>
+      </c>
+      <c r="M200" s="41">
+        <v>0.5</v>
+      </c>
+      <c r="N200" s="41">
+        <v>0.1666667</v>
+      </c>
+      <c r="O200" s="41"/>
+      <c r="P200" s="41"/>
+      <c r="Q200" s="41"/>
+      <c r="R200" s="41" t="s">
+        <v>224</v>
+      </c>
+      <c r="S200" s="41"/>
+      <c r="T200" s="41"/>
+      <c r="U200" s="41"/>
+      <c r="V200" s="41"/>
+      <c r="W200" s="41"/>
+      <c r="X200" s="41"/>
+    </row>
+    <row r="201" spans="1:26" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A201" s="40" t="b">
+        <v>1</v>
+      </c>
+      <c r="B201" s="40" t="s">
+        <v>614</v>
+      </c>
+      <c r="C201" s="40" t="s">
+        <v>235</v>
+      </c>
+      <c r="D201" s="40" t="s">
+        <v>235</v>
+      </c>
+      <c r="E201" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="F201" s="40"/>
+      <c r="G201" s="40"/>
+      <c r="H201" s="40"/>
+      <c r="I201" s="40"/>
+      <c r="J201" s="40"/>
+      <c r="K201" s="40"/>
+      <c r="L201" s="40"/>
+      <c r="M201" s="40"/>
+      <c r="N201" s="40"/>
+      <c r="O201" s="40"/>
+      <c r="P201" s="40"/>
+      <c r="Q201" s="40"/>
+      <c r="R201" s="40"/>
+      <c r="S201" s="40"/>
+      <c r="T201" s="40"/>
+      <c r="U201" s="40"/>
+      <c r="V201" s="40"/>
+      <c r="W201" s="40"/>
+      <c r="X201" s="40"/>
+    </row>
+    <row r="202" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A202" s="10"/>
+      <c r="B202" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C202" s="10"/>
+      <c r="D202" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="E202" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="F202" s="10"/>
+      <c r="G202" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="H202" s="10"/>
+      <c r="I202" s="10" t="s">
+        <v>615</v>
+      </c>
+      <c r="J202" s="10"/>
+      <c r="K202" s="10"/>
+      <c r="L202" s="10"/>
+      <c r="M202" s="10"/>
+      <c r="N202" s="10"/>
+      <c r="O202" s="10"/>
+      <c r="P202" s="10"/>
+      <c r="Q202" s="10"/>
+      <c r="R202" s="10"/>
+      <c r="S202" s="10"/>
+      <c r="T202" s="10"/>
+      <c r="U202" s="10"/>
+      <c r="V202" s="10"/>
+      <c r="W202" s="10"/>
+      <c r="X202" s="10"/>
+      <c r="Y202" s="15"/>
+      <c r="Z202" s="15"/>
+    </row>
+    <row r="203" spans="1:26" s="37" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A203" s="41"/>
+      <c r="B203" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="C203" s="41"/>
+      <c r="D203" s="41" t="s">
+        <v>616</v>
+      </c>
+      <c r="E203" s="41" t="s">
+        <v>237</v>
+      </c>
+      <c r="F203" s="41"/>
+      <c r="G203" s="41" t="s">
+        <v>170</v>
+      </c>
+      <c r="H203" s="41"/>
+      <c r="I203" s="41">
+        <v>0.5</v>
+      </c>
+      <c r="J203" s="41"/>
+      <c r="K203" s="41">
+        <v>0</v>
+      </c>
+      <c r="L203" s="41">
+        <v>1</v>
+      </c>
+      <c r="M203" s="41">
+        <v>0.5</v>
+      </c>
+      <c r="N203" s="41">
+        <v>0.1666667</v>
+      </c>
+      <c r="O203" s="41"/>
+      <c r="P203" s="41"/>
+      <c r="Q203" s="41"/>
+      <c r="R203" s="41" t="s">
+        <v>224</v>
+      </c>
+      <c r="S203" s="41"/>
+      <c r="T203" s="41"/>
+      <c r="U203" s="41"/>
+      <c r="V203" s="41"/>
+      <c r="W203" s="41"/>
+      <c r="X203" s="41"/>
+    </row>
+    <row r="204" spans="1:26" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A204" s="40" t="b">
+        <v>0</v>
+      </c>
+      <c r="B204" s="40" t="s">
+        <v>617</v>
+      </c>
+      <c r="C204" s="40" t="s">
+        <v>235</v>
+      </c>
+      <c r="D204" s="40" t="s">
+        <v>235</v>
+      </c>
+      <c r="E204" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="F204" s="40"/>
+      <c r="G204" s="40"/>
+      <c r="H204" s="40"/>
+      <c r="I204" s="40"/>
+      <c r="J204" s="40"/>
+      <c r="K204" s="40"/>
+      <c r="L204" s="40"/>
+      <c r="M204" s="40"/>
+      <c r="N204" s="40"/>
+      <c r="O204" s="40"/>
+      <c r="P204" s="40"/>
+      <c r="Q204" s="40"/>
+      <c r="R204" s="40"/>
+      <c r="S204" s="40"/>
+      <c r="T204" s="40"/>
+      <c r="U204" s="40"/>
+      <c r="V204" s="40"/>
+      <c r="W204" s="40"/>
+      <c r="X204" s="40"/>
+    </row>
+    <row r="205" spans="1:26" s="21" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A205" s="10"/>
+      <c r="B205" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C205" s="10"/>
+      <c r="D205" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="E205" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="F205" s="10"/>
+      <c r="G205" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="H205" s="10"/>
+      <c r="I205" s="10" t="s">
+        <v>618</v>
+      </c>
+      <c r="J205" s="10"/>
+      <c r="K205" s="10"/>
+      <c r="L205" s="10"/>
+      <c r="M205" s="10"/>
+      <c r="N205" s="10"/>
+      <c r="O205" s="10"/>
+      <c r="P205" s="10"/>
+      <c r="Q205" s="10"/>
+      <c r="R205" s="10"/>
+      <c r="S205" s="10"/>
+      <c r="T205" s="10"/>
+      <c r="U205" s="10"/>
+      <c r="V205" s="10"/>
+      <c r="W205" s="10"/>
+      <c r="X205" s="10"/>
+      <c r="Y205" s="15"/>
+      <c r="Z205" s="15"/>
+    </row>
+    <row r="206" spans="1:26" s="37" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A206" s="41"/>
+      <c r="B206" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="C206" s="41"/>
+      <c r="D206" s="41" t="s">
+        <v>619</v>
+      </c>
+      <c r="E206" s="41" t="s">
+        <v>237</v>
+      </c>
+      <c r="F206" s="41"/>
+      <c r="G206" s="41" t="s">
+        <v>170</v>
+      </c>
+      <c r="H206" s="41"/>
+      <c r="I206" s="41">
+        <v>0.5</v>
+      </c>
+      <c r="J206" s="41"/>
+      <c r="K206" s="41">
+        <v>0</v>
+      </c>
+      <c r="L206" s="41">
+        <v>1</v>
+      </c>
+      <c r="M206" s="41">
+        <v>0.5</v>
+      </c>
+      <c r="N206" s="41">
+        <v>0.1666667</v>
+      </c>
+      <c r="O206" s="41"/>
+      <c r="P206" s="41"/>
+      <c r="Q206" s="41"/>
+      <c r="R206" s="41" t="s">
+        <v>224</v>
+      </c>
+      <c r="S206" s="41"/>
+      <c r="T206" s="41"/>
+      <c r="U206" s="41"/>
+      <c r="V206" s="41"/>
+      <c r="W206" s="41"/>
+      <c r="X206" s="41"/>
+    </row>
+    <row r="207" spans="1:26" s="39" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A207" s="42" t="b">
+        <v>1</v>
+      </c>
+      <c r="B207" s="42" t="s">
         <v>284</v>
       </c>
-      <c r="C192" s="42" t="s">
+      <c r="C207" s="42" t="s">
         <v>285</v>
       </c>
-      <c r="D192" s="42" t="s">
+      <c r="D207" s="42" t="s">
         <v>285</v>
       </c>
-      <c r="E192" s="42" t="s">
+      <c r="E207" s="42" t="s">
         <v>283</v>
       </c>
-      <c r="F192" s="42"/>
-      <c r="G192" s="42"/>
-      <c r="H192" s="43"/>
-      <c r="I192" s="43"/>
-      <c r="J192" s="42"/>
-      <c r="K192" s="42"/>
-      <c r="L192" s="42"/>
-      <c r="M192" s="42"/>
-      <c r="N192" s="42"/>
-      <c r="O192" s="42"/>
-      <c r="P192" s="42"/>
-      <c r="Q192" s="42"/>
-      <c r="R192" s="42"/>
-      <c r="S192" s="42"/>
-      <c r="T192" s="42"/>
-      <c r="U192" s="42"/>
-      <c r="V192" s="42"/>
-      <c r="W192" s="42"/>
-      <c r="X192" s="42"/>
-    </row>
-    <row r="193" spans="1:24" s="39" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A193" s="42" t="b">
+      <c r="F207" s="42"/>
+      <c r="G207" s="42"/>
+      <c r="H207" s="43"/>
+      <c r="I207" s="43"/>
+      <c r="J207" s="42"/>
+      <c r="K207" s="42"/>
+      <c r="L207" s="42"/>
+      <c r="M207" s="42"/>
+      <c r="N207" s="42"/>
+      <c r="O207" s="42"/>
+      <c r="P207" s="42"/>
+      <c r="Q207" s="42"/>
+      <c r="R207" s="42"/>
+      <c r="S207" s="42"/>
+      <c r="T207" s="42"/>
+      <c r="U207" s="42"/>
+      <c r="V207" s="42"/>
+      <c r="W207" s="42"/>
+      <c r="X207" s="42"/>
+    </row>
+    <row r="208" spans="1:26" s="39" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A208" s="42" t="b">
         <v>1</v>
       </c>
-      <c r="B193" s="42" t="s">
+      <c r="B208" s="42" t="s">
+        <v>538</v>
+      </c>
+      <c r="C208" s="42" t="s">
         <v>539</v>
       </c>
-      <c r="C193" s="42" t="s">
-        <v>540</v>
-      </c>
-      <c r="D193" s="42" t="s">
-        <v>540</v>
-      </c>
-      <c r="E193" s="42" t="s">
+      <c r="D208" s="42" t="s">
+        <v>539</v>
+      </c>
+      <c r="E208" s="42" t="s">
         <v>283</v>
       </c>
-      <c r="F193" s="42"/>
-      <c r="G193" s="42"/>
-      <c r="H193" s="43"/>
-      <c r="I193" s="43"/>
-      <c r="J193" s="42"/>
-      <c r="K193" s="42"/>
-      <c r="L193" s="42"/>
-      <c r="M193" s="42"/>
-      <c r="N193" s="42"/>
-      <c r="O193" s="42"/>
-      <c r="P193" s="42"/>
-      <c r="Q193" s="42"/>
-      <c r="R193" s="42"/>
-      <c r="S193" s="42"/>
-      <c r="T193" s="42"/>
-      <c r="U193" s="42"/>
-      <c r="V193" s="42"/>
-      <c r="W193" s="42"/>
-      <c r="X193" s="42"/>
-    </row>
-    <row r="194" spans="1:24" s="39" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A194" s="42" t="b">
+      <c r="F208" s="42"/>
+      <c r="G208" s="42"/>
+      <c r="H208" s="43"/>
+      <c r="I208" s="43"/>
+      <c r="J208" s="42"/>
+      <c r="K208" s="42"/>
+      <c r="L208" s="42"/>
+      <c r="M208" s="42"/>
+      <c r="N208" s="42"/>
+      <c r="O208" s="42"/>
+      <c r="P208" s="42"/>
+      <c r="Q208" s="42"/>
+      <c r="R208" s="42"/>
+      <c r="S208" s="42"/>
+      <c r="T208" s="42"/>
+      <c r="U208" s="42"/>
+      <c r="V208" s="42"/>
+      <c r="W208" s="42"/>
+      <c r="X208" s="42"/>
+    </row>
+    <row r="209" spans="1:24" s="39" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A209" s="42" t="b">
         <v>1</v>
       </c>
-      <c r="B194" s="42" t="s">
+      <c r="B209" s="42" t="s">
         <v>352</v>
       </c>
-      <c r="C194" s="42" t="s">
+      <c r="C209" s="42" t="s">
         <v>351</v>
       </c>
-      <c r="D194" s="42" t="s">
+      <c r="D209" s="42" t="s">
         <v>351</v>
       </c>
-      <c r="E194" s="42" t="s">
+      <c r="E209" s="42" t="s">
         <v>283</v>
       </c>
-      <c r="F194" s="42"/>
-      <c r="G194" s="42"/>
-      <c r="H194" s="43"/>
-      <c r="I194" s="43"/>
-      <c r="J194" s="42"/>
-      <c r="K194" s="42"/>
-      <c r="L194" s="42"/>
-      <c r="M194" s="42"/>
-      <c r="N194" s="42"/>
-      <c r="O194" s="42"/>
-      <c r="P194" s="42"/>
-      <c r="Q194" s="42"/>
-      <c r="R194" s="42"/>
-      <c r="S194" s="42"/>
-      <c r="T194" s="42"/>
-      <c r="U194" s="42"/>
-      <c r="V194" s="42"/>
-      <c r="W194" s="42"/>
-      <c r="X194" s="42"/>
+      <c r="F209" s="42"/>
+      <c r="G209" s="42"/>
+      <c r="H209" s="43"/>
+      <c r="I209" s="43"/>
+      <c r="J209" s="42"/>
+      <c r="K209" s="42"/>
+      <c r="L209" s="42"/>
+      <c r="M209" s="42"/>
+      <c r="N209" s="42"/>
+      <c r="O209" s="42"/>
+      <c r="P209" s="42"/>
+      <c r="Q209" s="42"/>
+      <c r="R209" s="42"/>
+      <c r="S209" s="42"/>
+      <c r="T209" s="42"/>
+      <c r="U209" s="42"/>
+      <c r="V209" s="42"/>
+      <c r="W209" s="42"/>
+      <c r="X209" s="42"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:AA3"/>
@@ -13896,7 +14571,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M82"/>
+  <dimension ref="A1:M87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
@@ -14642,10 +15317,10 @@
     </row>
     <row r="29" spans="1:13" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="49" t="s">
+        <v>596</v>
+      </c>
+      <c r="D29" s="49" t="s">
         <v>597</v>
-      </c>
-      <c r="D29" s="49" t="s">
-        <v>598</v>
       </c>
       <c r="F29" s="49" t="s">
         <v>286</v>
@@ -14682,10 +15357,10 @@
     </row>
     <row r="31" spans="1:13" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="49" t="s">
+        <v>598</v>
+      </c>
+      <c r="D31" s="49" t="s">
         <v>599</v>
-      </c>
-      <c r="D31" s="49" t="s">
-        <v>600</v>
       </c>
       <c r="F31" s="49" t="s">
         <v>286</v>
@@ -14842,10 +15517,10 @@
     </row>
     <row r="39" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="49" t="s">
+        <v>603</v>
+      </c>
+      <c r="D39" s="49" t="s">
         <v>604</v>
-      </c>
-      <c r="D39" s="49" t="s">
-        <v>605</v>
       </c>
       <c r="F39" s="49" t="s">
         <v>286</v>
@@ -15022,10 +15697,10 @@
     </row>
     <row r="48" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="49" t="s">
+        <v>582</v>
+      </c>
+      <c r="D48" s="49" t="s">
         <v>583</v>
-      </c>
-      <c r="D48" s="49" t="s">
-        <v>584</v>
       </c>
       <c r="F48" s="49" t="s">
         <v>286</v>
@@ -15042,10 +15717,10 @@
     </row>
     <row r="49" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="49" t="s">
+        <v>584</v>
+      </c>
+      <c r="D49" s="49" t="s">
         <v>585</v>
-      </c>
-      <c r="D49" s="49" t="s">
-        <v>586</v>
       </c>
       <c r="F49" s="49" t="s">
         <v>286</v>
@@ -15360,112 +16035,112 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="48" t="s">
-        <v>541</v>
-      </c>
-      <c r="D65" s="14" t="s">
-        <v>564</v>
-      </c>
-      <c r="F65" s="14" t="s">
+    <row r="65" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="49" t="s">
+        <v>620</v>
+      </c>
+      <c r="D65" s="49" t="s">
+        <v>621</v>
+      </c>
+      <c r="F65" s="49" t="s">
         <v>286</v>
       </c>
-      <c r="G65" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="H65" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="I65" s="14" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="48" t="s">
-        <v>542</v>
-      </c>
-      <c r="D66" s="14" t="s">
-        <v>565</v>
-      </c>
-      <c r="F66" s="14" t="s">
+      <c r="G65" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H65" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I65" s="49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="49" t="s">
+        <v>622</v>
+      </c>
+      <c r="D66" s="49" t="s">
+        <v>623</v>
+      </c>
+      <c r="F66" s="49" t="s">
         <v>286</v>
       </c>
-      <c r="G66" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="H66" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="I66" s="14" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="48" t="s">
-        <v>543</v>
-      </c>
-      <c r="D67" s="14" t="s">
-        <v>566</v>
-      </c>
-      <c r="F67" s="14" t="s">
+      <c r="G66" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H66" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I66" s="49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="49" t="s">
+        <v>624</v>
+      </c>
+      <c r="D67" s="49" t="s">
+        <v>625</v>
+      </c>
+      <c r="F67" s="49" t="s">
         <v>286</v>
       </c>
-      <c r="G67" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="H67" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="I67" s="14" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="48" t="s">
-        <v>544</v>
-      </c>
-      <c r="D68" s="14" t="s">
-        <v>567</v>
-      </c>
-      <c r="F68" s="14" t="s">
+      <c r="G67" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H67" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I67" s="49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="49" t="s">
+        <v>626</v>
+      </c>
+      <c r="D68" s="49" t="s">
+        <v>627</v>
+      </c>
+      <c r="F68" s="49" t="s">
         <v>286</v>
       </c>
-      <c r="G68" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="H68" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="I68" s="14" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="48" t="s">
-        <v>545</v>
-      </c>
-      <c r="D69" s="14" t="s">
-        <v>568</v>
-      </c>
-      <c r="F69" s="14" t="s">
+      <c r="G68" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H68" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I68" s="49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="49" t="s">
+        <v>628</v>
+      </c>
+      <c r="D69" s="49" t="s">
+        <v>629</v>
+      </c>
+      <c r="F69" s="49" t="s">
         <v>286</v>
       </c>
-      <c r="G69" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="H69" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="I69" s="14" t="b">
+      <c r="G69" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H69" s="49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I69" s="49" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="48" t="s">
-        <v>546</v>
+        <v>540</v>
       </c>
       <c r="D70" s="14" t="s">
-        <v>569</v>
+        <v>563</v>
       </c>
       <c r="F70" s="14" t="s">
         <v>286</v>
@@ -15482,10 +16157,10 @@
     </row>
     <row r="71" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="48" t="s">
-        <v>547</v>
+        <v>541</v>
       </c>
       <c r="D71" s="14" t="s">
-        <v>570</v>
+        <v>564</v>
       </c>
       <c r="F71" s="14" t="s">
         <v>286</v>
@@ -15502,10 +16177,10 @@
     </row>
     <row r="72" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="48" t="s">
-        <v>548</v>
+        <v>542</v>
       </c>
       <c r="D72" s="14" t="s">
-        <v>571</v>
+        <v>565</v>
       </c>
       <c r="F72" s="14" t="s">
         <v>286</v>
@@ -15522,10 +16197,10 @@
     </row>
     <row r="73" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="48" t="s">
-        <v>549</v>
+        <v>543</v>
       </c>
       <c r="D73" s="14" t="s">
-        <v>572</v>
+        <v>566</v>
       </c>
       <c r="F73" s="14" t="s">
         <v>286</v>
@@ -15542,10 +16217,10 @@
     </row>
     <row r="74" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="48" t="s">
-        <v>550</v>
+        <v>544</v>
       </c>
       <c r="D74" s="14" t="s">
-        <v>573</v>
+        <v>567</v>
       </c>
       <c r="F74" s="14" t="s">
         <v>286</v>
@@ -15562,10 +16237,10 @@
     </row>
     <row r="75" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="48" t="s">
-        <v>551</v>
+        <v>545</v>
       </c>
       <c r="D75" s="14" t="s">
-        <v>574</v>
+        <v>568</v>
       </c>
       <c r="F75" s="14" t="s">
         <v>286</v>
@@ -15582,10 +16257,10 @@
     </row>
     <row r="76" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="48" t="s">
-        <v>552</v>
+        <v>546</v>
       </c>
       <c r="D76" s="14" t="s">
-        <v>575</v>
+        <v>569</v>
       </c>
       <c r="F76" s="14" t="s">
         <v>286</v>
@@ -15601,11 +16276,11 @@
       </c>
     </row>
     <row r="77" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="14" t="s">
-        <v>553</v>
+      <c r="A77" s="48" t="s">
+        <v>547</v>
       </c>
       <c r="D77" s="14" t="s">
-        <v>576</v>
+        <v>570</v>
       </c>
       <c r="F77" s="14" t="s">
         <v>286</v>
@@ -15621,11 +16296,11 @@
       </c>
     </row>
     <row r="78" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="14" t="s">
-        <v>554</v>
+      <c r="A78" s="48" t="s">
+        <v>548</v>
       </c>
       <c r="D78" s="14" t="s">
-        <v>563</v>
+        <v>571</v>
       </c>
       <c r="F78" s="14" t="s">
         <v>286</v>
@@ -15641,11 +16316,11 @@
       </c>
     </row>
     <row r="79" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="14" t="s">
-        <v>555</v>
+      <c r="A79" s="48" t="s">
+        <v>549</v>
       </c>
       <c r="D79" s="14" t="s">
-        <v>562</v>
+        <v>572</v>
       </c>
       <c r="F79" s="14" t="s">
         <v>286</v>
@@ -15661,11 +16336,11 @@
       </c>
     </row>
     <row r="80" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="14" t="s">
-        <v>556</v>
+      <c r="A80" s="48" t="s">
+        <v>550</v>
       </c>
       <c r="D80" s="14" t="s">
-        <v>561</v>
+        <v>573</v>
       </c>
       <c r="F80" s="14" t="s">
         <v>286</v>
@@ -15681,11 +16356,11 @@
       </c>
     </row>
     <row r="81" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="14" t="s">
-        <v>557</v>
+      <c r="A81" s="48" t="s">
+        <v>551</v>
       </c>
       <c r="D81" s="14" t="s">
-        <v>560</v>
+        <v>574</v>
       </c>
       <c r="F81" s="14" t="s">
         <v>286</v>
@@ -15702,10 +16377,10 @@
     </row>
     <row r="82" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="14" t="s">
-        <v>558</v>
+        <v>552</v>
       </c>
       <c r="D82" s="14" t="s">
-        <v>559</v>
+        <v>575</v>
       </c>
       <c r="F82" s="14" t="s">
         <v>286</v>
@@ -15717,6 +16392,106 @@
         <v>0</v>
       </c>
       <c r="I82" s="14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="14" t="s">
+        <v>553</v>
+      </c>
+      <c r="D83" s="14" t="s">
+        <v>562</v>
+      </c>
+      <c r="F83" s="14" t="s">
+        <v>286</v>
+      </c>
+      <c r="G83" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H83" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I83" s="14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="14" t="s">
+        <v>554</v>
+      </c>
+      <c r="D84" s="14" t="s">
+        <v>561</v>
+      </c>
+      <c r="F84" s="14" t="s">
+        <v>286</v>
+      </c>
+      <c r="G84" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H84" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I84" s="14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="14" t="s">
+        <v>555</v>
+      </c>
+      <c r="D85" s="14" t="s">
+        <v>560</v>
+      </c>
+      <c r="F85" s="14" t="s">
+        <v>286</v>
+      </c>
+      <c r="G85" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H85" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I85" s="14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="14" t="s">
+        <v>556</v>
+      </c>
+      <c r="D86" s="14" t="s">
+        <v>559</v>
+      </c>
+      <c r="F86" s="14" t="s">
+        <v>286</v>
+      </c>
+      <c r="G86" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H86" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I86" s="14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="14" t="s">
+        <v>557</v>
+      </c>
+      <c r="D87" s="14" t="s">
+        <v>558</v>
+      </c>
+      <c r="F87" s="14" t="s">
+        <v>286</v>
+      </c>
+      <c r="G87" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H87" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I87" s="14" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added meta measure for EnergyPlus measures. Airflow measure now runs successfully in workflow, addresses #4. Latest measures.
</commit_message>
<xml_diff>
--- a/projects/res_stock_national_existing.xlsx
+++ b/projects/res_stock_national_existing.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1519" uniqueCount="631">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1519" uniqueCount="633">
   <si>
     <t>type</t>
   </si>
@@ -1927,6 +1927,12 @@
   </si>
   <si>
     <t>1.19.0-rc0</t>
+  </si>
+  <si>
+    <t>CallMetaMeasureEnergyPlus</t>
+  </si>
+  <si>
+    <t>EnergyPlusMeasure</t>
   </si>
 </sst>
 </file>
@@ -14334,13 +14340,13 @@
         <v>617</v>
       </c>
       <c r="C204" s="40" t="s">
-        <v>235</v>
+        <v>631</v>
       </c>
       <c r="D204" s="40" t="s">
-        <v>235</v>
+        <v>631</v>
       </c>
       <c r="E204" s="40" t="s">
-        <v>41</v>
+        <v>632</v>
       </c>
       <c r="F204" s="40"/>
       <c r="G204" s="40"/>

</xml_diff>

<commit_message>
Initial implementation of running upgrades by switching to diagonal sampling algorithm.
</commit_message>
<xml_diff>
--- a/projects/res_stock_national_existing.xlsx
+++ b/projects/res_stock_national_existing.xlsx
@@ -29,12 +29,12 @@
     <definedName name="TrueFalse">Lookups!$C$14:$C$15</definedName>
     <definedName name="Workflow">Lookups!$E$14:$E$15</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1519" uniqueCount="633">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1452" uniqueCount="566">
   <si>
     <t>type</t>
   </si>
@@ -780,111 +780,54 @@
     <t>Probability Distributions File</t>
   </si>
   <si>
-    <t>Location Region Sample Value</t>
-  </si>
-  <si>
-    <t>Location EPW Sample Value</t>
-  </si>
-  <si>
-    <t>Vintage Sample Value</t>
-  </si>
-  <si>
     <t>Set Geometry</t>
   </si>
   <si>
-    <t>Geometry Sample Value</t>
-  </si>
-  <si>
     <t>Set Geometry Garage</t>
   </si>
   <si>
-    <t>Geometry Garage Sample Value</t>
-  </si>
-  <si>
     <t>Set Geometry Stories</t>
   </si>
   <si>
-    <t>Geometry Stories Sample Value</t>
-  </si>
-  <si>
     <t>Set Geometry House Size</t>
   </si>
   <si>
-    <t>Geometry House Size Sample Value</t>
-  </si>
-  <si>
     <t>Set Geometry Foundation Type</t>
   </si>
   <si>
-    <t>Geometry Foundation Type Sample Value</t>
-  </si>
-  <si>
     <t>Set Insulation Slab</t>
   </si>
   <si>
-    <t>Insulation Slab Sample Value</t>
-  </si>
-  <si>
     <t>Set Insulation Unfinished Basement</t>
   </si>
   <si>
-    <t>Insulation Unfinished Basement Sample Value</t>
-  </si>
-  <si>
     <t>Set Insulation Finished Basement</t>
   </si>
   <si>
-    <t>Insulation Finished Basement Sample Value</t>
-  </si>
-  <si>
     <t>Set Insulation Unfinished Attic</t>
   </si>
   <si>
-    <t>Insulation Unfinished Attic Sample Value</t>
-  </si>
-  <si>
     <t>Set Wall Sheathing</t>
   </si>
   <si>
-    <t>Wall Sheathing Sample Value</t>
-  </si>
-  <si>
     <t>Set Exterior Finish</t>
   </si>
   <si>
-    <t>Exterior Finish Sample Value</t>
-  </si>
-  <si>
     <t>Set Roof Material</t>
   </si>
   <si>
-    <t>Roof Material Sample Value</t>
-  </si>
-  <si>
     <t>Set Floor Covering</t>
   </si>
   <si>
-    <t>Floor Covering Sample Value</t>
-  </si>
-  <si>
     <t>Set Orientation</t>
   </si>
   <si>
-    <t>Orientation Sample Value</t>
-  </si>
-  <si>
     <t>Set Door Area</t>
   </si>
   <si>
-    <t>Door Area Sample Value</t>
-  </si>
-  <si>
     <t>Set Doors</t>
   </si>
   <si>
-    <t>Doors Sample Value</t>
-  </si>
-  <si>
     <t>ReportingMeasure</t>
   </si>
   <si>
@@ -900,57 +843,30 @@
     <t>Set Refrigerator</t>
   </si>
   <si>
-    <t>Refrigerator Sample Value</t>
-  </si>
-  <si>
     <t>Set Usage Level</t>
   </si>
   <si>
-    <t>Usage Level Sample Value</t>
-  </si>
-  <si>
     <t>Set Cooking Range</t>
   </si>
   <si>
-    <t>Cooking Range Sample Value</t>
-  </si>
-  <si>
     <t>Set Heating Fuel</t>
   </si>
   <si>
-    <t>Heating Fuel Sample Value</t>
-  </si>
-  <si>
     <t>Set Dishwasher</t>
   </si>
   <si>
-    <t>Dishwasher Sample Value</t>
-  </si>
-  <si>
     <t>Set Clothes Washer</t>
   </si>
   <si>
-    <t>Clothes Washer Sample Value</t>
-  </si>
-  <si>
     <t>Set Clothes Dryer</t>
   </si>
   <si>
-    <t>Clothes Dryer Sample Value</t>
-  </si>
-  <si>
     <t>Set Plug Loads</t>
   </si>
   <si>
-    <t>Plug Loads Sample Value</t>
-  </si>
-  <si>
     <t>Set Water Heater</t>
   </si>
   <si>
-    <t>Water Heater Sample Value</t>
-  </si>
-  <si>
     <t>Location Region</t>
   </si>
   <si>
@@ -1026,36 +942,24 @@
     <t>Set Neighbors</t>
   </si>
   <si>
-    <t>Neighbors Sample Value</t>
-  </si>
-  <si>
     <t>Neighbors</t>
   </si>
   <si>
     <t>Set Eaves</t>
   </si>
   <si>
-    <t>Eaves Sample Value</t>
-  </si>
-  <si>
     <t>Eaves</t>
   </si>
   <si>
     <t>Set Overhangs</t>
   </si>
   <si>
-    <t>Overhangs Sample Value</t>
-  </si>
-  <si>
     <t>Overhangs</t>
   </si>
   <si>
     <t>Set Uninsulated Surfaces</t>
   </si>
   <si>
-    <t>Uninsulated Surfaces Sample Value</t>
-  </si>
-  <si>
     <t>Uninsulated Surfaces</t>
   </si>
   <si>
@@ -1065,15 +969,9 @@
     <t>Set Window Areas</t>
   </si>
   <si>
-    <t>Window Areas Sample Value</t>
-  </si>
-  <si>
     <t>Set Windows</t>
   </si>
   <si>
-    <t>Windows Sample Value</t>
-  </si>
-  <si>
     <t>Windows</t>
   </si>
   <si>
@@ -1083,9 +981,6 @@
     <t>Set Lighting</t>
   </si>
   <si>
-    <t>Lighting Sample Value</t>
-  </si>
-  <si>
     <t>Lighting</t>
   </si>
   <si>
@@ -1107,15 +1002,9 @@
     <t>Set HVAC System Combined</t>
   </si>
   <si>
-    <t>HVAC System Combined Sample Value</t>
-  </si>
-  <si>
     <t>Set HVAC System Is Combined</t>
   </si>
   <si>
-    <t>HVAC System Is Combined Sample Value</t>
-  </si>
-  <si>
     <t>HVAC System Is Combined</t>
   </si>
   <si>
@@ -1134,21 +1023,12 @@
     <t>Set HVAC System Cooling</t>
   </si>
   <si>
-    <t>HVAC System Cooling Sample Value</t>
-  </si>
-  <si>
-    <t>HVAC System Heating Sample Value</t>
-  </si>
-  <si>
     <t>Hot Water Fixtures</t>
   </si>
   <si>
     <t>Set Hot Water Fixtures</t>
   </si>
   <si>
-    <t>Hot Water Fixtures Sample Value</t>
-  </si>
-  <si>
     <t>Clothes Dryer.tsv</t>
   </si>
   <si>
@@ -1551,105 +1431,54 @@
     <t>Set Insulation Wall</t>
   </si>
   <si>
-    <t>Insulation Wall Sample Value</t>
-  </si>
-  <si>
     <t>Set Insulation Interzonal Wall</t>
   </si>
   <si>
-    <t>Insulation Interzonal Wall Sample Value</t>
-  </si>
-  <si>
-    <t>Insulation Crawlspace Sample Value</t>
-  </si>
-  <si>
     <t>Set Insulation Crawlspace</t>
   </si>
   <si>
     <t>Set Insulation Pier Beam</t>
   </si>
   <si>
-    <t>Insulation Pier Beam Sample Value</t>
-  </si>
-  <si>
     <t>Set Insulation Interzonal Floor</t>
   </si>
   <si>
-    <t>Insulation Interzonal Floor Sample Value</t>
-  </si>
-  <si>
     <t>Set Thermal Mass Floor</t>
   </si>
   <si>
-    <t>Thermal Mass Floor Sample Value</t>
-  </si>
-  <si>
     <t>Set Thermal Mass Exterior Wall</t>
   </si>
   <si>
-    <t>Thermal Mass Exterior Wall Sample Value</t>
-  </si>
-  <si>
     <t>Set Thermal Mass Partition Wall</t>
   </si>
   <si>
-    <t>Thermal Mass Partition Wall Sample Value</t>
-  </si>
-  <si>
     <t>Set Thermal Mass Ceiling</t>
   </si>
   <si>
-    <t>Thermal Mass Ceiling Sample Value</t>
-  </si>
-  <si>
-    <t>Misc Extra Refrigerator Sample Value</t>
-  </si>
-  <si>
     <t>Set Misc Extra Refrigerator</t>
   </si>
   <si>
     <t>Set Misc Freezer</t>
   </si>
   <si>
-    <t>Misc Freezer Sample Value</t>
-  </si>
-  <si>
     <t>Set Misc Gas Fireplace</t>
   </si>
   <si>
-    <t>Misc Gas Fireplace Sample Value</t>
-  </si>
-  <si>
     <t>Set Misc Gas Grill</t>
   </si>
   <si>
-    <t>Misc Gas Grill Sample Value</t>
-  </si>
-  <si>
     <t>Set Misc Gas Lighting</t>
   </si>
   <si>
-    <t>Misc Gas Lighting Sample Value</t>
-  </si>
-  <si>
     <t>Set Misc Hot Tub Spa</t>
   </si>
   <si>
-    <t>Misc Hot Tub Spa Sample Value</t>
-  </si>
-  <si>
     <t>Set Misc Pool</t>
   </si>
   <si>
-    <t>Misc Pool Sample Value</t>
-  </si>
-  <si>
     <t>Set Misc Well Pump</t>
   </si>
   <si>
-    <t>Misc Well Pump Sample Value</t>
-  </si>
-  <si>
     <t>Standard Reports</t>
   </si>
   <si>
@@ -1770,12 +1599,6 @@
     <t>Set Heating Setpoint</t>
   </si>
   <si>
-    <t>Heating Setpoint Sample Value</t>
-  </si>
-  <si>
-    <t>Cooling Setpoint Sample Value</t>
-  </si>
-  <si>
     <t>Cooling Setpoint.tsv</t>
   </si>
   <si>
@@ -1812,18 +1635,12 @@
     <t>Roof Sheathing.tsv</t>
   </si>
   <si>
-    <t>Roof Sheathing Sample Value</t>
-  </si>
-  <si>
     <t>Set Floor Sheathing</t>
   </si>
   <si>
     <t>Floor Sheathing.tsv</t>
   </si>
   <si>
-    <t>Floor Sheathing Sample Value</t>
-  </si>
-  <si>
     <t>Roof Sheathing</t>
   </si>
   <si>
@@ -1839,9 +1656,6 @@
     <t>Set Thermal Mass Furniture</t>
   </si>
   <si>
-    <t>Thermal Mass Furniture Sample Value</t>
-  </si>
-  <si>
     <t>Thermal Mass Furniture.tsv</t>
   </si>
   <si>
@@ -1857,43 +1671,28 @@
     <t>Ducts.tsv</t>
   </si>
   <si>
-    <t>Ducts Sample Value</t>
-  </si>
-  <si>
     <t>Set Infiltration</t>
   </si>
   <si>
     <t>Infiltration.tsv</t>
   </si>
   <si>
-    <t>Infiltration Sample Value</t>
-  </si>
-  <si>
     <t>Set Natural Ventilation</t>
   </si>
   <si>
     <t>Natural Ventilation.tsv</t>
   </si>
   <si>
-    <t>Natural Ventilation Sample Value</t>
-  </si>
-  <si>
     <t>Set Mechanical Ventilation</t>
   </si>
   <si>
     <t>Mechanical Ventilation.tsv</t>
   </si>
   <si>
-    <t>Mechanical Ventilation Sample Value</t>
-  </si>
-  <si>
     <t>Set Airflow</t>
   </si>
   <si>
     <t>Airflow.tsv</t>
-  </si>
-  <si>
-    <t>Airflow Sample Value</t>
   </si>
   <si>
     <t>Ducts</t>
@@ -5524,7 +5323,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5583,7 +5384,7 @@
         <v>75</v>
       </c>
       <c r="B5" s="44" t="s">
-        <v>630</v>
+        <v>563</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>155</v>
@@ -5694,7 +5495,7 @@
         <v>36</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>347</v>
+        <v>313</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>77</v>
@@ -5716,7 +5517,7 @@
         <v>23</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>586</v>
+        <v>527</v>
       </c>
       <c r="F15" s="22" t="s">
         <v>156</v>
@@ -6029,7 +5830,7 @@
         <v>26</v>
       </c>
       <c r="B38" s="25" t="s">
-        <v>587</v>
+        <v>528</v>
       </c>
     </row>
     <row r="40" spans="1:6" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -6085,13 +5886,13 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="47" t="s">
-        <v>353</v>
+        <v>318</v>
       </c>
       <c r="B44" s="17" t="s">
-        <v>354</v>
+        <v>319</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>355</v>
+        <v>320</v>
       </c>
     </row>
     <row r="46" spans="1:6" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -6161,7 +5962,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z209"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6343,7 +6146,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="40" t="s">
-        <v>589</v>
+        <v>530</v>
       </c>
       <c r="C4" s="40" t="s">
         <v>240</v>
@@ -6392,7 +6195,7 @@
       </c>
       <c r="H5" s="10"/>
       <c r="I5" s="10" t="s">
-        <v>588</v>
+        <v>529</v>
       </c>
       <c r="J5" s="10"/>
       <c r="K5" s="10"/>
@@ -6466,7 +6269,7 @@
       </c>
       <c r="H7" s="10"/>
       <c r="I7" s="10" t="s">
-        <v>401</v>
+        <v>361</v>
       </c>
       <c r="J7" s="10"/>
       <c r="K7" s="10"/>
@@ -6492,8 +6295,9 @@
         <v>21</v>
       </c>
       <c r="C8" s="41"/>
-      <c r="D8" s="41" t="s">
-        <v>248</v>
+      <c r="D8" s="41" t="str">
+        <f>MID(B6,5,1000) &amp; " Sample Value"</f>
+        <v>Location Region Sample Value</v>
       </c>
       <c r="E8" s="41" t="s">
         <v>237</v>
@@ -6586,7 +6390,7 @@
       </c>
       <c r="H10" s="10"/>
       <c r="I10" s="10" t="s">
-        <v>400</v>
+        <v>360</v>
       </c>
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
@@ -6612,8 +6416,9 @@
         <v>21</v>
       </c>
       <c r="C11" s="41"/>
-      <c r="D11" s="41" t="s">
-        <v>249</v>
+      <c r="D11" s="41" t="str">
+        <f>MID(B9,5,1000) &amp; " Sample Value"</f>
+        <v>Location EPW Sample Value</v>
       </c>
       <c r="E11" s="41" t="s">
         <v>237</v>
@@ -6706,7 +6511,7 @@
       </c>
       <c r="H13" s="10"/>
       <c r="I13" s="10" t="s">
-        <v>422</v>
+        <v>382</v>
       </c>
       <c r="J13" s="10"/>
       <c r="K13" s="10"/>
@@ -6732,8 +6537,9 @@
         <v>21</v>
       </c>
       <c r="C14" s="41"/>
-      <c r="D14" s="41" t="s">
-        <v>250</v>
+      <c r="D14" s="41" t="str">
+        <f>MID(B12,5,1000) &amp; " Sample Value"</f>
+        <v>Vintage Sample Value</v>
       </c>
       <c r="E14" s="41" t="s">
         <v>237</v>
@@ -6777,7 +6583,7 @@
         <v>1</v>
       </c>
       <c r="B15" s="40" t="s">
-        <v>293</v>
+        <v>271</v>
       </c>
       <c r="C15" s="40" t="s">
         <v>235</v>
@@ -6826,7 +6632,7 @@
       </c>
       <c r="H16" s="10"/>
       <c r="I16" s="10" t="s">
-        <v>385</v>
+        <v>345</v>
       </c>
       <c r="J16" s="10"/>
       <c r="K16" s="10"/>
@@ -6852,8 +6658,9 @@
         <v>21</v>
       </c>
       <c r="C17" s="41"/>
-      <c r="D17" s="41" t="s">
-        <v>294</v>
+      <c r="D17" s="41" t="str">
+        <f>MID(B15,5,1000) &amp; " Sample Value"</f>
+        <v>Heating Fuel Sample Value</v>
       </c>
       <c r="E17" s="41" t="s">
         <v>237</v>
@@ -6897,7 +6704,7 @@
         <v>1</v>
       </c>
       <c r="B18" s="40" t="s">
-        <v>289</v>
+        <v>269</v>
       </c>
       <c r="C18" s="40" t="s">
         <v>235</v>
@@ -6946,7 +6753,7 @@
       </c>
       <c r="H19" s="10"/>
       <c r="I19" s="10" t="s">
-        <v>421</v>
+        <v>381</v>
       </c>
       <c r="J19" s="10"/>
       <c r="K19" s="10"/>
@@ -6972,8 +6779,9 @@
         <v>21</v>
       </c>
       <c r="C20" s="41"/>
-      <c r="D20" s="41" t="s">
-        <v>290</v>
+      <c r="D20" s="41" t="str">
+        <f>MID(B18,5,1000) &amp; " Sample Value"</f>
+        <v>Usage Level Sample Value</v>
       </c>
       <c r="E20" s="41" t="s">
         <v>237</v>
@@ -7017,7 +6825,7 @@
         <v>1</v>
       </c>
       <c r="B21" s="40" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="C21" s="40" t="s">
         <v>235</v>
@@ -7066,7 +6874,7 @@
       </c>
       <c r="H22" s="10"/>
       <c r="I22" s="10" t="s">
-        <v>380</v>
+        <v>340</v>
       </c>
       <c r="J22" s="10"/>
       <c r="K22" s="10"/>
@@ -7092,8 +6900,9 @@
         <v>21</v>
       </c>
       <c r="C23" s="41"/>
-      <c r="D23" s="41" t="s">
-        <v>260</v>
+      <c r="D23" s="41" t="str">
+        <f>MID(B21,5,1000) &amp; " Sample Value"</f>
+        <v>Geometry Foundation Type Sample Value</v>
       </c>
       <c r="E23" s="41" t="s">
         <v>237</v>
@@ -7137,7 +6946,7 @@
         <v>1</v>
       </c>
       <c r="B24" s="40" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="C24" s="40" t="s">
         <v>235</v>
@@ -7186,7 +6995,7 @@
       </c>
       <c r="H25" s="10"/>
       <c r="I25" s="10" t="s">
-        <v>382</v>
+        <v>342</v>
       </c>
       <c r="J25" s="10"/>
       <c r="K25" s="10"/>
@@ -7212,8 +7021,9 @@
         <v>21</v>
       </c>
       <c r="C26" s="41"/>
-      <c r="D26" s="41" t="s">
-        <v>258</v>
+      <c r="D26" s="41" t="str">
+        <f>MID(B24,5,1000) &amp; " Sample Value"</f>
+        <v>Geometry House Size Sample Value</v>
       </c>
       <c r="E26" s="41" t="s">
         <v>237</v>
@@ -7257,7 +7067,7 @@
         <v>1</v>
       </c>
       <c r="B27" s="40" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="C27" s="40" t="s">
         <v>235</v>
@@ -7306,7 +7116,7 @@
       </c>
       <c r="H28" s="10"/>
       <c r="I28" s="10" t="s">
-        <v>383</v>
+        <v>343</v>
       </c>
       <c r="J28" s="10"/>
       <c r="K28" s="10"/>
@@ -7332,8 +7142,9 @@
         <v>21</v>
       </c>
       <c r="C29" s="41"/>
-      <c r="D29" s="41" t="s">
-        <v>256</v>
+      <c r="D29" s="41" t="str">
+        <f>MID(B27,5,1000) &amp; " Sample Value"</f>
+        <v>Geometry Stories Sample Value</v>
       </c>
       <c r="E29" s="41" t="s">
         <v>237</v>
@@ -7377,7 +7188,7 @@
         <v>1</v>
       </c>
       <c r="B30" s="40" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="C30" s="40" t="s">
         <v>235</v>
@@ -7426,7 +7237,7 @@
       </c>
       <c r="H31" s="10"/>
       <c r="I31" s="10" t="s">
-        <v>381</v>
+        <v>341</v>
       </c>
       <c r="J31" s="10"/>
       <c r="K31" s="10"/>
@@ -7452,8 +7263,9 @@
         <v>21</v>
       </c>
       <c r="C32" s="41"/>
-      <c r="D32" s="41" t="s">
-        <v>254</v>
+      <c r="D32" s="41" t="str">
+        <f>MID(B30,5,1000) &amp; " Sample Value"</f>
+        <v>Geometry Garage Sample Value</v>
       </c>
       <c r="E32" s="41" t="s">
         <v>237</v>
@@ -7497,7 +7309,7 @@
         <v>1</v>
       </c>
       <c r="B33" s="40" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C33" s="40" t="s">
         <v>235</v>
@@ -7546,7 +7358,7 @@
       </c>
       <c r="H34" s="10"/>
       <c r="I34" s="10" t="s">
-        <v>384</v>
+        <v>344</v>
       </c>
       <c r="J34" s="10"/>
       <c r="K34" s="10"/>
@@ -7572,8 +7384,9 @@
         <v>21</v>
       </c>
       <c r="C35" s="41"/>
-      <c r="D35" s="41" t="s">
-        <v>252</v>
+      <c r="D35" s="41" t="str">
+        <f>MID(B33,5,1000) &amp; " Sample Value"</f>
+        <v>Geometry Sample Value</v>
       </c>
       <c r="E35" s="41" t="s">
         <v>237</v>
@@ -7617,7 +7430,7 @@
         <v>1</v>
       </c>
       <c r="B36" s="40" t="s">
-        <v>277</v>
+        <v>261</v>
       </c>
       <c r="C36" s="40" t="s">
         <v>235</v>
@@ -7666,7 +7479,7 @@
       </c>
       <c r="H37" s="10"/>
       <c r="I37" s="10" t="s">
-        <v>411</v>
+        <v>371</v>
       </c>
       <c r="J37" s="10"/>
       <c r="K37" s="10"/>
@@ -7692,8 +7505,9 @@
         <v>21</v>
       </c>
       <c r="C38" s="41"/>
-      <c r="D38" s="41" t="s">
-        <v>278</v>
+      <c r="D38" s="41" t="str">
+        <f>MID(B36,5,1000) &amp; " Sample Value"</f>
+        <v>Orientation Sample Value</v>
       </c>
       <c r="E38" s="41" t="s">
         <v>237</v>
@@ -7737,7 +7551,7 @@
         <v>1</v>
       </c>
       <c r="B39" s="40" t="s">
-        <v>332</v>
+        <v>303</v>
       </c>
       <c r="C39" s="40" t="s">
         <v>235</v>
@@ -7786,7 +7600,7 @@
       </c>
       <c r="H40" s="10"/>
       <c r="I40" s="10" t="s">
-        <v>377</v>
+        <v>337</v>
       </c>
       <c r="J40" s="10"/>
       <c r="K40" s="10"/>
@@ -7812,8 +7626,9 @@
         <v>21</v>
       </c>
       <c r="C41" s="41"/>
-      <c r="D41" s="41" t="s">
-        <v>333</v>
+      <c r="D41" s="41" t="str">
+        <f>MID(B39,5,1000) &amp; " Sample Value"</f>
+        <v>Eaves Sample Value</v>
       </c>
       <c r="E41" s="41" t="s">
         <v>237</v>
@@ -7857,7 +7672,7 @@
         <v>1</v>
       </c>
       <c r="B42" s="40" t="s">
-        <v>335</v>
+        <v>305</v>
       </c>
       <c r="C42" s="40" t="s">
         <v>235</v>
@@ -7906,7 +7721,7 @@
       </c>
       <c r="H43" s="10"/>
       <c r="I43" s="10" t="s">
-        <v>412</v>
+        <v>372</v>
       </c>
       <c r="J43" s="10"/>
       <c r="K43" s="10"/>
@@ -7932,8 +7747,9 @@
         <v>21</v>
       </c>
       <c r="C44" s="41"/>
-      <c r="D44" s="41" t="s">
-        <v>336</v>
+      <c r="D44" s="41" t="str">
+        <f>MID(B42,5,1000) &amp; " Sample Value"</f>
+        <v>Overhangs Sample Value</v>
       </c>
       <c r="E44" s="41" t="s">
         <v>237</v>
@@ -7977,7 +7793,7 @@
         <v>1</v>
       </c>
       <c r="B45" s="40" t="s">
-        <v>279</v>
+        <v>262</v>
       </c>
       <c r="C45" s="40" t="s">
         <v>235</v>
@@ -8026,7 +7842,7 @@
       </c>
       <c r="H46" s="10"/>
       <c r="I46" s="10" t="s">
-        <v>375</v>
+        <v>335</v>
       </c>
       <c r="J46" s="10"/>
       <c r="K46" s="10"/>
@@ -8052,8 +7868,9 @@
         <v>21</v>
       </c>
       <c r="C47" s="41"/>
-      <c r="D47" s="41" t="s">
-        <v>280</v>
+      <c r="D47" s="41" t="str">
+        <f>MID(B45,5,1000) &amp; " Sample Value"</f>
+        <v>Door Area Sample Value</v>
       </c>
       <c r="E47" s="41" t="s">
         <v>237</v>
@@ -8097,7 +7914,7 @@
         <v>1</v>
       </c>
       <c r="B48" s="40" t="s">
-        <v>342</v>
+        <v>310</v>
       </c>
       <c r="C48" s="40" t="s">
         <v>235</v>
@@ -8146,7 +7963,7 @@
       </c>
       <c r="H49" s="10"/>
       <c r="I49" s="10" t="s">
-        <v>425</v>
+        <v>385</v>
       </c>
       <c r="J49" s="10"/>
       <c r="K49" s="10"/>
@@ -8172,8 +7989,9 @@
         <v>21</v>
       </c>
       <c r="C50" s="41"/>
-      <c r="D50" s="41" t="s">
-        <v>343</v>
+      <c r="D50" s="41" t="str">
+        <f>MID(B48,5,1000) &amp; " Sample Value"</f>
+        <v>Window Areas Sample Value</v>
       </c>
       <c r="E50" s="41" t="s">
         <v>237</v>
@@ -8217,7 +8035,7 @@
         <v>1</v>
       </c>
       <c r="B51" s="40" t="s">
-        <v>329</v>
+        <v>301</v>
       </c>
       <c r="C51" s="40" t="s">
         <v>235</v>
@@ -8266,7 +8084,7 @@
       </c>
       <c r="H52" s="10"/>
       <c r="I52" s="10" t="s">
-        <v>410</v>
+        <v>370</v>
       </c>
       <c r="J52" s="10"/>
       <c r="K52" s="10"/>
@@ -8292,8 +8110,9 @@
         <v>21</v>
       </c>
       <c r="C53" s="41"/>
-      <c r="D53" s="41" t="s">
-        <v>330</v>
+      <c r="D53" s="41" t="str">
+        <f>MID(B51,5,1000) &amp; " Sample Value"</f>
+        <v>Neighbors Sample Value</v>
       </c>
       <c r="E53" s="41" t="s">
         <v>237</v>
@@ -8337,7 +8156,7 @@
         <v>1</v>
       </c>
       <c r="B54" s="40" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
       <c r="C54" s="40" t="s">
         <v>235</v>
@@ -8386,7 +8205,7 @@
       </c>
       <c r="H55" s="10"/>
       <c r="I55" s="10" t="s">
-        <v>396</v>
+        <v>356</v>
       </c>
       <c r="J55" s="10"/>
       <c r="K55" s="10"/>
@@ -8412,8 +8231,9 @@
         <v>21</v>
       </c>
       <c r="C56" s="41"/>
-      <c r="D56" s="41" t="s">
-        <v>268</v>
+      <c r="D56" s="41" t="str">
+        <f>MID(B54,5,1000) &amp; " Sample Value"</f>
+        <v>Insulation Unfinished Attic Sample Value</v>
       </c>
       <c r="E56" s="41" t="s">
         <v>237</v>
@@ -8457,7 +8277,7 @@
         <v>1</v>
       </c>
       <c r="B57" s="40" t="s">
-        <v>504</v>
+        <v>464</v>
       </c>
       <c r="C57" s="40" t="s">
         <v>235</v>
@@ -8506,7 +8326,7 @@
       </c>
       <c r="H58" s="10"/>
       <c r="I58" s="10" t="s">
-        <v>398</v>
+        <v>358</v>
       </c>
       <c r="J58" s="10"/>
       <c r="K58" s="10"/>
@@ -8532,8 +8352,9 @@
         <v>21</v>
       </c>
       <c r="C59" s="41"/>
-      <c r="D59" s="41" t="s">
-        <v>505</v>
+      <c r="D59" s="41" t="str">
+        <f>MID(B57,5,1000) &amp; " Sample Value"</f>
+        <v>Insulation Wall Sample Value</v>
       </c>
       <c r="E59" s="41" t="s">
         <v>237</v>
@@ -8577,7 +8398,7 @@
         <v>1</v>
       </c>
       <c r="B60" s="40" t="s">
-        <v>506</v>
+        <v>465</v>
       </c>
       <c r="C60" s="40" t="s">
         <v>235</v>
@@ -8626,7 +8447,7 @@
       </c>
       <c r="H61" s="10"/>
       <c r="I61" s="10" t="s">
-        <v>394</v>
+        <v>354</v>
       </c>
       <c r="J61" s="10"/>
       <c r="K61" s="10"/>
@@ -8652,8 +8473,9 @@
         <v>21</v>
       </c>
       <c r="C62" s="41"/>
-      <c r="D62" s="41" t="s">
-        <v>507</v>
+      <c r="D62" s="41" t="str">
+        <f>MID(B60,5,1000) &amp; " Sample Value"</f>
+        <v>Insulation Interzonal Wall Sample Value</v>
       </c>
       <c r="E62" s="41" t="s">
         <v>237</v>
@@ -8697,7 +8519,7 @@
         <v>1</v>
       </c>
       <c r="B63" s="40" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="C63" s="40" t="s">
         <v>235</v>
@@ -8746,7 +8568,7 @@
       </c>
       <c r="H64" s="10"/>
       <c r="I64" s="10" t="s">
-        <v>395</v>
+        <v>355</v>
       </c>
       <c r="J64" s="10"/>
       <c r="K64" s="10"/>
@@ -8772,8 +8594,9 @@
         <v>21</v>
       </c>
       <c r="C65" s="41"/>
-      <c r="D65" s="41" t="s">
-        <v>262</v>
+      <c r="D65" s="41" t="str">
+        <f>MID(B63,5,1000) &amp; " Sample Value"</f>
+        <v>Insulation Slab Sample Value</v>
       </c>
       <c r="E65" s="41" t="s">
         <v>237</v>
@@ -8817,7 +8640,7 @@
         <v>1</v>
       </c>
       <c r="B66" s="40" t="s">
-        <v>509</v>
+        <v>466</v>
       </c>
       <c r="C66" s="40" t="s">
         <v>235</v>
@@ -8866,7 +8689,7 @@
       </c>
       <c r="H67" s="10"/>
       <c r="I67" s="10" t="s">
-        <v>391</v>
+        <v>351</v>
       </c>
       <c r="J67" s="10"/>
       <c r="K67" s="10"/>
@@ -8892,8 +8715,9 @@
         <v>21</v>
       </c>
       <c r="C68" s="41"/>
-      <c r="D68" s="41" t="s">
-        <v>508</v>
+      <c r="D68" s="41" t="str">
+        <f>MID(B66,5,1000) &amp; " Sample Value"</f>
+        <v>Insulation Crawlspace Sample Value</v>
       </c>
       <c r="E68" s="41" t="s">
         <v>237</v>
@@ -8937,7 +8761,7 @@
         <v>1</v>
       </c>
       <c r="B69" s="40" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
       <c r="C69" s="40" t="s">
         <v>235</v>
@@ -8986,7 +8810,7 @@
       </c>
       <c r="H70" s="10"/>
       <c r="I70" s="10" t="s">
-        <v>397</v>
+        <v>357</v>
       </c>
       <c r="J70" s="10"/>
       <c r="K70" s="10"/>
@@ -9012,8 +8836,9 @@
         <v>21</v>
       </c>
       <c r="C71" s="41"/>
-      <c r="D71" s="41" t="s">
-        <v>264</v>
+      <c r="D71" s="41" t="str">
+        <f>MID(B69,5,1000) &amp; " Sample Value"</f>
+        <v>Insulation Unfinished Basement Sample Value</v>
       </c>
       <c r="E71" s="41" t="s">
         <v>237</v>
@@ -9057,7 +8882,7 @@
         <v>1</v>
       </c>
       <c r="B72" s="40" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="C72" s="40" t="s">
         <v>235</v>
@@ -9106,7 +8931,7 @@
       </c>
       <c r="H73" s="10"/>
       <c r="I73" s="10" t="s">
-        <v>392</v>
+        <v>352</v>
       </c>
       <c r="J73" s="10"/>
       <c r="K73" s="10"/>
@@ -9132,8 +8957,9 @@
         <v>21</v>
       </c>
       <c r="C74" s="41"/>
-      <c r="D74" s="41" t="s">
-        <v>266</v>
+      <c r="D74" s="41" t="str">
+        <f>MID(B72,5,1000) &amp; " Sample Value"</f>
+        <v>Insulation Finished Basement Sample Value</v>
       </c>
       <c r="E74" s="41" t="s">
         <v>237</v>
@@ -9177,7 +9003,7 @@
         <v>0</v>
       </c>
       <c r="B75" s="40" t="s">
-        <v>510</v>
+        <v>467</v>
       </c>
       <c r="C75" s="40" t="s">
         <v>235</v>
@@ -9226,7 +9052,7 @@
       </c>
       <c r="H76" s="10"/>
       <c r="I76" s="10" t="s">
-        <v>427</v>
+        <v>387</v>
       </c>
       <c r="J76" s="10"/>
       <c r="K76" s="10"/>
@@ -9252,8 +9078,9 @@
         <v>21</v>
       </c>
       <c r="C77" s="41"/>
-      <c r="D77" s="41" t="s">
-        <v>511</v>
+      <c r="D77" s="41" t="str">
+        <f>MID(B75,5,1000) &amp; " Sample Value"</f>
+        <v>Insulation Pier Beam Sample Value</v>
       </c>
       <c r="E77" s="41" t="s">
         <v>237</v>
@@ -9297,7 +9124,7 @@
         <v>1</v>
       </c>
       <c r="B78" s="40" t="s">
-        <v>512</v>
+        <v>468</v>
       </c>
       <c r="C78" s="40" t="s">
         <v>235</v>
@@ -9346,7 +9173,7 @@
       </c>
       <c r="H79" s="10"/>
       <c r="I79" s="10" t="s">
-        <v>393</v>
+        <v>353</v>
       </c>
       <c r="J79" s="10"/>
       <c r="K79" s="10"/>
@@ -9372,8 +9199,9 @@
         <v>21</v>
       </c>
       <c r="C80" s="41"/>
-      <c r="D80" s="41" t="s">
-        <v>513</v>
+      <c r="D80" s="41" t="str">
+        <f>MID(B78,5,1000) &amp; " Sample Value"</f>
+        <v>Insulation Interzonal Floor Sample Value</v>
       </c>
       <c r="E80" s="41" t="s">
         <v>237</v>
@@ -9417,7 +9245,7 @@
         <v>1</v>
       </c>
       <c r="B81" s="40" t="s">
-        <v>338</v>
+        <v>307</v>
       </c>
       <c r="C81" s="40" t="s">
         <v>235</v>
@@ -9466,7 +9294,7 @@
       </c>
       <c r="H82" s="10"/>
       <c r="I82" s="10" t="s">
-        <v>420</v>
+        <v>380</v>
       </c>
       <c r="J82" s="10"/>
       <c r="K82" s="10"/>
@@ -9492,8 +9320,9 @@
         <v>21</v>
       </c>
       <c r="C83" s="41"/>
-      <c r="D83" s="41" t="s">
-        <v>339</v>
+      <c r="D83" s="41" t="str">
+        <f>MID(B81,5,1000) &amp; " Sample Value"</f>
+        <v>Uninsulated Surfaces Sample Value</v>
       </c>
       <c r="E83" s="41" t="s">
         <v>237</v>
@@ -9537,7 +9366,7 @@
         <v>1</v>
       </c>
       <c r="B84" s="40" t="s">
-        <v>590</v>
+        <v>531</v>
       </c>
       <c r="C84" s="40" t="s">
         <v>235</v>
@@ -9586,7 +9415,7 @@
       </c>
       <c r="H85" s="10"/>
       <c r="I85" s="10" t="s">
-        <v>591</v>
+        <v>532</v>
       </c>
       <c r="J85" s="10"/>
       <c r="K85" s="10"/>
@@ -9612,8 +9441,9 @@
         <v>21</v>
       </c>
       <c r="C86" s="41"/>
-      <c r="D86" s="41" t="s">
-        <v>592</v>
+      <c r="D86" s="41" t="str">
+        <f>MID(B84,5,1000) &amp; " Sample Value"</f>
+        <v>Roof Sheathing Sample Value</v>
       </c>
       <c r="E86" s="41" t="s">
         <v>237</v>
@@ -9657,7 +9487,7 @@
         <v>1</v>
       </c>
       <c r="B87" s="40" t="s">
-        <v>269</v>
+        <v>257</v>
       </c>
       <c r="C87" s="40" t="s">
         <v>235</v>
@@ -9706,7 +9536,7 @@
       </c>
       <c r="H88" s="10"/>
       <c r="I88" s="10" t="s">
-        <v>423</v>
+        <v>383</v>
       </c>
       <c r="J88" s="10"/>
       <c r="K88" s="10"/>
@@ -9732,8 +9562,9 @@
         <v>21</v>
       </c>
       <c r="C89" s="41"/>
-      <c r="D89" s="41" t="s">
-        <v>270</v>
+      <c r="D89" s="41" t="str">
+        <f>MID(B87,5,1000) &amp; " Sample Value"</f>
+        <v>Wall Sheathing Sample Value</v>
       </c>
       <c r="E89" s="41" t="s">
         <v>237</v>
@@ -9777,7 +9608,7 @@
         <v>1</v>
       </c>
       <c r="B90" s="40" t="s">
-        <v>593</v>
+        <v>533</v>
       </c>
       <c r="C90" s="40" t="s">
         <v>235</v>
@@ -9826,7 +9657,7 @@
       </c>
       <c r="H91" s="10"/>
       <c r="I91" s="10" t="s">
-        <v>594</v>
+        <v>534</v>
       </c>
       <c r="J91" s="10"/>
       <c r="K91" s="10"/>
@@ -9852,8 +9683,9 @@
         <v>21</v>
       </c>
       <c r="C92" s="41"/>
-      <c r="D92" s="41" t="s">
-        <v>595</v>
+      <c r="D92" s="41" t="str">
+        <f>MID(B90,5,1000) &amp; " Sample Value"</f>
+        <v>Floor Sheathing Sample Value</v>
       </c>
       <c r="E92" s="41" t="s">
         <v>237</v>
@@ -9897,7 +9729,7 @@
         <v>1</v>
       </c>
       <c r="B93" s="40" t="s">
-        <v>271</v>
+        <v>258</v>
       </c>
       <c r="C93" s="40" t="s">
         <v>235</v>
@@ -9946,7 +9778,7 @@
       </c>
       <c r="H94" s="10"/>
       <c r="I94" s="10" t="s">
-        <v>378</v>
+        <v>338</v>
       </c>
       <c r="J94" s="10"/>
       <c r="K94" s="10"/>
@@ -9972,8 +9804,9 @@
         <v>21</v>
       </c>
       <c r="C95" s="41"/>
-      <c r="D95" s="41" t="s">
-        <v>272</v>
+      <c r="D95" s="41" t="str">
+        <f>MID(B93,5,1000) &amp; " Sample Value"</f>
+        <v>Exterior Finish Sample Value</v>
       </c>
       <c r="E95" s="41" t="s">
         <v>237</v>
@@ -10017,7 +9850,7 @@
         <v>1</v>
       </c>
       <c r="B96" s="40" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="C96" s="40" t="s">
         <v>235</v>
@@ -10066,7 +9899,7 @@
       </c>
       <c r="H97" s="10"/>
       <c r="I97" s="10" t="s">
-        <v>415</v>
+        <v>375</v>
       </c>
       <c r="J97" s="10"/>
       <c r="K97" s="10"/>
@@ -10092,8 +9925,9 @@
         <v>21</v>
       </c>
       <c r="C98" s="41"/>
-      <c r="D98" s="41" t="s">
-        <v>274</v>
+      <c r="D98" s="41" t="str">
+        <f>MID(B96,5,1000) &amp; " Sample Value"</f>
+        <v>Roof Material Sample Value</v>
       </c>
       <c r="E98" s="41" t="s">
         <v>237</v>
@@ -10137,7 +9971,7 @@
         <v>1</v>
       </c>
       <c r="B99" s="40" t="s">
-        <v>275</v>
+        <v>260</v>
       </c>
       <c r="C99" s="40" t="s">
         <v>235</v>
@@ -10186,7 +10020,7 @@
       </c>
       <c r="H100" s="10"/>
       <c r="I100" s="10" t="s">
-        <v>379</v>
+        <v>339</v>
       </c>
       <c r="J100" s="10"/>
       <c r="K100" s="10"/>
@@ -10212,8 +10046,9 @@
         <v>21</v>
       </c>
       <c r="C101" s="41"/>
-      <c r="D101" s="41" t="s">
-        <v>276</v>
+      <c r="D101" s="41" t="str">
+        <f>MID(B99,5,1000) &amp; " Sample Value"</f>
+        <v>Floor Covering Sample Value</v>
       </c>
       <c r="E101" s="41" t="s">
         <v>237</v>
@@ -10257,7 +10092,7 @@
         <v>1</v>
       </c>
       <c r="B102" s="40" t="s">
-        <v>514</v>
+        <v>469</v>
       </c>
       <c r="C102" s="40" t="s">
         <v>235</v>
@@ -10306,7 +10141,7 @@
       </c>
       <c r="H103" s="10"/>
       <c r="I103" s="10" t="s">
-        <v>418</v>
+        <v>378</v>
       </c>
       <c r="J103" s="10"/>
       <c r="K103" s="10"/>
@@ -10332,8 +10167,9 @@
         <v>21</v>
       </c>
       <c r="C104" s="41"/>
-      <c r="D104" s="41" t="s">
-        <v>515</v>
+      <c r="D104" s="41" t="str">
+        <f>MID(B102,5,1000) &amp; " Sample Value"</f>
+        <v>Thermal Mass Floor Sample Value</v>
       </c>
       <c r="E104" s="41" t="s">
         <v>237</v>
@@ -10377,7 +10213,7 @@
         <v>1</v>
       </c>
       <c r="B105" s="40" t="s">
-        <v>516</v>
+        <v>470</v>
       </c>
       <c r="C105" s="40" t="s">
         <v>235</v>
@@ -10426,7 +10262,7 @@
       </c>
       <c r="H106" s="10"/>
       <c r="I106" s="10" t="s">
-        <v>417</v>
+        <v>377</v>
       </c>
       <c r="J106" s="10"/>
       <c r="K106" s="10"/>
@@ -10452,8 +10288,9 @@
         <v>21</v>
       </c>
       <c r="C107" s="41"/>
-      <c r="D107" s="41" t="s">
-        <v>517</v>
+      <c r="D107" s="41" t="str">
+        <f>MID(B105,5,1000) &amp; " Sample Value"</f>
+        <v>Thermal Mass Exterior Wall Sample Value</v>
       </c>
       <c r="E107" s="41" t="s">
         <v>237</v>
@@ -10497,7 +10334,7 @@
         <v>1</v>
       </c>
       <c r="B108" s="40" t="s">
-        <v>518</v>
+        <v>471</v>
       </c>
       <c r="C108" s="40" t="s">
         <v>235</v>
@@ -10546,7 +10383,7 @@
       </c>
       <c r="H109" s="10"/>
       <c r="I109" s="10" t="s">
-        <v>419</v>
+        <v>379</v>
       </c>
       <c r="J109" s="10"/>
       <c r="K109" s="10"/>
@@ -10572,8 +10409,9 @@
         <v>21</v>
       </c>
       <c r="C110" s="41"/>
-      <c r="D110" s="41" t="s">
-        <v>519</v>
+      <c r="D110" s="41" t="str">
+        <f>MID(B108,5,1000) &amp; " Sample Value"</f>
+        <v>Thermal Mass Partition Wall Sample Value</v>
       </c>
       <c r="E110" s="41" t="s">
         <v>237</v>
@@ -10617,7 +10455,7 @@
         <v>1</v>
       </c>
       <c r="B111" s="40" t="s">
-        <v>520</v>
+        <v>472</v>
       </c>
       <c r="C111" s="40" t="s">
         <v>235</v>
@@ -10666,7 +10504,7 @@
       </c>
       <c r="H112" s="10"/>
       <c r="I112" s="10" t="s">
-        <v>416</v>
+        <v>376</v>
       </c>
       <c r="J112" s="10"/>
       <c r="K112" s="10"/>
@@ -10692,8 +10530,9 @@
         <v>21</v>
       </c>
       <c r="C113" s="41"/>
-      <c r="D113" s="41" t="s">
-        <v>521</v>
+      <c r="D113" s="41" t="str">
+        <f>MID(B111,5,1000) &amp; " Sample Value"</f>
+        <v>Thermal Mass Ceiling Sample Value</v>
       </c>
       <c r="E113" s="41" t="s">
         <v>237</v>
@@ -10737,7 +10576,7 @@
         <v>1</v>
       </c>
       <c r="B114" s="40" t="s">
-        <v>600</v>
+        <v>539</v>
       </c>
       <c r="C114" s="40" t="s">
         <v>235</v>
@@ -10786,7 +10625,7 @@
       </c>
       <c r="H115" s="10"/>
       <c r="I115" s="10" t="s">
-        <v>602</v>
+        <v>540</v>
       </c>
       <c r="J115" s="10"/>
       <c r="K115" s="10"/>
@@ -10812,8 +10651,9 @@
         <v>21</v>
       </c>
       <c r="C116" s="41"/>
-      <c r="D116" s="41" t="s">
-        <v>601</v>
+      <c r="D116" s="41" t="str">
+        <f>MID(B114,5,1000) &amp; " Sample Value"</f>
+        <v>Thermal Mass Furniture Sample Value</v>
       </c>
       <c r="E116" s="41" t="s">
         <v>237</v>
@@ -10857,7 +10697,7 @@
         <v>1</v>
       </c>
       <c r="B117" s="40" t="s">
-        <v>281</v>
+        <v>263</v>
       </c>
       <c r="C117" s="40" t="s">
         <v>235</v>
@@ -10906,7 +10746,7 @@
       </c>
       <c r="H118" s="10"/>
       <c r="I118" s="10" t="s">
-        <v>376</v>
+        <v>336</v>
       </c>
       <c r="J118" s="10"/>
       <c r="K118" s="10"/>
@@ -10932,8 +10772,9 @@
         <v>21</v>
       </c>
       <c r="C119" s="41"/>
-      <c r="D119" s="41" t="s">
-        <v>282</v>
+      <c r="D119" s="41" t="str">
+        <f>MID(B117,5,1000) &amp; " Sample Value"</f>
+        <v>Doors Sample Value</v>
       </c>
       <c r="E119" s="41" t="s">
         <v>237</v>
@@ -10977,7 +10818,7 @@
         <v>1</v>
       </c>
       <c r="B120" s="40" t="s">
-        <v>344</v>
+        <v>311</v>
       </c>
       <c r="C120" s="40" t="s">
         <v>235</v>
@@ -11026,7 +10867,7 @@
       </c>
       <c r="H121" s="10"/>
       <c r="I121" s="10" t="s">
-        <v>426</v>
+        <v>386</v>
       </c>
       <c r="J121" s="10"/>
       <c r="K121" s="10"/>
@@ -11052,8 +10893,9 @@
         <v>21</v>
       </c>
       <c r="C122" s="41"/>
-      <c r="D122" s="41" t="s">
-        <v>345</v>
+      <c r="D122" s="41" t="str">
+        <f>MID(B120,5,1000) &amp; " Sample Value"</f>
+        <v>Windows Sample Value</v>
       </c>
       <c r="E122" s="41" t="s">
         <v>237</v>
@@ -11097,7 +10939,7 @@
         <v>1</v>
       </c>
       <c r="B123" s="40" t="s">
-        <v>303</v>
+        <v>276</v>
       </c>
       <c r="C123" s="40" t="s">
         <v>235</v>
@@ -11146,7 +10988,7 @@
       </c>
       <c r="H124" s="10"/>
       <c r="I124" s="10" t="s">
-        <v>424</v>
+        <v>384</v>
       </c>
       <c r="J124" s="10"/>
       <c r="K124" s="10"/>
@@ -11172,8 +11014,9 @@
         <v>21</v>
       </c>
       <c r="C125" s="41"/>
-      <c r="D125" s="41" t="s">
-        <v>304</v>
+      <c r="D125" s="41" t="str">
+        <f>MID(B123,5,1000) &amp; " Sample Value"</f>
+        <v>Water Heater Sample Value</v>
       </c>
       <c r="E125" s="41" t="s">
         <v>237</v>
@@ -11217,7 +11060,7 @@
         <v>1</v>
       </c>
       <c r="B126" s="40" t="s">
-        <v>369</v>
+        <v>330</v>
       </c>
       <c r="C126" s="40" t="s">
         <v>235</v>
@@ -11266,7 +11109,7 @@
       </c>
       <c r="H127" s="10"/>
       <c r="I127" s="10" t="s">
-        <v>386</v>
+        <v>346</v>
       </c>
       <c r="J127" s="10"/>
       <c r="K127" s="10"/>
@@ -11292,8 +11135,9 @@
         <v>21</v>
       </c>
       <c r="C128" s="41"/>
-      <c r="D128" s="41" t="s">
-        <v>370</v>
+      <c r="D128" s="41" t="str">
+        <f>MID(B126,5,1000) &amp; " Sample Value"</f>
+        <v>Hot Water Fixtures Sample Value</v>
       </c>
       <c r="E128" s="41" t="s">
         <v>237</v>
@@ -11337,7 +11181,7 @@
         <v>1</v>
       </c>
       <c r="B129" s="40" t="s">
-        <v>358</v>
+        <v>322</v>
       </c>
       <c r="C129" s="40" t="s">
         <v>235</v>
@@ -11386,7 +11230,7 @@
       </c>
       <c r="H130" s="10"/>
       <c r="I130" s="10" t="s">
-        <v>390</v>
+        <v>350</v>
       </c>
       <c r="J130" s="10"/>
       <c r="K130" s="10"/>
@@ -11412,8 +11256,9 @@
         <v>21</v>
       </c>
       <c r="C131" s="41"/>
-      <c r="D131" s="41" t="s">
-        <v>359</v>
+      <c r="D131" s="41" t="str">
+        <f>MID(B129,5,1000) &amp; " Sample Value"</f>
+        <v>HVAC System Is Combined Sample Value</v>
       </c>
       <c r="E131" s="41" t="s">
         <v>237</v>
@@ -11457,7 +11302,7 @@
         <v>1</v>
       </c>
       <c r="B132" s="40" t="s">
-        <v>356</v>
+        <v>321</v>
       </c>
       <c r="C132" s="40" t="s">
         <v>235</v>
@@ -11506,7 +11351,7 @@
       </c>
       <c r="H133" s="10"/>
       <c r="I133" s="10" t="s">
-        <v>387</v>
+        <v>347</v>
       </c>
       <c r="J133" s="10"/>
       <c r="K133" s="10"/>
@@ -11532,8 +11377,9 @@
         <v>21</v>
       </c>
       <c r="C134" s="41"/>
-      <c r="D134" s="41" t="s">
-        <v>357</v>
+      <c r="D134" s="41" t="str">
+        <f>MID(B132,5,1000) &amp; " Sample Value"</f>
+        <v>HVAC System Combined Sample Value</v>
       </c>
       <c r="E134" s="41" t="s">
         <v>237</v>
@@ -11577,7 +11423,7 @@
         <v>1</v>
       </c>
       <c r="B135" s="40" t="s">
-        <v>364</v>
+        <v>327</v>
       </c>
       <c r="C135" s="40" t="s">
         <v>235</v>
@@ -11626,7 +11472,7 @@
       </c>
       <c r="H136" s="10"/>
       <c r="I136" s="10" t="s">
-        <v>389</v>
+        <v>349</v>
       </c>
       <c r="J136" s="10"/>
       <c r="K136" s="10"/>
@@ -11652,8 +11498,9 @@
         <v>21</v>
       </c>
       <c r="C137" s="41"/>
-      <c r="D137" s="41" t="s">
-        <v>367</v>
+      <c r="D137" s="41" t="str">
+        <f>MID(B135,5,1000) &amp; " Sample Value"</f>
+        <v>HVAC System Heating Sample Value</v>
       </c>
       <c r="E137" s="41" t="s">
         <v>237</v>
@@ -11697,7 +11544,7 @@
         <v>1</v>
       </c>
       <c r="B138" s="40" t="s">
-        <v>365</v>
+        <v>328</v>
       </c>
       <c r="C138" s="40" t="s">
         <v>235</v>
@@ -11746,7 +11593,7 @@
       </c>
       <c r="H139" s="10"/>
       <c r="I139" s="10" t="s">
-        <v>388</v>
+        <v>348</v>
       </c>
       <c r="J139" s="10"/>
       <c r="K139" s="10"/>
@@ -11772,8 +11619,9 @@
         <v>21</v>
       </c>
       <c r="C140" s="41"/>
-      <c r="D140" s="41" t="s">
-        <v>366</v>
+      <c r="D140" s="41" t="str">
+        <f>MID(B138,5,1000) &amp; " Sample Value"</f>
+        <v>HVAC System Cooling Sample Value</v>
       </c>
       <c r="E140" s="41" t="s">
         <v>237</v>
@@ -11817,7 +11665,7 @@
         <v>1</v>
       </c>
       <c r="B141" s="40" t="s">
-        <v>577</v>
+        <v>520</v>
       </c>
       <c r="C141" s="40" t="s">
         <v>235</v>
@@ -11866,7 +11714,7 @@
       </c>
       <c r="H142" s="10"/>
       <c r="I142" s="10" t="s">
-        <v>581</v>
+        <v>522</v>
       </c>
       <c r="J142" s="10"/>
       <c r="K142" s="10"/>
@@ -11892,8 +11740,9 @@
         <v>21</v>
       </c>
       <c r="C143" s="41"/>
-      <c r="D143" s="41" t="s">
-        <v>578</v>
+      <c r="D143" s="41" t="str">
+        <f>MID(B141,5,1000) &amp; " Sample Value"</f>
+        <v>Heating Setpoint Sample Value</v>
       </c>
       <c r="E143" s="41" t="s">
         <v>237</v>
@@ -11937,7 +11786,7 @@
         <v>1</v>
       </c>
       <c r="B144" s="40" t="s">
-        <v>576</v>
+        <v>519</v>
       </c>
       <c r="C144" s="40" t="s">
         <v>235</v>
@@ -11986,7 +11835,7 @@
       </c>
       <c r="H145" s="10"/>
       <c r="I145" s="10" t="s">
-        <v>580</v>
+        <v>521</v>
       </c>
       <c r="J145" s="10"/>
       <c r="K145" s="10"/>
@@ -12012,8 +11861,9 @@
         <v>21</v>
       </c>
       <c r="C146" s="41"/>
-      <c r="D146" s="41" t="s">
-        <v>579</v>
+      <c r="D146" s="41" t="str">
+        <f>MID(B144,5,1000) &amp; " Sample Value"</f>
+        <v>Cooling Setpoint Sample Value</v>
       </c>
       <c r="E146" s="41" t="s">
         <v>237</v>
@@ -12057,7 +11907,7 @@
         <v>1</v>
       </c>
       <c r="B147" s="40" t="s">
-        <v>287</v>
+        <v>268</v>
       </c>
       <c r="C147" s="40" t="s">
         <v>235</v>
@@ -12106,7 +11956,7 @@
       </c>
       <c r="H148" s="10"/>
       <c r="I148" s="10" t="s">
-        <v>414</v>
+        <v>374</v>
       </c>
       <c r="J148" s="10"/>
       <c r="K148" s="10"/>
@@ -12132,8 +11982,9 @@
         <v>21</v>
       </c>
       <c r="C149" s="41"/>
-      <c r="D149" s="41" t="s">
-        <v>288</v>
+      <c r="D149" s="41" t="str">
+        <f>MID(B147,5,1000) &amp; " Sample Value"</f>
+        <v>Refrigerator Sample Value</v>
       </c>
       <c r="E149" s="41" t="s">
         <v>237</v>
@@ -12177,7 +12028,7 @@
         <v>1</v>
       </c>
       <c r="B150" s="40" t="s">
-        <v>291</v>
+        <v>270</v>
       </c>
       <c r="C150" s="40" t="s">
         <v>235</v>
@@ -12226,7 +12077,7 @@
       </c>
       <c r="H151" s="10"/>
       <c r="I151" s="10" t="s">
-        <v>373</v>
+        <v>333</v>
       </c>
       <c r="J151" s="10"/>
       <c r="K151" s="10"/>
@@ -12252,8 +12103,9 @@
         <v>21</v>
       </c>
       <c r="C152" s="41"/>
-      <c r="D152" s="41" t="s">
-        <v>292</v>
+      <c r="D152" s="41" t="str">
+        <f>MID(B150,5,1000) &amp; " Sample Value"</f>
+        <v>Cooking Range Sample Value</v>
       </c>
       <c r="E152" s="41" t="s">
         <v>237</v>
@@ -12297,7 +12149,7 @@
         <v>1</v>
       </c>
       <c r="B153" s="40" t="s">
-        <v>295</v>
+        <v>272</v>
       </c>
       <c r="C153" s="40" t="s">
         <v>235</v>
@@ -12346,7 +12198,7 @@
       </c>
       <c r="H154" s="10"/>
       <c r="I154" s="10" t="s">
-        <v>374</v>
+        <v>334</v>
       </c>
       <c r="J154" s="10"/>
       <c r="K154" s="10"/>
@@ -12372,8 +12224,9 @@
         <v>21</v>
       </c>
       <c r="C155" s="41"/>
-      <c r="D155" s="41" t="s">
-        <v>296</v>
+      <c r="D155" s="41" t="str">
+        <f>MID(B153,5,1000) &amp; " Sample Value"</f>
+        <v>Dishwasher Sample Value</v>
       </c>
       <c r="E155" s="41" t="s">
         <v>237</v>
@@ -12417,7 +12270,7 @@
         <v>1</v>
       </c>
       <c r="B156" s="40" t="s">
-        <v>297</v>
+        <v>273</v>
       </c>
       <c r="C156" s="40" t="s">
         <v>235</v>
@@ -12466,7 +12319,7 @@
       </c>
       <c r="H157" s="10"/>
       <c r="I157" s="10" t="s">
-        <v>372</v>
+        <v>332</v>
       </c>
       <c r="J157" s="10"/>
       <c r="K157" s="10"/>
@@ -12492,8 +12345,9 @@
         <v>21</v>
       </c>
       <c r="C158" s="41"/>
-      <c r="D158" s="41" t="s">
-        <v>298</v>
+      <c r="D158" s="41" t="str">
+        <f>MID(B156,5,1000) &amp; " Sample Value"</f>
+        <v>Clothes Washer Sample Value</v>
       </c>
       <c r="E158" s="41" t="s">
         <v>237</v>
@@ -12537,7 +12391,7 @@
         <v>1</v>
       </c>
       <c r="B159" s="40" t="s">
-        <v>299</v>
+        <v>274</v>
       </c>
       <c r="C159" s="40" t="s">
         <v>235</v>
@@ -12586,7 +12440,7 @@
       </c>
       <c r="H160" s="10"/>
       <c r="I160" s="10" t="s">
-        <v>371</v>
+        <v>331</v>
       </c>
       <c r="J160" s="10"/>
       <c r="K160" s="10"/>
@@ -12612,8 +12466,9 @@
         <v>21</v>
       </c>
       <c r="C161" s="41"/>
-      <c r="D161" s="41" t="s">
-        <v>300</v>
+      <c r="D161" s="41" t="str">
+        <f>MID(B159,5,1000) &amp; " Sample Value"</f>
+        <v>Clothes Dryer Sample Value</v>
       </c>
       <c r="E161" s="41" t="s">
         <v>237</v>
@@ -12657,7 +12512,7 @@
         <v>1</v>
       </c>
       <c r="B162" s="40" t="s">
-        <v>348</v>
+        <v>314</v>
       </c>
       <c r="C162" s="40" t="s">
         <v>235</v>
@@ -12706,7 +12561,7 @@
       </c>
       <c r="H163" s="10"/>
       <c r="I163" s="10" t="s">
-        <v>399</v>
+        <v>359</v>
       </c>
       <c r="J163" s="10"/>
       <c r="K163" s="10"/>
@@ -12732,8 +12587,9 @@
         <v>21</v>
       </c>
       <c r="C164" s="41"/>
-      <c r="D164" s="41" t="s">
-        <v>349</v>
+      <c r="D164" s="41" t="str">
+        <f>MID(B162,5,1000) &amp; " Sample Value"</f>
+        <v>Lighting Sample Value</v>
       </c>
       <c r="E164" s="41" t="s">
         <v>237</v>
@@ -12777,7 +12633,7 @@
         <v>1</v>
       </c>
       <c r="B165" s="40" t="s">
-        <v>301</v>
+        <v>275</v>
       </c>
       <c r="C165" s="40" t="s">
         <v>235</v>
@@ -12826,7 +12682,7 @@
       </c>
       <c r="H166" s="10"/>
       <c r="I166" s="10" t="s">
-        <v>413</v>
+        <v>373</v>
       </c>
       <c r="J166" s="10"/>
       <c r="K166" s="10"/>
@@ -12852,8 +12708,9 @@
         <v>21</v>
       </c>
       <c r="C167" s="41"/>
-      <c r="D167" s="41" t="s">
-        <v>302</v>
+      <c r="D167" s="41" t="str">
+        <f>MID(B165,5,1000) &amp; " Sample Value"</f>
+        <v>Plug Loads Sample Value</v>
       </c>
       <c r="E167" s="41" t="s">
         <v>237</v>
@@ -12897,7 +12754,7 @@
         <v>1</v>
       </c>
       <c r="B168" s="40" t="s">
-        <v>523</v>
+        <v>473</v>
       </c>
       <c r="C168" s="40" t="s">
         <v>235</v>
@@ -12946,7 +12803,7 @@
       </c>
       <c r="H169" s="10"/>
       <c r="I169" s="10" t="s">
-        <v>402</v>
+        <v>362</v>
       </c>
       <c r="J169" s="10"/>
       <c r="K169" s="10"/>
@@ -12972,8 +12829,9 @@
         <v>21</v>
       </c>
       <c r="C170" s="41"/>
-      <c r="D170" s="41" t="s">
-        <v>522</v>
+      <c r="D170" s="41" t="str">
+        <f>MID(B168,5,1000) &amp; " Sample Value"</f>
+        <v>Misc Extra Refrigerator Sample Value</v>
       </c>
       <c r="E170" s="41" t="s">
         <v>237</v>
@@ -13017,7 +12875,7 @@
         <v>1</v>
       </c>
       <c r="B171" s="40" t="s">
-        <v>524</v>
+        <v>474</v>
       </c>
       <c r="C171" s="40" t="s">
         <v>235</v>
@@ -13066,7 +12924,7 @@
       </c>
       <c r="H172" s="10"/>
       <c r="I172" s="10" t="s">
-        <v>403</v>
+        <v>363</v>
       </c>
       <c r="J172" s="10"/>
       <c r="K172" s="10"/>
@@ -13092,8 +12950,9 @@
         <v>21</v>
       </c>
       <c r="C173" s="41"/>
-      <c r="D173" s="41" t="s">
-        <v>525</v>
+      <c r="D173" s="41" t="str">
+        <f>MID(B171,5,1000) &amp; " Sample Value"</f>
+        <v>Misc Freezer Sample Value</v>
       </c>
       <c r="E173" s="41" t="s">
         <v>237</v>
@@ -13137,7 +12996,7 @@
         <v>1</v>
       </c>
       <c r="B174" s="40" t="s">
-        <v>526</v>
+        <v>475</v>
       </c>
       <c r="C174" s="40" t="s">
         <v>235</v>
@@ -13186,7 +13045,7 @@
       </c>
       <c r="H175" s="10"/>
       <c r="I175" s="10" t="s">
-        <v>404</v>
+        <v>364</v>
       </c>
       <c r="J175" s="10"/>
       <c r="K175" s="10"/>
@@ -13212,8 +13071,9 @@
         <v>21</v>
       </c>
       <c r="C176" s="41"/>
-      <c r="D176" s="41" t="s">
-        <v>527</v>
+      <c r="D176" s="41" t="str">
+        <f>MID(B174,5,1000) &amp; " Sample Value"</f>
+        <v>Misc Gas Fireplace Sample Value</v>
       </c>
       <c r="E176" s="41" t="s">
         <v>237</v>
@@ -13257,7 +13117,7 @@
         <v>1</v>
       </c>
       <c r="B177" s="40" t="s">
-        <v>528</v>
+        <v>476</v>
       </c>
       <c r="C177" s="40" t="s">
         <v>235</v>
@@ -13306,7 +13166,7 @@
       </c>
       <c r="H178" s="10"/>
       <c r="I178" s="10" t="s">
-        <v>405</v>
+        <v>365</v>
       </c>
       <c r="J178" s="10"/>
       <c r="K178" s="10"/>
@@ -13332,8 +13192,9 @@
         <v>21</v>
       </c>
       <c r="C179" s="41"/>
-      <c r="D179" s="41" t="s">
-        <v>529</v>
+      <c r="D179" s="41" t="str">
+        <f>MID(B177,5,1000) &amp; " Sample Value"</f>
+        <v>Misc Gas Grill Sample Value</v>
       </c>
       <c r="E179" s="41" t="s">
         <v>237</v>
@@ -13377,7 +13238,7 @@
         <v>1</v>
       </c>
       <c r="B180" s="40" t="s">
-        <v>530</v>
+        <v>477</v>
       </c>
       <c r="C180" s="40" t="s">
         <v>235</v>
@@ -13426,7 +13287,7 @@
       </c>
       <c r="H181" s="10"/>
       <c r="I181" s="10" t="s">
-        <v>406</v>
+        <v>366</v>
       </c>
       <c r="J181" s="10"/>
       <c r="K181" s="10"/>
@@ -13452,8 +13313,9 @@
         <v>21</v>
       </c>
       <c r="C182" s="41"/>
-      <c r="D182" s="41" t="s">
-        <v>531</v>
+      <c r="D182" s="41" t="str">
+        <f>MID(B180,5,1000) &amp; " Sample Value"</f>
+        <v>Misc Gas Lighting Sample Value</v>
       </c>
       <c r="E182" s="41" t="s">
         <v>237</v>
@@ -13497,7 +13359,7 @@
         <v>1</v>
       </c>
       <c r="B183" s="40" t="s">
-        <v>532</v>
+        <v>478</v>
       </c>
       <c r="C183" s="40" t="s">
         <v>235</v>
@@ -13546,7 +13408,7 @@
       </c>
       <c r="H184" s="10"/>
       <c r="I184" s="10" t="s">
-        <v>407</v>
+        <v>367</v>
       </c>
       <c r="J184" s="10"/>
       <c r="K184" s="10"/>
@@ -13572,8 +13434,9 @@
         <v>21</v>
       </c>
       <c r="C185" s="41"/>
-      <c r="D185" s="41" t="s">
-        <v>533</v>
+      <c r="D185" s="41" t="str">
+        <f>MID(B183,5,1000) &amp; " Sample Value"</f>
+        <v>Misc Hot Tub Spa Sample Value</v>
       </c>
       <c r="E185" s="41" t="s">
         <v>237</v>
@@ -13617,7 +13480,7 @@
         <v>1</v>
       </c>
       <c r="B186" s="40" t="s">
-        <v>534</v>
+        <v>479</v>
       </c>
       <c r="C186" s="40" t="s">
         <v>235</v>
@@ -13666,7 +13529,7 @@
       </c>
       <c r="H187" s="10"/>
       <c r="I187" s="10" t="s">
-        <v>408</v>
+        <v>368</v>
       </c>
       <c r="J187" s="10"/>
       <c r="K187" s="10"/>
@@ -13692,8 +13555,9 @@
         <v>21</v>
       </c>
       <c r="C188" s="41"/>
-      <c r="D188" s="41" t="s">
-        <v>535</v>
+      <c r="D188" s="41" t="str">
+        <f>MID(B186,5,1000) &amp; " Sample Value"</f>
+        <v>Misc Pool Sample Value</v>
       </c>
       <c r="E188" s="41" t="s">
         <v>237</v>
@@ -13737,7 +13601,7 @@
         <v>1</v>
       </c>
       <c r="B189" s="40" t="s">
-        <v>536</v>
+        <v>480</v>
       </c>
       <c r="C189" s="40" t="s">
         <v>235</v>
@@ -13786,7 +13650,7 @@
       </c>
       <c r="H190" s="10"/>
       <c r="I190" s="10" t="s">
-        <v>409</v>
+        <v>369</v>
       </c>
       <c r="J190" s="10"/>
       <c r="K190" s="10"/>
@@ -13812,8 +13676,9 @@
         <v>21</v>
       </c>
       <c r="C191" s="41"/>
-      <c r="D191" s="41" t="s">
-        <v>537</v>
+      <c r="D191" s="41" t="str">
+        <f>MID(B189,5,1000) &amp; " Sample Value"</f>
+        <v>Misc Well Pump Sample Value</v>
       </c>
       <c r="E191" s="41" t="s">
         <v>237</v>
@@ -13857,7 +13722,7 @@
         <v>1</v>
       </c>
       <c r="B192" s="40" t="s">
-        <v>605</v>
+        <v>543</v>
       </c>
       <c r="C192" s="40" t="s">
         <v>235</v>
@@ -13906,7 +13771,7 @@
       </c>
       <c r="H193" s="10"/>
       <c r="I193" s="10" t="s">
-        <v>606</v>
+        <v>544</v>
       </c>
       <c r="J193" s="10"/>
       <c r="K193" s="10"/>
@@ -13932,8 +13797,9 @@
         <v>21</v>
       </c>
       <c r="C194" s="41"/>
-      <c r="D194" s="41" t="s">
-        <v>607</v>
+      <c r="D194" s="41" t="str">
+        <f>MID(B192,5,1000) &amp; " Sample Value"</f>
+        <v>Ducts Sample Value</v>
       </c>
       <c r="E194" s="41" t="s">
         <v>237</v>
@@ -13977,7 +13843,7 @@
         <v>1</v>
       </c>
       <c r="B195" s="40" t="s">
-        <v>608</v>
+        <v>545</v>
       </c>
       <c r="C195" s="40" t="s">
         <v>235</v>
@@ -14026,7 +13892,7 @@
       </c>
       <c r="H196" s="10"/>
       <c r="I196" s="10" t="s">
-        <v>609</v>
+        <v>546</v>
       </c>
       <c r="J196" s="10"/>
       <c r="K196" s="10"/>
@@ -14052,8 +13918,9 @@
         <v>21</v>
       </c>
       <c r="C197" s="41"/>
-      <c r="D197" s="41" t="s">
-        <v>610</v>
+      <c r="D197" s="41" t="str">
+        <f>MID(B195,5,1000) &amp; " Sample Value"</f>
+        <v>Infiltration Sample Value</v>
       </c>
       <c r="E197" s="41" t="s">
         <v>237</v>
@@ -14097,7 +13964,7 @@
         <v>1</v>
       </c>
       <c r="B198" s="40" t="s">
-        <v>611</v>
+        <v>547</v>
       </c>
       <c r="C198" s="40" t="s">
         <v>235</v>
@@ -14146,7 +14013,7 @@
       </c>
       <c r="H199" s="10"/>
       <c r="I199" s="10" t="s">
-        <v>612</v>
+        <v>548</v>
       </c>
       <c r="J199" s="10"/>
       <c r="K199" s="10"/>
@@ -14172,8 +14039,9 @@
         <v>21</v>
       </c>
       <c r="C200" s="41"/>
-      <c r="D200" s="41" t="s">
-        <v>613</v>
+      <c r="D200" s="41" t="str">
+        <f>MID(B198,5,1000) &amp; " Sample Value"</f>
+        <v>Natural Ventilation Sample Value</v>
       </c>
       <c r="E200" s="41" t="s">
         <v>237</v>
@@ -14217,7 +14085,7 @@
         <v>1</v>
       </c>
       <c r="B201" s="40" t="s">
-        <v>614</v>
+        <v>549</v>
       </c>
       <c r="C201" s="40" t="s">
         <v>235</v>
@@ -14266,7 +14134,7 @@
       </c>
       <c r="H202" s="10"/>
       <c r="I202" s="10" t="s">
-        <v>615</v>
+        <v>550</v>
       </c>
       <c r="J202" s="10"/>
       <c r="K202" s="10"/>
@@ -14292,8 +14160,9 @@
         <v>21</v>
       </c>
       <c r="C203" s="41"/>
-      <c r="D203" s="41" t="s">
-        <v>616</v>
+      <c r="D203" s="41" t="str">
+        <f>MID(B201,5,1000) &amp; " Sample Value"</f>
+        <v>Mechanical Ventilation Sample Value</v>
       </c>
       <c r="E203" s="41" t="s">
         <v>237</v>
@@ -14337,16 +14206,16 @@
         <v>0</v>
       </c>
       <c r="B204" s="40" t="s">
-        <v>617</v>
+        <v>551</v>
       </c>
       <c r="C204" s="40" t="s">
-        <v>631</v>
+        <v>564</v>
       </c>
       <c r="D204" s="40" t="s">
-        <v>631</v>
+        <v>564</v>
       </c>
       <c r="E204" s="40" t="s">
-        <v>632</v>
+        <v>565</v>
       </c>
       <c r="F204" s="40"/>
       <c r="G204" s="40"/>
@@ -14386,7 +14255,7 @@
       </c>
       <c r="H205" s="10"/>
       <c r="I205" s="10" t="s">
-        <v>618</v>
+        <v>552</v>
       </c>
       <c r="J205" s="10"/>
       <c r="K205" s="10"/>
@@ -14412,8 +14281,9 @@
         <v>21</v>
       </c>
       <c r="C206" s="41"/>
-      <c r="D206" s="41" t="s">
-        <v>619</v>
+      <c r="D206" s="41" t="str">
+        <f>MID(B204,5,1000) &amp; " Sample Value"</f>
+        <v>Airflow Sample Value</v>
       </c>
       <c r="E206" s="41" t="s">
         <v>237</v>
@@ -14457,16 +14327,16 @@
         <v>1</v>
       </c>
       <c r="B207" s="42" t="s">
-        <v>284</v>
+        <v>265</v>
       </c>
       <c r="C207" s="42" t="s">
-        <v>285</v>
+        <v>266</v>
       </c>
       <c r="D207" s="42" t="s">
-        <v>285</v>
+        <v>266</v>
       </c>
       <c r="E207" s="42" t="s">
-        <v>283</v>
+        <v>264</v>
       </c>
       <c r="F207" s="42"/>
       <c r="G207" s="42"/>
@@ -14493,16 +14363,16 @@
         <v>1</v>
       </c>
       <c r="B208" s="42" t="s">
-        <v>538</v>
+        <v>481</v>
       </c>
       <c r="C208" s="42" t="s">
-        <v>539</v>
+        <v>482</v>
       </c>
       <c r="D208" s="42" t="s">
-        <v>539</v>
+        <v>482</v>
       </c>
       <c r="E208" s="42" t="s">
-        <v>283</v>
+        <v>264</v>
       </c>
       <c r="F208" s="42"/>
       <c r="G208" s="42"/>
@@ -14529,16 +14399,16 @@
         <v>1</v>
       </c>
       <c r="B209" s="42" t="s">
-        <v>352</v>
+        <v>317</v>
       </c>
       <c r="C209" s="42" t="s">
-        <v>351</v>
+        <v>316</v>
       </c>
       <c r="D209" s="42" t="s">
-        <v>351</v>
+        <v>316</v>
       </c>
       <c r="E209" s="42" t="s">
-        <v>283</v>
+        <v>264</v>
       </c>
       <c r="F209" s="42"/>
       <c r="G209" s="42"/>
@@ -14697,16 +14567,16 @@
     </row>
     <row r="4" spans="1:13" s="50" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="49" t="s">
-        <v>305</v>
+        <v>277</v>
       </c>
       <c r="B4" s="49"/>
       <c r="C4" s="49"/>
       <c r="D4" s="49" t="s">
-        <v>428</v>
+        <v>388</v>
       </c>
       <c r="E4" s="49"/>
       <c r="F4" s="49" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G4" s="49" t="b">
         <v>0</v>
@@ -14724,16 +14594,16 @@
     </row>
     <row r="5" spans="1:13" s="50" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="49" t="s">
-        <v>306</v>
+        <v>278</v>
       </c>
       <c r="B5" s="49"/>
       <c r="C5" s="49"/>
       <c r="D5" s="49" t="s">
-        <v>458</v>
+        <v>418</v>
       </c>
       <c r="E5" s="49"/>
       <c r="F5" s="49" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G5" s="49" t="b">
         <v>0</v>
@@ -14751,16 +14621,16 @@
     </row>
     <row r="6" spans="1:13" s="50" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="49" t="s">
-        <v>307</v>
+        <v>279</v>
       </c>
       <c r="B6" s="49"/>
       <c r="C6" s="49"/>
       <c r="D6" s="49" t="s">
-        <v>479</v>
+        <v>439</v>
       </c>
       <c r="E6" s="49"/>
       <c r="F6" s="49" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G6" s="49" t="b">
         <v>0</v>
@@ -14778,16 +14648,16 @@
     </row>
     <row r="7" spans="1:13" s="50" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="49" t="s">
-        <v>308</v>
+        <v>280</v>
       </c>
       <c r="B7" s="49"/>
       <c r="C7" s="49"/>
       <c r="D7" s="49" t="s">
-        <v>443</v>
+        <v>403</v>
       </c>
       <c r="E7" s="49"/>
       <c r="F7" s="49" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G7" s="49" t="b">
         <v>0</v>
@@ -14805,16 +14675,16 @@
     </row>
     <row r="8" spans="1:13" s="50" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="49" t="s">
-        <v>309</v>
+        <v>281</v>
       </c>
       <c r="B8" s="49"/>
       <c r="C8" s="49"/>
       <c r="D8" s="49" t="s">
-        <v>478</v>
+        <v>438</v>
       </c>
       <c r="E8" s="49"/>
       <c r="F8" s="49" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G8" s="49" t="b">
         <v>0</v>
@@ -14832,16 +14702,16 @@
     </row>
     <row r="9" spans="1:13" s="50" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="49" t="s">
-        <v>484</v>
+        <v>444</v>
       </c>
       <c r="B9" s="49"/>
       <c r="C9" s="49"/>
       <c r="D9" s="49" t="s">
-        <v>438</v>
+        <v>398</v>
       </c>
       <c r="E9" s="49"/>
       <c r="F9" s="49" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G9" s="49" t="b">
         <v>0</v>
@@ -14859,16 +14729,16 @@
     </row>
     <row r="10" spans="1:13" s="50" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="49" t="s">
-        <v>485</v>
+        <v>445</v>
       </c>
       <c r="B10" s="49"/>
       <c r="C10" s="49"/>
       <c r="D10" s="49" t="s">
-        <v>440</v>
+        <v>400</v>
       </c>
       <c r="E10" s="49"/>
       <c r="F10" s="49" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G10" s="49" t="b">
         <v>0</v>
@@ -14886,16 +14756,16 @@
     </row>
     <row r="11" spans="1:13" s="50" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="49" t="s">
-        <v>486</v>
+        <v>446</v>
       </c>
       <c r="B11" s="49"/>
       <c r="C11" s="49"/>
       <c r="D11" s="49" t="s">
-        <v>441</v>
+        <v>401</v>
       </c>
       <c r="E11" s="49"/>
       <c r="F11" s="49" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G11" s="49" t="b">
         <v>0</v>
@@ -14913,16 +14783,16 @@
     </row>
     <row r="12" spans="1:13" s="50" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" s="49" t="s">
-        <v>487</v>
+        <v>447</v>
       </c>
       <c r="B12" s="49"/>
       <c r="C12" s="49"/>
       <c r="D12" s="49" t="s">
-        <v>439</v>
+        <v>399</v>
       </c>
       <c r="E12" s="49"/>
       <c r="F12" s="49" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G12" s="49" t="b">
         <v>0</v>
@@ -14940,16 +14810,16 @@
     </row>
     <row r="13" spans="1:13" s="50" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="49" t="s">
-        <v>310</v>
+        <v>282</v>
       </c>
       <c r="B13" s="49"/>
       <c r="C13" s="49"/>
       <c r="D13" s="49" t="s">
-        <v>442</v>
+        <v>402</v>
       </c>
       <c r="E13" s="49"/>
       <c r="F13" s="49" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G13" s="49" t="b">
         <v>0</v>
@@ -14967,16 +14837,16 @@
     </row>
     <row r="14" spans="1:13" s="50" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="49" t="s">
-        <v>311</v>
+        <v>283</v>
       </c>
       <c r="B14" s="49"/>
       <c r="C14" s="49"/>
       <c r="D14" s="49" t="s">
-        <v>468</v>
+        <v>428</v>
       </c>
       <c r="E14" s="49"/>
       <c r="F14" s="49" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G14" s="49" t="b">
         <v>0</v>
@@ -14994,16 +14864,16 @@
     </row>
     <row r="15" spans="1:13" s="50" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="49" t="s">
-        <v>334</v>
+        <v>304</v>
       </c>
       <c r="B15" s="49"/>
       <c r="C15" s="49"/>
       <c r="D15" s="49" t="s">
-        <v>435</v>
+        <v>395</v>
       </c>
       <c r="E15" s="49"/>
       <c r="F15" s="49" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G15" s="49" t="b">
         <v>0</v>
@@ -15021,16 +14891,16 @@
     </row>
     <row r="16" spans="1:13" s="50" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" s="49" t="s">
-        <v>337</v>
+        <v>306</v>
       </c>
       <c r="B16" s="49"/>
       <c r="C16" s="49"/>
       <c r="D16" s="49" t="s">
-        <v>469</v>
+        <v>429</v>
       </c>
       <c r="E16" s="49"/>
       <c r="F16" s="49" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G16" s="49" t="b">
         <v>0</v>
@@ -15048,13 +14918,13 @@
     </row>
     <row r="17" spans="1:13" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="49" t="s">
-        <v>320</v>
+        <v>292</v>
       </c>
       <c r="D17" s="49" t="s">
-        <v>433</v>
+        <v>393</v>
       </c>
       <c r="F17" s="49" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G17" s="49" t="b">
         <v>0</v>
@@ -15068,13 +14938,13 @@
     </row>
     <row r="18" spans="1:13" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="49" t="s">
-        <v>341</v>
+        <v>309</v>
       </c>
       <c r="D18" s="49" t="s">
-        <v>482</v>
+        <v>442</v>
       </c>
       <c r="F18" s="49" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G18" s="49" t="b">
         <v>0</v>
@@ -15088,16 +14958,16 @@
     </row>
     <row r="19" spans="1:13" s="50" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19" s="49" t="s">
-        <v>331</v>
+        <v>302</v>
       </c>
       <c r="B19" s="49"/>
       <c r="C19" s="49"/>
       <c r="D19" s="49" t="s">
-        <v>467</v>
+        <v>427</v>
       </c>
       <c r="E19" s="49"/>
       <c r="F19" s="49" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G19" s="49" t="b">
         <v>0</v>
@@ -15115,16 +14985,16 @@
     </row>
     <row r="20" spans="1:13" s="50" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" s="49" t="s">
-        <v>312</v>
+        <v>284</v>
       </c>
       <c r="B20" s="49"/>
       <c r="C20" s="49"/>
       <c r="D20" s="49" t="s">
-        <v>454</v>
+        <v>414</v>
       </c>
       <c r="E20" s="49"/>
       <c r="F20" s="49" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G20" s="49" t="b">
         <v>0</v>
@@ -15142,16 +15012,16 @@
     </row>
     <row r="21" spans="1:13" s="50" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" s="49" t="s">
-        <v>488</v>
+        <v>448</v>
       </c>
       <c r="B21" s="49"/>
       <c r="C21" s="49"/>
       <c r="D21" s="49" t="s">
-        <v>456</v>
+        <v>416</v>
       </c>
       <c r="E21" s="49"/>
       <c r="F21" s="49" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G21" s="49" t="b">
         <v>0</v>
@@ -15169,16 +15039,16 @@
     </row>
     <row r="22" spans="1:13" s="50" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22" s="49" t="s">
-        <v>489</v>
+        <v>449</v>
       </c>
       <c r="B22" s="49"/>
       <c r="C22" s="49"/>
       <c r="D22" s="49" t="s">
-        <v>452</v>
+        <v>412</v>
       </c>
       <c r="E22" s="49"/>
       <c r="F22" s="49" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G22" s="49" t="b">
         <v>0</v>
@@ -15196,16 +15066,16 @@
     </row>
     <row r="23" spans="1:13" s="50" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A23" s="49" t="s">
-        <v>313</v>
+        <v>285</v>
       </c>
       <c r="B23" s="49"/>
       <c r="C23" s="49"/>
       <c r="D23" s="49" t="s">
-        <v>453</v>
+        <v>413</v>
       </c>
       <c r="E23" s="49"/>
       <c r="F23" s="49" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G23" s="49" t="b">
         <v>0</v>
@@ -15223,13 +15093,13 @@
     </row>
     <row r="24" spans="1:13" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="49" t="s">
-        <v>490</v>
+        <v>450</v>
       </c>
       <c r="D24" s="49" t="s">
-        <v>449</v>
+        <v>409</v>
       </c>
       <c r="F24" s="49" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G24" s="49" t="b">
         <v>0</v>
@@ -15243,13 +15113,13 @@
     </row>
     <row r="25" spans="1:13" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="49" t="s">
-        <v>314</v>
+        <v>286</v>
       </c>
       <c r="D25" s="49" t="s">
-        <v>455</v>
+        <v>415</v>
       </c>
       <c r="F25" s="49" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G25" s="49" t="b">
         <v>0</v>
@@ -15263,13 +15133,13 @@
     </row>
     <row r="26" spans="1:13" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="49" t="s">
-        <v>315</v>
+        <v>287</v>
       </c>
       <c r="D26" s="49" t="s">
-        <v>450</v>
+        <v>410</v>
       </c>
       <c r="F26" s="49" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G26" s="49" t="b">
         <v>0</v>
@@ -15283,13 +15153,13 @@
     </row>
     <row r="27" spans="1:13" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="49" t="s">
-        <v>491</v>
+        <v>451</v>
       </c>
       <c r="D27" s="49" t="s">
-        <v>451</v>
+        <v>411</v>
       </c>
       <c r="F27" s="49" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G27" s="49" t="b">
         <v>0</v>
@@ -15303,13 +15173,13 @@
     </row>
     <row r="28" spans="1:13" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="49" t="s">
-        <v>340</v>
+        <v>308</v>
       </c>
       <c r="D28" s="49" t="s">
-        <v>477</v>
+        <v>437</v>
       </c>
       <c r="F28" s="49" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G28" s="49" t="b">
         <v>0</v>
@@ -15323,13 +15193,13 @@
     </row>
     <row r="29" spans="1:13" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="49" t="s">
-        <v>596</v>
+        <v>535</v>
       </c>
       <c r="D29" s="49" t="s">
-        <v>597</v>
+        <v>536</v>
       </c>
       <c r="F29" s="49" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G29" s="49" t="b">
         <v>0</v>
@@ -15343,13 +15213,13 @@
     </row>
     <row r="30" spans="1:13" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="49" t="s">
-        <v>316</v>
+        <v>288</v>
       </c>
       <c r="D30" s="49" t="s">
-        <v>480</v>
+        <v>440</v>
       </c>
       <c r="F30" s="49" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G30" s="49" t="b">
         <v>0</v>
@@ -15363,13 +15233,13 @@
     </row>
     <row r="31" spans="1:13" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="49" t="s">
-        <v>598</v>
+        <v>537</v>
       </c>
       <c r="D31" s="49" t="s">
-        <v>599</v>
+        <v>538</v>
       </c>
       <c r="F31" s="49" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G31" s="49" t="b">
         <v>0</v>
@@ -15383,13 +15253,13 @@
     </row>
     <row r="32" spans="1:13" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="49" t="s">
-        <v>317</v>
+        <v>289</v>
       </c>
       <c r="D32" s="49" t="s">
-        <v>436</v>
+        <v>396</v>
       </c>
       <c r="F32" s="49" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G32" s="49" t="b">
         <v>0</v>
@@ -15403,13 +15273,13 @@
     </row>
     <row r="33" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="49" t="s">
-        <v>318</v>
+        <v>290</v>
       </c>
       <c r="D33" s="49" t="s">
-        <v>472</v>
+        <v>432</v>
       </c>
       <c r="F33" s="49" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G33" s="49" t="b">
         <v>0</v>
@@ -15423,13 +15293,13 @@
     </row>
     <row r="34" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="49" t="s">
-        <v>319</v>
+        <v>291</v>
       </c>
       <c r="D34" s="49" t="s">
-        <v>437</v>
+        <v>397</v>
       </c>
       <c r="F34" s="49" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G34" s="49" t="b">
         <v>0</v>
@@ -15443,13 +15313,13 @@
     </row>
     <row r="35" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="49" t="s">
-        <v>492</v>
+        <v>452</v>
       </c>
       <c r="D35" s="49" t="s">
-        <v>475</v>
+        <v>435</v>
       </c>
       <c r="F35" s="49" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G35" s="49" t="b">
         <v>0</v>
@@ -15463,13 +15333,13 @@
     </row>
     <row r="36" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="49" t="s">
-        <v>493</v>
+        <v>453</v>
       </c>
       <c r="D36" s="49" t="s">
-        <v>474</v>
+        <v>434</v>
       </c>
       <c r="F36" s="49" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G36" s="49" t="b">
         <v>0</v>
@@ -15483,13 +15353,13 @@
     </row>
     <row r="37" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="49" t="s">
-        <v>494</v>
+        <v>454</v>
       </c>
       <c r="D37" s="49" t="s">
-        <v>476</v>
+        <v>436</v>
       </c>
       <c r="F37" s="49" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G37" s="49" t="b">
         <v>0</v>
@@ -15503,13 +15373,13 @@
     </row>
     <row r="38" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="49" t="s">
-        <v>495</v>
+        <v>455</v>
       </c>
       <c r="D38" s="49" t="s">
-        <v>473</v>
+        <v>433</v>
       </c>
       <c r="F38" s="49" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G38" s="49" t="b">
         <v>0</v>
@@ -15523,13 +15393,13 @@
     </row>
     <row r="39" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="49" t="s">
-        <v>603</v>
+        <v>541</v>
       </c>
       <c r="D39" s="49" t="s">
-        <v>604</v>
+        <v>542</v>
       </c>
       <c r="F39" s="49" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G39" s="49" t="b">
         <v>0</v>
@@ -15543,13 +15413,13 @@
     </row>
     <row r="40" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="49" t="s">
-        <v>321</v>
+        <v>293</v>
       </c>
       <c r="D40" s="49" t="s">
-        <v>434</v>
+        <v>394</v>
       </c>
       <c r="F40" s="49" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G40" s="49" t="b">
         <v>0</v>
@@ -15563,13 +15433,13 @@
     </row>
     <row r="41" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="49" t="s">
-        <v>346</v>
+        <v>312</v>
       </c>
       <c r="D41" s="49" t="s">
-        <v>483</v>
+        <v>443</v>
       </c>
       <c r="F41" s="49" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G41" s="49" t="b">
         <v>0</v>
@@ -15583,13 +15453,13 @@
     </row>
     <row r="42" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="49" t="s">
-        <v>322</v>
+        <v>294</v>
       </c>
       <c r="D42" s="49" t="s">
-        <v>481</v>
+        <v>441</v>
       </c>
       <c r="F42" s="49" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G42" s="49" t="b">
         <v>0</v>
@@ -15603,13 +15473,13 @@
     </row>
     <row r="43" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="49" t="s">
-        <v>368</v>
+        <v>329</v>
       </c>
       <c r="D43" s="49" t="s">
-        <v>444</v>
+        <v>404</v>
       </c>
       <c r="F43" s="49" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G43" s="49" t="b">
         <v>0</v>
@@ -15623,13 +15493,13 @@
     </row>
     <row r="44" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="49" t="s">
-        <v>360</v>
+        <v>323</v>
       </c>
       <c r="D44" s="49" t="s">
-        <v>448</v>
+        <v>408</v>
       </c>
       <c r="F44" s="49" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G44" s="49" t="b">
         <v>0</v>
@@ -15643,13 +15513,13 @@
     </row>
     <row r="45" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="49" t="s">
-        <v>361</v>
+        <v>324</v>
       </c>
       <c r="D45" s="49" t="s">
-        <v>445</v>
+        <v>405</v>
       </c>
       <c r="F45" s="49" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G45" s="49" t="b">
         <v>0</v>
@@ -15663,13 +15533,13 @@
     </row>
     <row r="46" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="49" t="s">
-        <v>363</v>
+        <v>326</v>
       </c>
       <c r="D46" s="49" t="s">
-        <v>447</v>
+        <v>407</v>
       </c>
       <c r="F46" s="49" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G46" s="49" t="b">
         <v>0</v>
@@ -15683,13 +15553,13 @@
     </row>
     <row r="47" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="49" t="s">
-        <v>362</v>
+        <v>325</v>
       </c>
       <c r="D47" s="49" t="s">
-        <v>446</v>
+        <v>406</v>
       </c>
       <c r="F47" s="49" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G47" s="49" t="b">
         <v>0</v>
@@ -15703,13 +15573,13 @@
     </row>
     <row r="48" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="49" t="s">
-        <v>582</v>
+        <v>523</v>
       </c>
       <c r="D48" s="49" t="s">
-        <v>583</v>
+        <v>524</v>
       </c>
       <c r="F48" s="49" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G48" s="49" t="b">
         <v>0</v>
@@ -15723,13 +15593,13 @@
     </row>
     <row r="49" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="49" t="s">
-        <v>584</v>
+        <v>525</v>
       </c>
       <c r="D49" s="49" t="s">
-        <v>585</v>
+        <v>526</v>
       </c>
       <c r="F49" s="49" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G49" s="49" t="b">
         <v>0</v>
@@ -15743,13 +15613,13 @@
     </row>
     <row r="50" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="49" t="s">
-        <v>323</v>
+        <v>295</v>
       </c>
       <c r="D50" s="49" t="s">
-        <v>471</v>
+        <v>431</v>
       </c>
       <c r="F50" s="49" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G50" s="49" t="b">
         <v>0</v>
@@ -15763,13 +15633,13 @@
     </row>
     <row r="51" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="49" t="s">
-        <v>324</v>
+        <v>296</v>
       </c>
       <c r="D51" s="49" t="s">
-        <v>431</v>
+        <v>391</v>
       </c>
       <c r="F51" s="49" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G51" s="49" t="b">
         <v>0</v>
@@ -15783,13 +15653,13 @@
     </row>
     <row r="52" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="49" t="s">
-        <v>325</v>
+        <v>297</v>
       </c>
       <c r="D52" s="49" t="s">
-        <v>432</v>
+        <v>392</v>
       </c>
       <c r="F52" s="49" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G52" s="49" t="b">
         <v>0</v>
@@ -15803,13 +15673,13 @@
     </row>
     <row r="53" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="49" t="s">
-        <v>326</v>
+        <v>298</v>
       </c>
       <c r="D53" s="49" t="s">
-        <v>430</v>
+        <v>390</v>
       </c>
       <c r="F53" s="49" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G53" s="49" t="b">
         <v>0</v>
@@ -15823,13 +15693,13 @@
     </row>
     <row r="54" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="49" t="s">
-        <v>327</v>
+        <v>299</v>
       </c>
       <c r="D54" s="49" t="s">
-        <v>429</v>
+        <v>389</v>
       </c>
       <c r="F54" s="49" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G54" s="49" t="b">
         <v>0</v>
@@ -15843,13 +15713,13 @@
     </row>
     <row r="55" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="49" t="s">
-        <v>350</v>
+        <v>315</v>
       </c>
       <c r="D55" s="49" t="s">
-        <v>457</v>
+        <v>417</v>
       </c>
       <c r="F55" s="49" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G55" s="49" t="b">
         <v>0</v>
@@ -15863,13 +15733,13 @@
     </row>
     <row r="56" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="49" t="s">
-        <v>328</v>
+        <v>300</v>
       </c>
       <c r="D56" s="49" t="s">
-        <v>470</v>
+        <v>430</v>
       </c>
       <c r="F56" s="49" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G56" s="49" t="b">
         <v>0</v>
@@ -15883,13 +15753,13 @@
     </row>
     <row r="57" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="49" t="s">
-        <v>496</v>
+        <v>456</v>
       </c>
       <c r="D57" s="49" t="s">
-        <v>459</v>
+        <v>419</v>
       </c>
       <c r="F57" s="49" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G57" s="49" t="b">
         <v>0</v>
@@ -15903,13 +15773,13 @@
     </row>
     <row r="58" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="49" t="s">
-        <v>497</v>
+        <v>457</v>
       </c>
       <c r="D58" s="49" t="s">
-        <v>460</v>
+        <v>420</v>
       </c>
       <c r="F58" s="49" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G58" s="49" t="b">
         <v>0</v>
@@ -15923,13 +15793,13 @@
     </row>
     <row r="59" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="49" t="s">
-        <v>498</v>
+        <v>458</v>
       </c>
       <c r="D59" s="49" t="s">
-        <v>461</v>
+        <v>421</v>
       </c>
       <c r="F59" s="49" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G59" s="49" t="b">
         <v>0</v>
@@ -15943,13 +15813,13 @@
     </row>
     <row r="60" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="49" t="s">
-        <v>499</v>
+        <v>459</v>
       </c>
       <c r="D60" s="49" t="s">
-        <v>462</v>
+        <v>422</v>
       </c>
       <c r="F60" s="49" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G60" s="49" t="b">
         <v>0</v>
@@ -15963,13 +15833,13 @@
     </row>
     <row r="61" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="49" t="s">
-        <v>500</v>
+        <v>460</v>
       </c>
       <c r="D61" s="49" t="s">
-        <v>463</v>
+        <v>423</v>
       </c>
       <c r="F61" s="49" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G61" s="49" t="b">
         <v>0</v>
@@ -15983,13 +15853,13 @@
     </row>
     <row r="62" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="49" t="s">
-        <v>501</v>
+        <v>461</v>
       </c>
       <c r="D62" s="49" t="s">
-        <v>464</v>
+        <v>424</v>
       </c>
       <c r="F62" s="49" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G62" s="49" t="b">
         <v>0</v>
@@ -16003,13 +15873,13 @@
     </row>
     <row r="63" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="49" t="s">
-        <v>502</v>
+        <v>462</v>
       </c>
       <c r="D63" s="49" t="s">
-        <v>465</v>
+        <v>425</v>
       </c>
       <c r="F63" s="49" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G63" s="49" t="b">
         <v>0</v>
@@ -16023,13 +15893,13 @@
     </row>
     <row r="64" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="49" t="s">
-        <v>503</v>
+        <v>463</v>
       </c>
       <c r="D64" s="49" t="s">
-        <v>466</v>
+        <v>426</v>
       </c>
       <c r="F64" s="49" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G64" s="49" t="b">
         <v>0</v>
@@ -16043,13 +15913,13 @@
     </row>
     <row r="65" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="49" t="s">
-        <v>620</v>
+        <v>553</v>
       </c>
       <c r="D65" s="49" t="s">
-        <v>621</v>
+        <v>554</v>
       </c>
       <c r="F65" s="49" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G65" s="49" t="b">
         <v>0</v>
@@ -16063,13 +15933,13 @@
     </row>
     <row r="66" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="49" t="s">
-        <v>622</v>
+        <v>555</v>
       </c>
       <c r="D66" s="49" t="s">
-        <v>623</v>
+        <v>556</v>
       </c>
       <c r="F66" s="49" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G66" s="49" t="b">
         <v>0</v>
@@ -16083,13 +15953,13 @@
     </row>
     <row r="67" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="49" t="s">
-        <v>624</v>
+        <v>557</v>
       </c>
       <c r="D67" s="49" t="s">
-        <v>625</v>
+        <v>558</v>
       </c>
       <c r="F67" s="49" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G67" s="49" t="b">
         <v>0</v>
@@ -16103,13 +15973,13 @@
     </row>
     <row r="68" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="49" t="s">
-        <v>626</v>
+        <v>559</v>
       </c>
       <c r="D68" s="49" t="s">
-        <v>627</v>
+        <v>560</v>
       </c>
       <c r="F68" s="49" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G68" s="49" t="b">
         <v>0</v>
@@ -16123,13 +15993,13 @@
     </row>
     <row r="69" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="49" t="s">
-        <v>628</v>
+        <v>561</v>
       </c>
       <c r="D69" s="49" t="s">
-        <v>629</v>
+        <v>562</v>
       </c>
       <c r="F69" s="49" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G69" s="49" t="b">
         <v>0</v>
@@ -16143,13 +16013,13 @@
     </row>
     <row r="70" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="48" t="s">
-        <v>540</v>
+        <v>483</v>
       </c>
       <c r="D70" s="14" t="s">
-        <v>563</v>
+        <v>506</v>
       </c>
       <c r="F70" s="14" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G70" s="14" t="b">
         <v>0</v>
@@ -16163,13 +16033,13 @@
     </row>
     <row r="71" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="48" t="s">
-        <v>541</v>
+        <v>484</v>
       </c>
       <c r="D71" s="14" t="s">
-        <v>564</v>
+        <v>507</v>
       </c>
       <c r="F71" s="14" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G71" s="14" t="b">
         <v>0</v>
@@ -16183,13 +16053,13 @@
     </row>
     <row r="72" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="48" t="s">
-        <v>542</v>
+        <v>485</v>
       </c>
       <c r="D72" s="14" t="s">
-        <v>565</v>
+        <v>508</v>
       </c>
       <c r="F72" s="14" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G72" s="14" t="b">
         <v>0</v>
@@ -16203,13 +16073,13 @@
     </row>
     <row r="73" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="48" t="s">
-        <v>543</v>
+        <v>486</v>
       </c>
       <c r="D73" s="14" t="s">
-        <v>566</v>
+        <v>509</v>
       </c>
       <c r="F73" s="14" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G73" s="14" t="b">
         <v>0</v>
@@ -16223,13 +16093,13 @@
     </row>
     <row r="74" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="48" t="s">
-        <v>544</v>
+        <v>487</v>
       </c>
       <c r="D74" s="14" t="s">
-        <v>567</v>
+        <v>510</v>
       </c>
       <c r="F74" s="14" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G74" s="14" t="b">
         <v>0</v>
@@ -16243,13 +16113,13 @@
     </row>
     <row r="75" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="48" t="s">
-        <v>545</v>
+        <v>488</v>
       </c>
       <c r="D75" s="14" t="s">
-        <v>568</v>
+        <v>511</v>
       </c>
       <c r="F75" s="14" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G75" s="14" t="b">
         <v>0</v>
@@ -16263,13 +16133,13 @@
     </row>
     <row r="76" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="48" t="s">
-        <v>546</v>
+        <v>489</v>
       </c>
       <c r="D76" s="14" t="s">
-        <v>569</v>
+        <v>512</v>
       </c>
       <c r="F76" s="14" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G76" s="14" t="b">
         <v>0</v>
@@ -16283,13 +16153,13 @@
     </row>
     <row r="77" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="48" t="s">
-        <v>547</v>
+        <v>490</v>
       </c>
       <c r="D77" s="14" t="s">
-        <v>570</v>
+        <v>513</v>
       </c>
       <c r="F77" s="14" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G77" s="14" t="b">
         <v>0</v>
@@ -16303,13 +16173,13 @@
     </row>
     <row r="78" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="48" t="s">
-        <v>548</v>
+        <v>491</v>
       </c>
       <c r="D78" s="14" t="s">
-        <v>571</v>
+        <v>514</v>
       </c>
       <c r="F78" s="14" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G78" s="14" t="b">
         <v>0</v>
@@ -16323,13 +16193,13 @@
     </row>
     <row r="79" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="48" t="s">
-        <v>549</v>
+        <v>492</v>
       </c>
       <c r="D79" s="14" t="s">
-        <v>572</v>
+        <v>515</v>
       </c>
       <c r="F79" s="14" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G79" s="14" t="b">
         <v>0</v>
@@ -16343,13 +16213,13 @@
     </row>
     <row r="80" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="48" t="s">
-        <v>550</v>
+        <v>493</v>
       </c>
       <c r="D80" s="14" t="s">
-        <v>573</v>
+        <v>516</v>
       </c>
       <c r="F80" s="14" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G80" s="14" t="b">
         <v>0</v>
@@ -16363,13 +16233,13 @@
     </row>
     <row r="81" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="48" t="s">
-        <v>551</v>
+        <v>494</v>
       </c>
       <c r="D81" s="14" t="s">
-        <v>574</v>
+        <v>517</v>
       </c>
       <c r="F81" s="14" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G81" s="14" t="b">
         <v>0</v>
@@ -16383,13 +16253,13 @@
     </row>
     <row r="82" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="14" t="s">
-        <v>552</v>
+        <v>495</v>
       </c>
       <c r="D82" s="14" t="s">
-        <v>575</v>
+        <v>518</v>
       </c>
       <c r="F82" s="14" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G82" s="14" t="b">
         <v>0</v>
@@ -16403,13 +16273,13 @@
     </row>
     <row r="83" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="14" t="s">
-        <v>553</v>
+        <v>496</v>
       </c>
       <c r="D83" s="14" t="s">
-        <v>562</v>
+        <v>505</v>
       </c>
       <c r="F83" s="14" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G83" s="14" t="b">
         <v>0</v>
@@ -16423,13 +16293,13 @@
     </row>
     <row r="84" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="14" t="s">
-        <v>554</v>
+        <v>497</v>
       </c>
       <c r="D84" s="14" t="s">
-        <v>561</v>
+        <v>504</v>
       </c>
       <c r="F84" s="14" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G84" s="14" t="b">
         <v>0</v>
@@ -16443,13 +16313,13 @@
     </row>
     <row r="85" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="14" t="s">
-        <v>555</v>
+        <v>498</v>
       </c>
       <c r="D85" s="14" t="s">
-        <v>560</v>
+        <v>503</v>
       </c>
       <c r="F85" s="14" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G85" s="14" t="b">
         <v>0</v>
@@ -16463,13 +16333,13 @@
     </row>
     <row r="86" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="14" t="s">
-        <v>556</v>
+        <v>499</v>
       </c>
       <c r="D86" s="14" t="s">
-        <v>559</v>
+        <v>502</v>
       </c>
       <c r="F86" s="14" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G86" s="14" t="b">
         <v>0</v>
@@ -16483,13 +16353,13 @@
     </row>
     <row r="87" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="14" t="s">
-        <v>557</v>
+        <v>500</v>
       </c>
       <c r="D87" s="14" t="s">
-        <v>558</v>
+        <v>501</v>
       </c>
       <c r="F87" s="14" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="G87" s="14" t="b">
         <v>0</v>

</xml_diff>